<commit_message>
Exportacion Excel y Pdf completa 2
</commit_message>
<xml_diff>
--- a/temp_reporte.xlsx
+++ b/temp_reporte.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="2" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja32" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Hoja31" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Hoja30" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Hoja28 (2)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hoja28" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Hoja27" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ADSCRIPCION">#REF!</definedName>
@@ -75,15 +75,15 @@
     <definedName name="TIPO_A">#REF!</definedName>
     <definedName name="TIPO_B">#REF!</definedName>
     <definedName name="VIERNES">#REF!</definedName>
-    <definedName name="ASIGNACION" localSheetId="0">Hoja32!$K:$K</definedName>
-    <definedName name="FORMATO" localSheetId="0">Hoja32!$A:$K</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Hoja32'!$A$1:$J$57</definedName>
-    <definedName name="ASIGNACION" localSheetId="1">Hoja31!$K:$K</definedName>
-    <definedName name="FORMATO" localSheetId="1">Hoja31!$A:$K</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Hoja31'!$A$1:$J$57</definedName>
-    <definedName name="ASIGNACION" localSheetId="2">Hoja30!$K:$K</definedName>
-    <definedName name="FORMATO" localSheetId="2">Hoja30!$A:$K</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Hoja30'!$A$1:$J$57</definedName>
+    <definedName name="ASIGNACION" localSheetId="0">'Hoja28 (2)'!$K:$K</definedName>
+    <definedName name="FORMATO" localSheetId="0">'Hoja28 (2)'!$A:$K</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Hoja28 (2)'!$A$1:$J$56</definedName>
+    <definedName name="ASIGNACION" localSheetId="1">Hoja28!$K:$K</definedName>
+    <definedName name="FORMATO" localSheetId="1">Hoja28!$A:$K</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Hoja28'!$A$1:$J$56</definedName>
+    <definedName name="ASIGNACION" localSheetId="2">Hoja27!$K:$K</definedName>
+    <definedName name="FORMATO" localSheetId="2">Hoja27!$A:$K</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Hoja27'!$A$1:$J$57</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -234,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -455,6 +455,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -478,7 +487,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="101">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -608,9 +617,20 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
@@ -625,13 +645,17 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -656,6 +680,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -668,6 +693,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,118 +704,30 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal 2 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="130">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="116">
     <dxf>
       <fill>
         <patternFill>
@@ -1713,26 +1652,27 @@
   <oneCellAnchor>
     <from>
       <col>0</col>
-      <colOff>0</colOff>
-      <row>47</row>
-      <rowOff>0</rowOff>
+      <colOff>19050</colOff>
+      <row>53</row>
+      <rowOff>85725</rowOff>
     </from>
-    <ext cx="8247539" cy="1821227"/>
+    <ext cx="8247539" cy="811577"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 2" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
-      <blipFill>
+      <blipFill rotWithShape="1">
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:srcRect t="55438"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
         <a:xfrm>
-          <a:off x="0" y="9820275"/>
-          <a:ext cx="8247539" cy="1821227"/>
+          <a:off x="19050" y="10829925"/>
+          <a:ext cx="8247539" cy="811577"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <avLst/>
@@ -1786,26 +1726,27 @@
   <oneCellAnchor>
     <from>
       <col>0</col>
-      <colOff>0</colOff>
-      <row>47</row>
-      <rowOff>0</rowOff>
+      <colOff>19050</colOff>
+      <row>53</row>
+      <rowOff>85725</rowOff>
     </from>
-    <ext cx="8247539" cy="1821227"/>
+    <ext cx="8247539" cy="811577"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 2" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
-      <blipFill>
+      <blipFill rotWithShape="1">
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:srcRect t="55438"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
         <a:xfrm>
-          <a:off x="0" y="9820275"/>
-          <a:ext cx="8247539" cy="1821227"/>
+          <a:off x="19050" y="10829925"/>
+          <a:ext cx="8247539" cy="811577"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <avLst/>
@@ -1894,9 +1835,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1934,7 +1875,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2040,7 +1981,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2182,7 +2123,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2190,29 +2131,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Hoja32">
+  <sheetPr>
     <tabColor rgb="FF90E8F4"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A4:Q57"/>
   <sheetViews>
-    <sheetView showZeros="0" showWhiteSpace="0" view="pageLayout" topLeftCell="A37" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:B46"/>
+    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A46" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col width="11.140625" customWidth="1" style="53" min="1" max="1"/>
-    <col width="19.42578125" customWidth="1" style="53" min="2" max="2"/>
-    <col width="7.85546875" customWidth="1" style="53" min="3" max="3"/>
-    <col width="5.85546875" customWidth="1" style="53" min="4" max="4"/>
-    <col width="13.140625" customWidth="1" style="53" min="5" max="5"/>
-    <col width="13.7109375" customWidth="1" style="53" min="6" max="6"/>
-    <col width="12.5703125" customWidth="1" style="53" min="7" max="7"/>
-    <col width="12.42578125" customWidth="1" style="53" min="8" max="8"/>
-    <col width="12" customWidth="1" style="53" min="9" max="9"/>
-    <col width="9.7109375" customWidth="1" style="53" min="10" max="10"/>
+    <col width="11.140625" customWidth="1" style="94" min="1" max="1"/>
+    <col width="19.42578125" customWidth="1" style="94" min="2" max="2"/>
+    <col width="7.85546875" customWidth="1" style="94" min="3" max="3"/>
+    <col width="5.85546875" customWidth="1" style="94" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" style="94" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" style="94" min="6" max="6"/>
+    <col width="12.5703125" customWidth="1" style="94" min="7" max="7"/>
+    <col width="12.42578125" customWidth="1" style="94" min="8" max="8"/>
+    <col width="12" customWidth="1" style="94" min="9" max="9"/>
+    <col width="9.7109375" customWidth="1" style="94" min="10" max="10"/>
     <col width="12.140625" customWidth="1" style="2" min="11" max="11"/>
     <col width="11.42578125" customWidth="1" style="3" min="12" max="15"/>
     <col width="25.42578125" customWidth="1" style="3" min="16" max="16"/>
@@ -2221,154 +2162,154 @@
     <col width="11.42578125" customWidth="1" style="3" min="20" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" s="87"/>
-    <row r="2" ht="12" customHeight="1" s="87"/>
-    <row r="3" ht="32.25" customHeight="1" s="87"/>
-    <row r="4" ht="12" customHeight="1" s="87">
-      <c r="A4" s="81" t="inlineStr">
+    <row r="1" ht="12" customHeight="1" s="96"/>
+    <row r="2" ht="12" customHeight="1" s="96"/>
+    <row r="3" ht="32.25" customHeight="1" s="96"/>
+    <row r="4" ht="12" customHeight="1" s="96">
+      <c r="A4" s="89" t="inlineStr">
         <is>
           <t>“2024. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="82" t="inlineStr">
+      <c r="A5" s="90" t="inlineStr">
         <is>
           <t>Asignación Académica</t>
         </is>
       </c>
-      <c r="B5" s="76" t="n"/>
-      <c r="C5" s="76" t="n"/>
-      <c r="D5" s="76" t="n"/>
-      <c r="E5" s="76" t="n"/>
-      <c r="F5" s="76" t="n"/>
-      <c r="G5" s="76" t="n"/>
-      <c r="H5" s="76" t="n"/>
-      <c r="I5" s="76" t="n"/>
-      <c r="J5" s="64" t="n"/>
-    </row>
-    <row r="6" ht="12" customHeight="1" s="87">
-      <c r="A6" s="77" t="inlineStr">
+      <c r="B5" s="81" t="n"/>
+      <c r="C5" s="81" t="n"/>
+      <c r="D5" s="81" t="n"/>
+      <c r="E5" s="81" t="n"/>
+      <c r="F5" s="81" t="n"/>
+      <c r="G5" s="81" t="n"/>
+      <c r="H5" s="81" t="n"/>
+      <c r="I5" s="81" t="n"/>
+      <c r="J5" s="82" t="n"/>
+    </row>
+    <row r="6" ht="12" customHeight="1" s="96">
+      <c r="A6" s="83" t="inlineStr">
         <is>
           <t>NOMBRE:</t>
         </is>
       </c>
-      <c r="B6" s="55" t="n"/>
-      <c r="C6" s="55" t="n"/>
-      <c r="D6" s="56" t="n"/>
-      <c r="E6" s="77" t="inlineStr">
+      <c r="B6" s="58" t="n"/>
+      <c r="C6" s="58" t="n"/>
+      <c r="D6" s="59" t="n"/>
+      <c r="E6" s="83" t="inlineStr">
         <is>
           <t>PROFESION:</t>
         </is>
       </c>
-      <c r="F6" s="55" t="n"/>
-      <c r="G6" s="55" t="n"/>
-      <c r="H6" s="55" t="n"/>
-      <c r="I6" s="55" t="n"/>
-      <c r="J6" s="56" t="n"/>
-    </row>
-    <row r="7" ht="12" customHeight="1" s="87">
-      <c r="A7" s="83" t="inlineStr">
+      <c r="F6" s="58" t="n"/>
+      <c r="G6" s="58" t="n"/>
+      <c r="H6" s="58" t="n"/>
+      <c r="I6" s="58" t="n"/>
+      <c r="J6" s="59" t="n"/>
+    </row>
+    <row r="7" ht="12" customHeight="1" s="96">
+      <c r="A7" s="91" t="inlineStr">
         <is>
           <t>AGUILAR GUGGEMBUHL JARUMI</t>
         </is>
       </c>
-      <c r="B7" s="61" t="n"/>
-      <c r="C7" s="61" t="n"/>
-      <c r="D7" s="62" t="n"/>
-      <c r="E7" s="80" t="inlineStr">
+      <c r="B7" s="64" t="n"/>
+      <c r="C7" s="64" t="n"/>
+      <c r="D7" s="65" t="n"/>
+      <c r="E7" s="86" t="inlineStr">
         <is>
           <t>LIC. VETERINARIA Y ZOOTECNIA/M. EN C. AGROPECUARIAS/ DR. BIOTECNOLOGÍA</t>
         </is>
       </c>
-      <c r="F7" s="61" t="n"/>
-      <c r="G7" s="61" t="n"/>
-      <c r="H7" s="61" t="n"/>
-      <c r="I7" s="61" t="n"/>
-      <c r="J7" s="62" t="n"/>
-    </row>
-    <row r="8" ht="12" customHeight="1" s="87">
-      <c r="A8" s="77" t="inlineStr">
+      <c r="F7" s="64" t="n"/>
+      <c r="G7" s="64" t="n"/>
+      <c r="H7" s="64" t="n"/>
+      <c r="I7" s="64" t="n"/>
+      <c r="J7" s="65" t="n"/>
+    </row>
+    <row r="8" ht="12" customHeight="1" s="96">
+      <c r="A8" s="83" t="inlineStr">
         <is>
           <t>ADSCRIPCIÓN:</t>
         </is>
       </c>
-      <c r="B8" s="55" t="n"/>
-      <c r="C8" s="55" t="n"/>
-      <c r="D8" s="56" t="n"/>
-      <c r="E8" s="77" t="inlineStr">
+      <c r="B8" s="58" t="n"/>
+      <c r="C8" s="58" t="n"/>
+      <c r="D8" s="59" t="n"/>
+      <c r="E8" s="83" t="inlineStr">
         <is>
           <t>INGRESO AL TECNOLÓGICO</t>
         </is>
       </c>
-      <c r="F8" s="55" t="n"/>
-      <c r="G8" s="56" t="n"/>
-      <c r="H8" s="77" t="inlineStr">
+      <c r="F8" s="58" t="n"/>
+      <c r="G8" s="59" t="n"/>
+      <c r="H8" s="83" t="inlineStr">
         <is>
           <t>TIEMPO INDETERMINADO</t>
         </is>
       </c>
-      <c r="I8" s="55" t="n"/>
-      <c r="J8" s="56" t="n"/>
-    </row>
-    <row r="9" ht="12" customHeight="1" s="87">
-      <c r="A9" s="80" t="inlineStr">
+      <c r="I8" s="58" t="n"/>
+      <c r="J8" s="59" t="n"/>
+    </row>
+    <row r="9" ht="12" customHeight="1" s="96">
+      <c r="A9" s="86" t="inlineStr">
         <is>
           <t>PROFESOR DE ASIGNATURA DE ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B9" s="61" t="n"/>
-      <c r="C9" s="61" t="n"/>
-      <c r="D9" s="62" t="n"/>
-      <c r="E9" s="80" t="inlineStr">
+      <c r="B9" s="64" t="n"/>
+      <c r="C9" s="64" t="n"/>
+      <c r="D9" s="65" t="n"/>
+      <c r="E9" s="86" t="inlineStr">
         <is>
           <t>01 DE SEPTIEMBRE 2014</t>
         </is>
       </c>
-      <c r="F9" s="61" t="n"/>
-      <c r="G9" s="62" t="n"/>
-      <c r="H9" s="80" t="inlineStr">
+      <c r="F9" s="64" t="n"/>
+      <c r="G9" s="65" t="n"/>
+      <c r="H9" s="86" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
       </c>
-      <c r="I9" s="61" t="n"/>
-      <c r="J9" s="62" t="n"/>
-    </row>
-    <row r="10" ht="12" customHeight="1" s="87">
-      <c r="A10" s="77" t="inlineStr">
+      <c r="I9" s="64" t="n"/>
+      <c r="J9" s="65" t="n"/>
+    </row>
+    <row r="10" ht="12" customHeight="1" s="96">
+      <c r="A10" s="83" t="inlineStr">
         <is>
           <t>PERIODO:</t>
         </is>
       </c>
-      <c r="B10" s="55" t="n"/>
-      <c r="C10" s="55" t="n"/>
-      <c r="D10" s="56" t="n"/>
-      <c r="E10" s="78" t="inlineStr">
+      <c r="B10" s="58" t="n"/>
+      <c r="C10" s="58" t="n"/>
+      <c r="D10" s="59" t="n"/>
+      <c r="E10" s="84" t="inlineStr">
         <is>
           <t>HORAS TIPO</t>
         </is>
       </c>
-      <c r="F10" s="76" t="n"/>
-      <c r="G10" s="76" t="n"/>
-      <c r="H10" s="64" t="n"/>
-      <c r="I10" s="78" t="inlineStr">
+      <c r="F10" s="81" t="n"/>
+      <c r="G10" s="81" t="n"/>
+      <c r="H10" s="82" t="n"/>
+      <c r="I10" s="84" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="J10" s="64" t="n"/>
-    </row>
-    <row r="11" ht="12" customHeight="1" s="87">
-      <c r="A11" s="79" t="inlineStr">
+      <c r="J10" s="82" t="n"/>
+    </row>
+    <row r="11" ht="12" customHeight="1" s="96">
+      <c r="A11" s="85" t="inlineStr">
         <is>
           <t>2024-1 (MARZO-AGOSTO 2024)</t>
         </is>
       </c>
-      <c r="B11" s="61" t="n"/>
-      <c r="C11" s="61" t="n"/>
-      <c r="D11" s="61" t="n"/>
-      <c r="E11" s="78" t="inlineStr">
+      <c r="B11" s="64" t="n"/>
+      <c r="C11" s="64" t="n"/>
+      <c r="D11" s="64" t="n"/>
+      <c r="E11" s="84" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -2394,7 +2335,7 @@
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
-    <row r="12" ht="5.1" customHeight="1" s="87">
+    <row r="12" ht="5.1" customHeight="1" s="96">
       <c r="A12" s="8" t="n"/>
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="8" t="n"/>
@@ -2406,23 +2347,23 @@
       <c r="I12" s="8" t="n"/>
       <c r="J12" s="8" t="n"/>
     </row>
-    <row r="13" ht="12" customHeight="1" s="87">
-      <c r="A13" s="78" t="inlineStr">
+    <row r="13" ht="12" customHeight="1" s="96">
+      <c r="A13" s="84" t="inlineStr">
         <is>
           <t>Asignación de Horas Frente a Grupo</t>
         </is>
       </c>
-      <c r="B13" s="76" t="n"/>
-      <c r="C13" s="76" t="n"/>
-      <c r="D13" s="76" t="n"/>
-      <c r="E13" s="76" t="n"/>
-      <c r="F13" s="76" t="n"/>
-      <c r="G13" s="76" t="n"/>
-      <c r="H13" s="76" t="n"/>
-      <c r="I13" s="76" t="n"/>
-      <c r="J13" s="64" t="n"/>
-    </row>
-    <row r="14" ht="12" customHeight="1" s="87">
+      <c r="B13" s="81" t="n"/>
+      <c r="C13" s="81" t="n"/>
+      <c r="D13" s="81" t="n"/>
+      <c r="E13" s="81" t="n"/>
+      <c r="F13" s="81" t="n"/>
+      <c r="G13" s="81" t="n"/>
+      <c r="H13" s="81" t="n"/>
+      <c r="I13" s="81" t="n"/>
+      <c r="J13" s="82" t="n"/>
+    </row>
+    <row r="14" ht="12" customHeight="1" s="96">
       <c r="A14" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -2526,9 +2467,9 @@
         </is>
       </c>
       <c r="K15" s="15" t="n"/>
-      <c r="N15" s="88" t="n"/>
-    </row>
-    <row r="16" ht="21.75" customHeight="1" s="87">
+      <c r="N15" s="97" t="n"/>
+    </row>
+    <row r="16" ht="21.75" customHeight="1" s="96">
       <c r="A16" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -2580,9 +2521,9 @@
         </is>
       </c>
       <c r="K16" s="17" t="n"/>
-      <c r="N16" s="88" t="n"/>
-    </row>
-    <row r="17" ht="21.75" customHeight="1" s="87">
+      <c r="N16" s="97" t="n"/>
+    </row>
+    <row r="17" ht="21.75" customHeight="1" s="96">
       <c r="A17" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -2676,7 +2617,7 @@
       </c>
       <c r="K18" s="17" t="n"/>
     </row>
-    <row r="19" ht="20.25" customHeight="1" s="87">
+    <row r="19" ht="20.25" customHeight="1" s="96">
       <c r="A19" s="10" t="n"/>
       <c r="B19" s="11" t="inlineStr"/>
       <c r="C19" s="12" t="inlineStr">
@@ -2717,7 +2658,7 @@
       </c>
       <c r="K19" s="17" t="n"/>
     </row>
-    <row r="20" ht="19.5" customHeight="1" s="87">
+    <row r="20" ht="19.5" customHeight="1" s="96">
       <c r="A20" s="10" t="n"/>
       <c r="B20" s="11" t="inlineStr"/>
       <c r="C20" s="12" t="inlineStr">
@@ -2758,7 +2699,7 @@
       </c>
       <c r="K20" s="17" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="87">
+    <row r="21" ht="18" customHeight="1" s="96">
       <c r="A21" s="10" t="n"/>
       <c r="B21" s="11" t="inlineStr"/>
       <c r="C21" s="12" t="inlineStr">
@@ -2799,7 +2740,7 @@
       </c>
       <c r="K21" s="17" t="n"/>
     </row>
-    <row r="22" ht="18" customHeight="1" s="87">
+    <row r="22" ht="18" customHeight="1" s="96">
       <c r="A22" s="10" t="n"/>
       <c r="B22" s="11" t="inlineStr"/>
       <c r="C22" s="12" t="inlineStr">
@@ -2861,14 +2802,14 @@
       <c r="J23" s="23" t="n"/>
       <c r="K23" s="17" t="n"/>
     </row>
-    <row r="24" ht="12" customHeight="1" s="87">
-      <c r="A24" s="67" t="inlineStr">
+    <row r="24" ht="12" customHeight="1" s="96">
+      <c r="A24" s="72" t="inlineStr">
         <is>
           <t>Asignación de Horas de Descarga para otras Actividades</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="12" customHeight="1" s="87">
+    <row r="25" ht="12" customHeight="1" s="96">
       <c r="A25" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -2920,7 +2861,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="24.75" customHeight="1" s="87">
+    <row r="26" ht="24.75" customHeight="1" s="96">
       <c r="A26" s="24" t="n"/>
       <c r="B26" s="25" t="inlineStr">
         <is>
@@ -2969,7 +2910,7 @@
       </c>
       <c r="K26" s="27" t="n"/>
     </row>
-    <row r="27" ht="28.5" customHeight="1" s="87">
+    <row r="27" ht="28.5" customHeight="1" s="96">
       <c r="A27" s="24" t="n"/>
       <c r="B27" s="25" t="inlineStr">
         <is>
@@ -3018,7 +2959,7 @@
       </c>
       <c r="K27" s="27" t="n"/>
     </row>
-    <row r="28" ht="26.25" customHeight="1" s="87">
+    <row r="28" ht="26.25" customHeight="1" s="96">
       <c r="A28" s="24" t="n"/>
       <c r="B28" s="25" t="inlineStr">
         <is>
@@ -3067,7 +3008,7 @@
       </c>
       <c r="K28" s="27" t="n"/>
     </row>
-    <row r="29" ht="30" customHeight="1" s="87">
+    <row r="29" ht="30" customHeight="1" s="96">
       <c r="A29" s="24" t="n"/>
       <c r="B29" s="25" t="inlineStr">
         <is>
@@ -3116,7 +3057,7 @@
       </c>
       <c r="K29" s="27" t="n"/>
     </row>
-    <row r="30" ht="33" customHeight="1" s="87">
+    <row r="30" ht="33" customHeight="1" s="96">
       <c r="A30" s="24" t="n"/>
       <c r="B30" s="25" t="inlineStr">
         <is>
@@ -3165,7 +3106,7 @@
       </c>
       <c r="K30" s="27" t="n"/>
     </row>
-    <row r="31" ht="19.5" customHeight="1" s="87">
+    <row r="31" ht="19.5" customHeight="1" s="96">
       <c r="A31" s="24" t="n"/>
       <c r="B31" s="25" t="inlineStr"/>
       <c r="C31" s="26" t="inlineStr"/>
@@ -3202,7 +3143,7 @@
       </c>
       <c r="K31" s="27" t="n"/>
     </row>
-    <row r="32" ht="34.5" customHeight="1" s="87">
+    <row r="32" ht="34.5" customHeight="1" s="96">
       <c r="A32" s="24" t="n"/>
       <c r="B32" s="25" t="inlineStr"/>
       <c r="C32" s="26" t="inlineStr"/>
@@ -3239,7 +3180,7 @@
       </c>
       <c r="K32" s="27" t="n"/>
     </row>
-    <row r="33" ht="21" customHeight="1" s="87">
+    <row r="33" ht="21" customHeight="1" s="96">
       <c r="A33" s="24" t="n"/>
       <c r="B33" s="25" t="inlineStr"/>
       <c r="C33" s="26" t="inlineStr"/>
@@ -3297,14 +3238,14 @@
       <c r="J34" s="28" t="n"/>
       <c r="K34" s="27" t="n"/>
     </row>
-    <row r="35" ht="12" customHeight="1" s="87">
-      <c r="A35" s="67" t="inlineStr">
+    <row r="35" ht="12" customHeight="1" s="96">
+      <c r="A35" s="72" t="inlineStr">
         <is>
           <t>Asignación de Horas de Presidente y Secretario de Academia</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="12" customHeight="1" s="87">
+    <row r="36" ht="12" customHeight="1" s="96">
       <c r="A36" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -3356,7 +3297,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="87">
+    <row r="37" ht="18.75" customHeight="1" s="96">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="25" t="inlineStr">
         <is>
@@ -3397,7 +3338,7 @@
       </c>
       <c r="K37" s="31" t="n"/>
     </row>
-    <row r="38" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="38" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A38" s="32" t="n"/>
       <c r="B38" s="33" t="n"/>
       <c r="C38" s="34" t="inlineStr">
@@ -3413,14 +3354,14 @@
       <c r="I38" s="26" t="n"/>
       <c r="J38" s="35" t="n"/>
     </row>
-    <row r="39" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="39" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A39" s="36" t="n"/>
-      <c r="B39" s="68" t="inlineStr">
+      <c r="B39" s="73" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="C39" s="69" t="n"/>
+      <c r="C39" s="74" t="n"/>
       <c r="D39" s="37" t="n">
         <v>40</v>
       </c>
@@ -3431,31 +3372,31 @@
       <c r="I39" s="38" t="n"/>
       <c r="J39" s="39" t="n"/>
     </row>
-    <row r="40" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="40" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A40" s="36" t="n"/>
       <c r="B40" s="40" t="n"/>
       <c r="C40" s="41" t="n"/>
       <c r="D40" s="38" t="n"/>
-      <c r="E40" s="70" t="inlineStr">
+      <c r="E40" s="75" t="inlineStr">
         <is>
           <t>FECHA DE APLICACIÓN</t>
         </is>
       </c>
-      <c r="G40" s="71" t="inlineStr">
-        <is>
-          <t>25/01/2025</t>
-        </is>
-      </c>
-      <c r="H40" s="69" t="n"/>
-      <c r="I40" s="69" t="n"/>
-      <c r="J40" s="72" t="n"/>
-    </row>
-    <row r="41" ht="12" customHeight="1" s="87" thickBot="1">
+      <c r="G40" s="76" t="inlineStr">
+        <is>
+          <t>28/01/2025</t>
+        </is>
+      </c>
+      <c r="H40" s="74" t="n"/>
+      <c r="I40" s="74" t="n"/>
+      <c r="J40" s="77" t="n"/>
+    </row>
+    <row r="41" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A41" s="36" t="n"/>
       <c r="B41" s="40" t="n"/>
       <c r="C41" s="41" t="n"/>
       <c r="D41" s="38" t="n"/>
-      <c r="E41" s="70" t="inlineStr">
+      <c r="E41" s="75" t="inlineStr">
         <is>
           <t>CONSECUTIVO</t>
         </is>
@@ -3469,7 +3410,7 @@
       <c r="I41" s="38" t="n"/>
       <c r="J41" s="39" t="n"/>
     </row>
-    <row r="42" ht="9.75" customFormat="1" customHeight="1" s="58">
+    <row r="42" ht="9.75" customFormat="1" customHeight="1" s="61">
       <c r="C42" s="44" t="n"/>
       <c r="D42" s="44" t="n"/>
       <c r="E42" s="44" t="n"/>
@@ -3480,72 +3421,80 @@
       <c r="J42" s="44" t="n"/>
       <c r="K42" s="45" t="n"/>
     </row>
-    <row r="43" customFormat="1" s="58">
-      <c r="A43" s="73" t="n"/>
-      <c r="B43" s="56" t="n"/>
-      <c r="C43" s="74" t="inlineStr">
+    <row r="43" customFormat="1" s="61">
+      <c r="A43" s="78" t="inlineStr">
+        <is>
+          <t>JEFA DE DIVISIÓN DE ING. INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B43" s="59" t="n"/>
+      <c r="C43" s="79" t="inlineStr">
         <is>
           <t>REVISO</t>
         </is>
       </c>
-      <c r="D43" s="55" t="n"/>
-      <c r="E43" s="55" t="n"/>
-      <c r="F43" s="56" t="n"/>
-      <c r="G43" s="75" t="inlineStr">
+      <c r="D43" s="58" t="n"/>
+      <c r="E43" s="58" t="n"/>
+      <c r="F43" s="59" t="n"/>
+      <c r="G43" s="80" t="inlineStr">
         <is>
           <t>FIRMA DE CONFORMIDAD</t>
         </is>
       </c>
-      <c r="H43" s="76" t="n"/>
-      <c r="I43" s="76" t="n"/>
-      <c r="J43" s="64" t="n"/>
+      <c r="H43" s="81" t="n"/>
+      <c r="I43" s="81" t="n"/>
+      <c r="J43" s="82" t="n"/>
       <c r="K43" s="45" t="n"/>
     </row>
-    <row r="44" ht="16.5" customFormat="1" customHeight="1" s="58">
+    <row r="44" ht="16.5" customFormat="1" customHeight="1" s="61">
       <c r="A44" s="46" t="n"/>
       <c r="B44" s="47" t="n"/>
       <c r="C44" s="48" t="n"/>
       <c r="D44" s="48" t="n"/>
       <c r="E44" s="48" t="n"/>
       <c r="F44" s="49" t="n"/>
-      <c r="G44" s="54" t="inlineStr">
+      <c r="G44" s="57" t="inlineStr">
         <is>
           <t>AGUILAR GUGGEMBUHL JARUMI</t>
         </is>
       </c>
-      <c r="H44" s="55" t="n"/>
-      <c r="I44" s="55" t="n"/>
-      <c r="J44" s="56" t="n"/>
+      <c r="H44" s="58" t="n"/>
+      <c r="I44" s="58" t="n"/>
+      <c r="J44" s="59" t="n"/>
       <c r="K44" s="45" t="n"/>
     </row>
-    <row r="45" ht="12" customFormat="1" customHeight="1" s="58">
+    <row r="45" ht="12" customFormat="1" customHeight="1" s="61">
       <c r="A45" s="0" t="n"/>
       <c r="B45" s="0" t="n"/>
-      <c r="C45" s="63" t="inlineStr">
+      <c r="C45" s="66" t="inlineStr">
         <is>
           <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ
 ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
         </is>
       </c>
-      <c r="F45" s="59" t="n"/>
-      <c r="G45" s="57" t="n"/>
-      <c r="J45" s="59" t="n"/>
+      <c r="F45" s="62" t="n"/>
+      <c r="G45" s="60" t="n"/>
+      <c r="J45" s="62" t="n"/>
       <c r="K45" s="45" t="n"/>
     </row>
-    <row r="46" ht="37.5" customFormat="1" customHeight="1" s="58">
-      <c r="A46" s="86" t="n"/>
-      <c r="B46" s="62" t="n"/>
-      <c r="C46" s="60" t="n"/>
-      <c r="D46" s="61" t="n"/>
-      <c r="E46" s="61" t="n"/>
-      <c r="F46" s="62" t="n"/>
-      <c r="G46" s="60" t="n"/>
-      <c r="H46" s="61" t="n"/>
-      <c r="I46" s="61" t="n"/>
-      <c r="J46" s="62" t="n"/>
+    <row r="46" ht="37.5" customFormat="1" customHeight="1" s="61">
+      <c r="A46" s="67" t="inlineStr">
+        <is>
+          <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
+        </is>
+      </c>
+      <c r="B46" s="65" t="n"/>
+      <c r="C46" s="63" t="n"/>
+      <c r="D46" s="64" t="n"/>
+      <c r="E46" s="64" t="n"/>
+      <c r="F46" s="65" t="n"/>
+      <c r="G46" s="63" t="n"/>
+      <c r="H46" s="64" t="n"/>
+      <c r="I46" s="64" t="n"/>
+      <c r="J46" s="65" t="n"/>
       <c r="K46" s="45" t="n"/>
     </row>
-    <row r="47" ht="1.35" customHeight="1" s="87">
+    <row r="47" ht="1.35" customHeight="1" s="96">
       <c r="A47" s="50" t="n"/>
       <c r="B47" s="50" t="n"/>
       <c r="C47" s="50" t="n"/>
@@ -3559,43 +3508,80 @@
       <c r="P47" s="51" t="n"/>
       <c r="Q47" s="51" t="n"/>
     </row>
-    <row r="48" ht="12.75" customHeight="1" s="87">
-      <c r="A48" s="65" t="n"/>
-      <c r="C48" s="66" t="n"/>
-      <c r="G48" s="66" t="n"/>
+    <row r="48" ht="12.75" customHeight="1" s="96">
+      <c r="A48" s="68" t="n"/>
+      <c r="C48" s="98" t="inlineStr">
+        <is>
+          <t>Vo. Bo</t>
+        </is>
+      </c>
+      <c r="G48" s="93" t="n"/>
       <c r="K48" s="3" t="n"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1" s="87">
+    <row r="49" ht="12.75" customHeight="1" s="96">
       <c r="K49" s="3" t="n"/>
     </row>
-    <row r="50" ht="12.75" customHeight="1" s="87">
+    <row r="50" ht="21" customHeight="1" s="96">
+      <c r="C50" s="64" t="n"/>
+      <c r="D50" s="64" t="n"/>
+      <c r="E50" s="64" t="n"/>
+      <c r="F50" s="64" t="n"/>
       <c r="K50" s="3" t="n"/>
     </row>
-    <row r="51" ht="17.25" customHeight="1" s="87">
+    <row r="51" ht="3" customHeight="1" s="96">
       <c r="A51" s="52" t="n"/>
+      <c r="B51" s="53" t="n"/>
+      <c r="C51" s="53" t="n"/>
+      <c r="D51" s="53" t="n"/>
+      <c r="E51" s="53" t="n"/>
+      <c r="F51" s="53" t="n"/>
+      <c r="G51" s="53" t="n"/>
+      <c r="H51" s="53" t="n"/>
+      <c r="I51" s="53" t="n"/>
+      <c r="J51" s="53" t="n"/>
       <c r="K51" s="3" t="n"/>
     </row>
-    <row r="52" ht="30" customHeight="1" s="87"/>
+    <row r="52" ht="10.5" customHeight="1" s="96">
+      <c r="A52" s="53" t="n"/>
+      <c r="B52" s="53" t="n"/>
+      <c r="C52" s="54" t="inlineStr">
+        <is>
+          <t>DRA C.CLAUDIA PÉREZ MARTÍNEZ</t>
+        </is>
+      </c>
+      <c r="G52" s="53" t="n"/>
+      <c r="H52" s="53" t="n"/>
+      <c r="I52" s="53" t="n"/>
+      <c r="J52" s="53" t="n"/>
+    </row>
+    <row r="53">
+      <c r="C53" s="54" t="inlineStr">
+        <is>
+          <t>DIRECTORA GENERAL</t>
+        </is>
+      </c>
+    </row>
     <row r="57">
       <c r="K57" s="3" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="C52:F52"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="C48:F50"/>
     <mergeCell ref="A35:J35"/>
-    <mergeCell ref="A51:J52"/>
+    <mergeCell ref="A4:J4"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A48:B50"/>
     <mergeCell ref="C45:F46"/>
-    <mergeCell ref="A48:B50"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A9:D9"/>
     <mergeCell ref="G40:J40"/>
-    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="C53:F53"/>
     <mergeCell ref="G44:J46"/>
     <mergeCell ref="G43:J43"/>
     <mergeCell ref="A46:B46"/>
@@ -3610,8 +3596,8 @@
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C43:F43"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C43:F43"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="H9:J9"/>
   </mergeCells>
@@ -3657,29 +3643,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Hoja31">
+  <sheetPr codeName="Hoja28">
     <tabColor rgb="FF90E8F4"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A4:Q57"/>
   <sheetViews>
-    <sheetView showZeros="0" showWhiteSpace="0" view="pageLayout" topLeftCell="A37" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:B46"/>
+    <sheetView showZeros="0" showWhiteSpace="0" view="pageLayout" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col width="11.140625" customWidth="1" style="53" min="1" max="1"/>
-    <col width="19.42578125" customWidth="1" style="53" min="2" max="2"/>
-    <col width="7.85546875" customWidth="1" style="53" min="3" max="3"/>
-    <col width="5.85546875" customWidth="1" style="53" min="4" max="4"/>
-    <col width="13.140625" customWidth="1" style="53" min="5" max="5"/>
-    <col width="13.7109375" customWidth="1" style="53" min="6" max="6"/>
-    <col width="12.5703125" customWidth="1" style="53" min="7" max="7"/>
-    <col width="12.42578125" customWidth="1" style="53" min="8" max="8"/>
-    <col width="12" customWidth="1" style="53" min="9" max="9"/>
-    <col width="9.7109375" customWidth="1" style="53" min="10" max="10"/>
+    <col width="11.140625" customWidth="1" style="94" min="1" max="1"/>
+    <col width="19.42578125" customWidth="1" style="94" min="2" max="2"/>
+    <col width="7.85546875" customWidth="1" style="94" min="3" max="3"/>
+    <col width="5.85546875" customWidth="1" style="94" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" style="94" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" style="94" min="6" max="6"/>
+    <col width="12.5703125" customWidth="1" style="94" min="7" max="7"/>
+    <col width="12.42578125" customWidth="1" style="94" min="8" max="8"/>
+    <col width="12" customWidth="1" style="94" min="9" max="9"/>
+    <col width="9.7109375" customWidth="1" style="94" min="10" max="10"/>
     <col width="12.140625" customWidth="1" style="2" min="11" max="11"/>
     <col width="11.42578125" customWidth="1" style="3" min="12" max="15"/>
     <col width="25.42578125" customWidth="1" style="3" min="16" max="16"/>
@@ -3688,154 +3674,154 @@
     <col width="11.42578125" customWidth="1" style="3" min="20" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" s="87"/>
-    <row r="2" ht="12" customHeight="1" s="87"/>
-    <row r="3" ht="32.25" customHeight="1" s="87"/>
-    <row r="4" ht="12" customHeight="1" s="87">
-      <c r="A4" s="81" t="inlineStr">
+    <row r="1" ht="12" customHeight="1" s="96"/>
+    <row r="2" ht="12" customHeight="1" s="96"/>
+    <row r="3" ht="32.25" customHeight="1" s="96"/>
+    <row r="4" ht="12" customHeight="1" s="96">
+      <c r="A4" s="89" t="inlineStr">
         <is>
           <t>“2024. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="82" t="inlineStr">
+      <c r="A5" s="90" t="inlineStr">
         <is>
           <t>Asignación Académica</t>
         </is>
       </c>
-      <c r="B5" s="76" t="n"/>
-      <c r="C5" s="76" t="n"/>
-      <c r="D5" s="76" t="n"/>
-      <c r="E5" s="76" t="n"/>
-      <c r="F5" s="76" t="n"/>
-      <c r="G5" s="76" t="n"/>
-      <c r="H5" s="76" t="n"/>
-      <c r="I5" s="76" t="n"/>
-      <c r="J5" s="64" t="n"/>
-    </row>
-    <row r="6" ht="12" customHeight="1" s="87">
-      <c r="A6" s="77" t="inlineStr">
+      <c r="B5" s="81" t="n"/>
+      <c r="C5" s="81" t="n"/>
+      <c r="D5" s="81" t="n"/>
+      <c r="E5" s="81" t="n"/>
+      <c r="F5" s="81" t="n"/>
+      <c r="G5" s="81" t="n"/>
+      <c r="H5" s="81" t="n"/>
+      <c r="I5" s="81" t="n"/>
+      <c r="J5" s="82" t="n"/>
+    </row>
+    <row r="6" ht="12" customHeight="1" s="96">
+      <c r="A6" s="83" t="inlineStr">
         <is>
           <t>NOMBRE:</t>
         </is>
       </c>
-      <c r="B6" s="55" t="n"/>
-      <c r="C6" s="55" t="n"/>
-      <c r="D6" s="56" t="n"/>
-      <c r="E6" s="77" t="inlineStr">
+      <c r="B6" s="58" t="n"/>
+      <c r="C6" s="58" t="n"/>
+      <c r="D6" s="59" t="n"/>
+      <c r="E6" s="83" t="inlineStr">
         <is>
           <t>PROFESION:</t>
         </is>
       </c>
-      <c r="F6" s="55" t="n"/>
-      <c r="G6" s="55" t="n"/>
-      <c r="H6" s="55" t="n"/>
-      <c r="I6" s="55" t="n"/>
-      <c r="J6" s="56" t="n"/>
-    </row>
-    <row r="7" ht="12" customHeight="1" s="87">
-      <c r="A7" s="83" t="inlineStr">
+      <c r="F6" s="58" t="n"/>
+      <c r="G6" s="58" t="n"/>
+      <c r="H6" s="58" t="n"/>
+      <c r="I6" s="58" t="n"/>
+      <c r="J6" s="59" t="n"/>
+    </row>
+    <row r="7" ht="12" customHeight="1" s="96">
+      <c r="A7" s="91" t="inlineStr">
         <is>
           <t>AGUILAR ORTEGA RICARDO</t>
         </is>
       </c>
-      <c r="B7" s="61" t="n"/>
-      <c r="C7" s="61" t="n"/>
-      <c r="D7" s="62" t="n"/>
-      <c r="E7" s="80" t="inlineStr">
+      <c r="B7" s="64" t="n"/>
+      <c r="C7" s="64" t="n"/>
+      <c r="D7" s="65" t="n"/>
+      <c r="E7" s="86" t="inlineStr">
         <is>
           <t>ING. CIVIL / M. EN RELACIONES INTERINSTITUCIONALES</t>
         </is>
       </c>
-      <c r="F7" s="61" t="n"/>
-      <c r="G7" s="61" t="n"/>
-      <c r="H7" s="61" t="n"/>
-      <c r="I7" s="61" t="n"/>
-      <c r="J7" s="62" t="n"/>
-    </row>
-    <row r="8" ht="12" customHeight="1" s="87">
-      <c r="A8" s="77" t="inlineStr">
+      <c r="F7" s="64" t="n"/>
+      <c r="G7" s="64" t="n"/>
+      <c r="H7" s="64" t="n"/>
+      <c r="I7" s="64" t="n"/>
+      <c r="J7" s="65" t="n"/>
+    </row>
+    <row r="8" ht="12" customHeight="1" s="96">
+      <c r="A8" s="83" t="inlineStr">
         <is>
           <t>ADSCRIPCIÓN:</t>
         </is>
       </c>
-      <c r="B8" s="55" t="n"/>
-      <c r="C8" s="55" t="n"/>
-      <c r="D8" s="56" t="n"/>
-      <c r="E8" s="77" t="inlineStr">
+      <c r="B8" s="58" t="n"/>
+      <c r="C8" s="58" t="n"/>
+      <c r="D8" s="59" t="n"/>
+      <c r="E8" s="83" t="inlineStr">
         <is>
           <t>INGRESO AL TECNOLÓGICO</t>
         </is>
       </c>
-      <c r="F8" s="55" t="n"/>
-      <c r="G8" s="56" t="n"/>
-      <c r="H8" s="77" t="inlineStr">
+      <c r="F8" s="58" t="n"/>
+      <c r="G8" s="59" t="n"/>
+      <c r="H8" s="83" t="inlineStr">
         <is>
           <t>TIEMPO INDETERMINADO</t>
         </is>
       </c>
-      <c r="I8" s="55" t="n"/>
-      <c r="J8" s="56" t="n"/>
-    </row>
-    <row r="9" ht="12" customHeight="1" s="87">
-      <c r="A9" s="80" t="inlineStr">
+      <c r="I8" s="58" t="n"/>
+      <c r="J8" s="59" t="n"/>
+    </row>
+    <row r="9" ht="12" customHeight="1" s="96">
+      <c r="A9" s="86" t="inlineStr">
         <is>
           <t>PROFESOR DE ASIGNATURA DE ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B9" s="61" t="n"/>
-      <c r="C9" s="61" t="n"/>
-      <c r="D9" s="62" t="n"/>
-      <c r="E9" s="80" t="inlineStr">
+      <c r="B9" s="64" t="n"/>
+      <c r="C9" s="64" t="n"/>
+      <c r="D9" s="65" t="n"/>
+      <c r="E9" s="86" t="inlineStr">
         <is>
           <t>01 DE MARZO DE 2011</t>
         </is>
       </c>
-      <c r="F9" s="61" t="n"/>
-      <c r="G9" s="62" t="n"/>
-      <c r="H9" s="80" t="inlineStr">
+      <c r="F9" s="64" t="n"/>
+      <c r="G9" s="65" t="n"/>
+      <c r="H9" s="86" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="I9" s="61" t="n"/>
-      <c r="J9" s="62" t="n"/>
-    </row>
-    <row r="10" ht="12" customHeight="1" s="87">
-      <c r="A10" s="77" t="inlineStr">
+      <c r="I9" s="64" t="n"/>
+      <c r="J9" s="65" t="n"/>
+    </row>
+    <row r="10" ht="12" customHeight="1" s="96">
+      <c r="A10" s="83" t="inlineStr">
         <is>
           <t>PERIODO:</t>
         </is>
       </c>
-      <c r="B10" s="55" t="n"/>
-      <c r="C10" s="55" t="n"/>
-      <c r="D10" s="56" t="n"/>
-      <c r="E10" s="78" t="inlineStr">
+      <c r="B10" s="58" t="n"/>
+      <c r="C10" s="58" t="n"/>
+      <c r="D10" s="59" t="n"/>
+      <c r="E10" s="84" t="inlineStr">
         <is>
           <t>HORAS TIPO</t>
         </is>
       </c>
-      <c r="F10" s="76" t="n"/>
-      <c r="G10" s="76" t="n"/>
-      <c r="H10" s="64" t="n"/>
-      <c r="I10" s="78" t="inlineStr">
+      <c r="F10" s="81" t="n"/>
+      <c r="G10" s="81" t="n"/>
+      <c r="H10" s="82" t="n"/>
+      <c r="I10" s="84" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="J10" s="64" t="n"/>
-    </row>
-    <row r="11" ht="12" customHeight="1" s="87">
-      <c r="A11" s="79" t="inlineStr">
+      <c r="J10" s="82" t="n"/>
+    </row>
+    <row r="11" ht="12" customHeight="1" s="96">
+      <c r="A11" s="85" t="inlineStr">
         <is>
           <t>2024-1 (MARZO-AGOSTO 2024)</t>
         </is>
       </c>
-      <c r="B11" s="61" t="n"/>
-      <c r="C11" s="61" t="n"/>
-      <c r="D11" s="61" t="n"/>
-      <c r="E11" s="78" t="inlineStr">
+      <c r="B11" s="64" t="n"/>
+      <c r="C11" s="64" t="n"/>
+      <c r="D11" s="64" t="n"/>
+      <c r="E11" s="84" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -3861,7 +3847,7 @@
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
-    <row r="12" ht="5.1" customHeight="1" s="87">
+    <row r="12" ht="5.1" customHeight="1" s="96">
       <c r="A12" s="8" t="n"/>
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="8" t="n"/>
@@ -3873,23 +3859,23 @@
       <c r="I12" s="8" t="n"/>
       <c r="J12" s="8" t="n"/>
     </row>
-    <row r="13" ht="12" customHeight="1" s="87">
-      <c r="A13" s="78" t="inlineStr">
+    <row r="13" ht="12" customHeight="1" s="96">
+      <c r="A13" s="84" t="inlineStr">
         <is>
           <t>Asignación de Horas Frente a Grupo</t>
         </is>
       </c>
-      <c r="B13" s="76" t="n"/>
-      <c r="C13" s="76" t="n"/>
-      <c r="D13" s="76" t="n"/>
-      <c r="E13" s="76" t="n"/>
-      <c r="F13" s="76" t="n"/>
-      <c r="G13" s="76" t="n"/>
-      <c r="H13" s="76" t="n"/>
-      <c r="I13" s="76" t="n"/>
-      <c r="J13" s="64" t="n"/>
-    </row>
-    <row r="14" ht="12" customHeight="1" s="87">
+      <c r="B13" s="81" t="n"/>
+      <c r="C13" s="81" t="n"/>
+      <c r="D13" s="81" t="n"/>
+      <c r="E13" s="81" t="n"/>
+      <c r="F13" s="81" t="n"/>
+      <c r="G13" s="81" t="n"/>
+      <c r="H13" s="81" t="n"/>
+      <c r="I13" s="81" t="n"/>
+      <c r="J13" s="82" t="n"/>
+    </row>
+    <row r="14" ht="12" customHeight="1" s="96">
       <c r="A14" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -3993,9 +3979,9 @@
         </is>
       </c>
       <c r="K15" s="15" t="n"/>
-      <c r="N15" s="88" t="n"/>
-    </row>
-    <row r="16" ht="21.75" customHeight="1" s="87">
+      <c r="N15" s="97" t="n"/>
+    </row>
+    <row r="16" ht="21.75" customHeight="1" s="96">
       <c r="A16" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -4047,9 +4033,9 @@
         </is>
       </c>
       <c r="K16" s="17" t="n"/>
-      <c r="N16" s="88" t="n"/>
-    </row>
-    <row r="17" ht="21.75" customHeight="1" s="87">
+      <c r="N16" s="97" t="n"/>
+    </row>
+    <row r="17" ht="21.75" customHeight="1" s="96">
       <c r="A17" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -4155,7 +4141,7 @@
       </c>
       <c r="K18" s="17" t="n"/>
     </row>
-    <row r="19" ht="20.25" customHeight="1" s="87">
+    <row r="19" ht="20.25" customHeight="1" s="96">
       <c r="A19" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -4208,7 +4194,7 @@
       </c>
       <c r="K19" s="17" t="n"/>
     </row>
-    <row r="20" ht="19.5" customHeight="1" s="87">
+    <row r="20" ht="19.5" customHeight="1" s="96">
       <c r="A20" s="10" t="n"/>
       <c r="B20" s="11" t="inlineStr"/>
       <c r="C20" s="12" t="inlineStr">
@@ -4249,7 +4235,7 @@
       </c>
       <c r="K20" s="17" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="87">
+    <row r="21" ht="18" customHeight="1" s="96">
       <c r="A21" s="10" t="n"/>
       <c r="B21" s="11" t="inlineStr"/>
       <c r="C21" s="12" t="inlineStr">
@@ -4290,7 +4276,7 @@
       </c>
       <c r="K21" s="17" t="n"/>
     </row>
-    <row r="22" ht="18" customHeight="1" s="87">
+    <row r="22" ht="18" customHeight="1" s="96">
       <c r="A22" s="10" t="n"/>
       <c r="B22" s="11" t="inlineStr"/>
       <c r="C22" s="12" t="inlineStr">
@@ -4352,14 +4338,14 @@
       <c r="J23" s="23" t="n"/>
       <c r="K23" s="17" t="n"/>
     </row>
-    <row r="24" ht="12" customHeight="1" s="87">
-      <c r="A24" s="67" t="inlineStr">
+    <row r="24" ht="12" customHeight="1" s="96">
+      <c r="A24" s="72" t="inlineStr">
         <is>
           <t>Asignación de Horas de Descarga para otras Actividades</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="12" customHeight="1" s="87">
+    <row r="25" ht="12" customHeight="1" s="96">
       <c r="A25" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -4411,7 +4397,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="24.75" customHeight="1" s="87">
+    <row r="26" ht="24.75" customHeight="1" s="96">
       <c r="A26" s="24" t="n"/>
       <c r="B26" s="25" t="inlineStr">
         <is>
@@ -4460,7 +4446,7 @@
       </c>
       <c r="K26" s="27" t="n"/>
     </row>
-    <row r="27" ht="28.5" customHeight="1" s="87">
+    <row r="27" ht="28.5" customHeight="1" s="96">
       <c r="A27" s="24" t="n"/>
       <c r="B27" s="25" t="inlineStr">
         <is>
@@ -4509,7 +4495,7 @@
       </c>
       <c r="K27" s="27" t="n"/>
     </row>
-    <row r="28" ht="26.25" customHeight="1" s="87">
+    <row r="28" ht="26.25" customHeight="1" s="96">
       <c r="A28" s="24" t="n"/>
       <c r="B28" s="25" t="inlineStr">
         <is>
@@ -4558,7 +4544,7 @@
       </c>
       <c r="K28" s="27" t="n"/>
     </row>
-    <row r="29" ht="30" customHeight="1" s="87">
+    <row r="29" ht="30" customHeight="1" s="96">
       <c r="A29" s="24" t="n"/>
       <c r="B29" s="25" t="inlineStr">
         <is>
@@ -4607,7 +4593,7 @@
       </c>
       <c r="K29" s="27" t="n"/>
     </row>
-    <row r="30" ht="33" customHeight="1" s="87">
+    <row r="30" ht="33" customHeight="1" s="96">
       <c r="A30" s="24" t="n"/>
       <c r="B30" s="25" t="inlineStr">
         <is>
@@ -4656,7 +4642,7 @@
       </c>
       <c r="K30" s="27" t="n"/>
     </row>
-    <row r="31" ht="19.5" customHeight="1" s="87">
+    <row r="31" ht="19.5" customHeight="1" s="96">
       <c r="A31" s="24" t="n"/>
       <c r="B31" s="25" t="inlineStr"/>
       <c r="C31" s="26" t="inlineStr"/>
@@ -4693,7 +4679,7 @@
       </c>
       <c r="K31" s="27" t="n"/>
     </row>
-    <row r="32" ht="34.5" customHeight="1" s="87">
+    <row r="32" ht="34.5" customHeight="1" s="96">
       <c r="A32" s="24" t="n"/>
       <c r="B32" s="25" t="inlineStr"/>
       <c r="C32" s="26" t="inlineStr"/>
@@ -4730,7 +4716,7 @@
       </c>
       <c r="K32" s="27" t="n"/>
     </row>
-    <row r="33" ht="21" customHeight="1" s="87">
+    <row r="33" ht="21" customHeight="1" s="96">
       <c r="A33" s="24" t="n"/>
       <c r="B33" s="25" t="inlineStr"/>
       <c r="C33" s="26" t="inlineStr"/>
@@ -4788,14 +4774,14 @@
       <c r="J34" s="28" t="n"/>
       <c r="K34" s="27" t="n"/>
     </row>
-    <row r="35" ht="12" customHeight="1" s="87">
-      <c r="A35" s="67" t="inlineStr">
+    <row r="35" ht="12" customHeight="1" s="96">
+      <c r="A35" s="72" t="inlineStr">
         <is>
           <t>Asignación de Horas de Presidente y Secretario de Academia</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="12" customHeight="1" s="87">
+    <row r="36" ht="12" customHeight="1" s="96">
       <c r="A36" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -4847,7 +4833,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="87">
+    <row r="37" ht="18.75" customHeight="1" s="96">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="25" t="inlineStr">
         <is>
@@ -4888,7 +4874,7 @@
       </c>
       <c r="K37" s="31" t="n"/>
     </row>
-    <row r="38" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="38" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A38" s="32" t="n"/>
       <c r="B38" s="33" t="n"/>
       <c r="C38" s="34" t="inlineStr">
@@ -4904,14 +4890,14 @@
       <c r="I38" s="26" t="n"/>
       <c r="J38" s="35" t="n"/>
     </row>
-    <row r="39" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="39" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A39" s="36" t="n"/>
-      <c r="B39" s="68" t="inlineStr">
+      <c r="B39" s="73" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="C39" s="69" t="n"/>
+      <c r="C39" s="74" t="n"/>
       <c r="D39" s="37" t="n">
         <v>28</v>
       </c>
@@ -4922,31 +4908,31 @@
       <c r="I39" s="38" t="n"/>
       <c r="J39" s="39" t="n"/>
     </row>
-    <row r="40" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="40" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A40" s="36" t="n"/>
       <c r="B40" s="40" t="n"/>
       <c r="C40" s="41" t="n"/>
       <c r="D40" s="38" t="n"/>
-      <c r="E40" s="70" t="inlineStr">
+      <c r="E40" s="75" t="inlineStr">
         <is>
           <t>FECHA DE APLICACIÓN</t>
         </is>
       </c>
-      <c r="G40" s="71" t="inlineStr">
-        <is>
-          <t>25/01/2025</t>
-        </is>
-      </c>
-      <c r="H40" s="69" t="n"/>
-      <c r="I40" s="69" t="n"/>
-      <c r="J40" s="72" t="n"/>
-    </row>
-    <row r="41" ht="12" customHeight="1" s="87" thickBot="1">
+      <c r="G40" s="76" t="inlineStr">
+        <is>
+          <t>28/01/2025</t>
+        </is>
+      </c>
+      <c r="H40" s="74" t="n"/>
+      <c r="I40" s="74" t="n"/>
+      <c r="J40" s="77" t="n"/>
+    </row>
+    <row r="41" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A41" s="36" t="n"/>
       <c r="B41" s="40" t="n"/>
       <c r="C41" s="41" t="n"/>
       <c r="D41" s="38" t="n"/>
-      <c r="E41" s="70" t="inlineStr">
+      <c r="E41" s="75" t="inlineStr">
         <is>
           <t>CONSECUTIVO</t>
         </is>
@@ -4960,7 +4946,7 @@
       <c r="I41" s="38" t="n"/>
       <c r="J41" s="39" t="n"/>
     </row>
-    <row r="42" ht="9.75" customFormat="1" customHeight="1" s="58">
+    <row r="42" ht="9.75" customFormat="1" customHeight="1" s="61">
       <c r="C42" s="44" t="n"/>
       <c r="D42" s="44" t="n"/>
       <c r="E42" s="44" t="n"/>
@@ -4971,72 +4957,80 @@
       <c r="J42" s="44" t="n"/>
       <c r="K42" s="45" t="n"/>
     </row>
-    <row r="43" customFormat="1" s="58">
-      <c r="A43" s="73" t="n"/>
-      <c r="B43" s="56" t="n"/>
-      <c r="C43" s="74" t="inlineStr">
+    <row r="43" customFormat="1" s="61">
+      <c r="A43" s="78" t="inlineStr">
+        <is>
+          <t>JEFA DE DIVISIÓN DE ING. INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B43" s="59" t="n"/>
+      <c r="C43" s="79" t="inlineStr">
         <is>
           <t>REVISO</t>
         </is>
       </c>
-      <c r="D43" s="55" t="n"/>
-      <c r="E43" s="55" t="n"/>
-      <c r="F43" s="56" t="n"/>
-      <c r="G43" s="75" t="inlineStr">
+      <c r="D43" s="58" t="n"/>
+      <c r="E43" s="58" t="n"/>
+      <c r="F43" s="59" t="n"/>
+      <c r="G43" s="80" t="inlineStr">
         <is>
           <t>FIRMA DE CONFORMIDAD</t>
         </is>
       </c>
-      <c r="H43" s="76" t="n"/>
-      <c r="I43" s="76" t="n"/>
-      <c r="J43" s="64" t="n"/>
+      <c r="H43" s="81" t="n"/>
+      <c r="I43" s="81" t="n"/>
+      <c r="J43" s="82" t="n"/>
       <c r="K43" s="45" t="n"/>
     </row>
-    <row r="44" ht="16.5" customFormat="1" customHeight="1" s="58">
+    <row r="44" ht="16.5" customFormat="1" customHeight="1" s="61">
       <c r="A44" s="46" t="n"/>
       <c r="B44" s="47" t="n"/>
       <c r="C44" s="48" t="n"/>
       <c r="D44" s="48" t="n"/>
       <c r="E44" s="48" t="n"/>
       <c r="F44" s="49" t="n"/>
-      <c r="G44" s="54" t="inlineStr">
+      <c r="G44" s="57" t="inlineStr">
         <is>
           <t>AGUILAR ORTEGA RICARDO</t>
         </is>
       </c>
-      <c r="H44" s="55" t="n"/>
-      <c r="I44" s="55" t="n"/>
-      <c r="J44" s="56" t="n"/>
+      <c r="H44" s="58" t="n"/>
+      <c r="I44" s="58" t="n"/>
+      <c r="J44" s="59" t="n"/>
       <c r="K44" s="45" t="n"/>
     </row>
-    <row r="45" ht="12" customFormat="1" customHeight="1" s="58">
+    <row r="45" ht="12" customFormat="1" customHeight="1" s="61">
       <c r="A45" s="0" t="n"/>
       <c r="B45" s="0" t="n"/>
-      <c r="C45" s="63" t="inlineStr">
+      <c r="C45" s="66" t="inlineStr">
         <is>
           <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ
 ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
         </is>
       </c>
-      <c r="F45" s="59" t="n"/>
-      <c r="G45" s="57" t="n"/>
-      <c r="J45" s="59" t="n"/>
+      <c r="F45" s="62" t="n"/>
+      <c r="G45" s="60" t="n"/>
+      <c r="J45" s="62" t="n"/>
       <c r="K45" s="45" t="n"/>
     </row>
-    <row r="46" ht="37.5" customFormat="1" customHeight="1" s="58">
-      <c r="A46" s="86" t="n"/>
-      <c r="B46" s="62" t="n"/>
-      <c r="C46" s="60" t="n"/>
-      <c r="D46" s="61" t="n"/>
-      <c r="E46" s="61" t="n"/>
-      <c r="F46" s="62" t="n"/>
-      <c r="G46" s="60" t="n"/>
-      <c r="H46" s="61" t="n"/>
-      <c r="I46" s="61" t="n"/>
-      <c r="J46" s="62" t="n"/>
+    <row r="46" ht="37.5" customFormat="1" customHeight="1" s="61">
+      <c r="A46" s="67" t="inlineStr">
+        <is>
+          <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
+        </is>
+      </c>
+      <c r="B46" s="65" t="n"/>
+      <c r="C46" s="63" t="n"/>
+      <c r="D46" s="64" t="n"/>
+      <c r="E46" s="64" t="n"/>
+      <c r="F46" s="65" t="n"/>
+      <c r="G46" s="63" t="n"/>
+      <c r="H46" s="64" t="n"/>
+      <c r="I46" s="64" t="n"/>
+      <c r="J46" s="65" t="n"/>
       <c r="K46" s="45" t="n"/>
     </row>
-    <row r="47" ht="1.35" customHeight="1" s="87">
+    <row r="47" ht="1.35" customHeight="1" s="96">
       <c r="A47" s="50" t="n"/>
       <c r="B47" s="50" t="n"/>
       <c r="C47" s="50" t="n"/>
@@ -5050,35 +5044,71 @@
       <c r="P47" s="51" t="n"/>
       <c r="Q47" s="51" t="n"/>
     </row>
-    <row r="48" ht="12.75" customHeight="1" s="87">
-      <c r="A48" s="65" t="n"/>
-      <c r="C48" s="66" t="n"/>
-      <c r="G48" s="66" t="n"/>
+    <row r="48" ht="12.75" customHeight="1" s="96">
+      <c r="A48" s="68" t="n"/>
+      <c r="C48" s="99" t="inlineStr">
+        <is>
+          <t>Vo. Bo</t>
+        </is>
+      </c>
+      <c r="G48" s="93" t="n"/>
       <c r="K48" s="3" t="n"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1" s="87">
+    <row r="49" ht="12.75" customHeight="1" s="96">
       <c r="K49" s="3" t="n"/>
     </row>
-    <row r="50" ht="12.75" customHeight="1" s="87">
+    <row r="50" ht="21" customHeight="1" s="96" thickBot="1">
+      <c r="C50" s="100" t="n"/>
+      <c r="D50" s="100" t="n"/>
+      <c r="E50" s="100" t="n"/>
+      <c r="F50" s="100" t="n"/>
       <c r="K50" s="3" t="n"/>
     </row>
-    <row r="51" ht="17.25" customHeight="1" s="87">
+    <row r="51" ht="3" customHeight="1" s="96">
       <c r="A51" s="52" t="n"/>
+      <c r="B51" s="53" t="n"/>
+      <c r="C51" s="53" t="n"/>
+      <c r="D51" s="53" t="n"/>
+      <c r="E51" s="53" t="n"/>
+      <c r="F51" s="53" t="n"/>
+      <c r="G51" s="53" t="n"/>
+      <c r="H51" s="53" t="n"/>
+      <c r="I51" s="53" t="n"/>
+      <c r="J51" s="53" t="n"/>
       <c r="K51" s="3" t="n"/>
     </row>
-    <row r="52" ht="30" customHeight="1" s="87"/>
+    <row r="52" ht="10.5" customHeight="1" s="96">
+      <c r="A52" s="53" t="n"/>
+      <c r="B52" s="53" t="n"/>
+      <c r="C52" s="54" t="inlineStr">
+        <is>
+          <t>DRA C.CLAUDIA PÉREZ MARTÍNEZ</t>
+        </is>
+      </c>
+      <c r="G52" s="53" t="n"/>
+      <c r="H52" s="53" t="n"/>
+      <c r="I52" s="53" t="n"/>
+      <c r="J52" s="53" t="n"/>
+    </row>
+    <row r="53">
+      <c r="C53" s="54" t="inlineStr">
+        <is>
+          <t>DIRECTORA GENERAL</t>
+        </is>
+      </c>
+    </row>
     <row r="57">
       <c r="K57" s="3" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="C52:F52"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="C48:F50"/>
     <mergeCell ref="A35:J35"/>
-    <mergeCell ref="A51:J52"/>
+    <mergeCell ref="A4:J4"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="A4:J4"/>
     <mergeCell ref="C45:F46"/>
     <mergeCell ref="A48:B50"/>
     <mergeCell ref="A10:D10"/>
@@ -5086,6 +5116,7 @@
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="G40:J40"/>
+    <mergeCell ref="C53:F53"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="G44:J46"/>
     <mergeCell ref="G43:J43"/>
@@ -5148,29 +5179,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Hoja30">
+  <sheetPr codeName="Hoja27">
     <tabColor rgb="FF90E8F4"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A4:Q57"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A37" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showZeros="0" showWhiteSpace="0" view="pageLayout" topLeftCell="A37" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="A46" sqref="A46:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col width="11.140625" customWidth="1" style="53" min="1" max="1"/>
-    <col width="19.42578125" customWidth="1" style="53" min="2" max="2"/>
-    <col width="7.85546875" customWidth="1" style="53" min="3" max="3"/>
-    <col width="5.85546875" customWidth="1" style="53" min="4" max="4"/>
-    <col width="13.140625" customWidth="1" style="53" min="5" max="5"/>
-    <col width="13.7109375" customWidth="1" style="53" min="6" max="6"/>
-    <col width="12.5703125" customWidth="1" style="53" min="7" max="7"/>
-    <col width="12.42578125" customWidth="1" style="53" min="8" max="8"/>
-    <col width="12" customWidth="1" style="53" min="9" max="9"/>
-    <col width="9.7109375" customWidth="1" style="53" min="10" max="10"/>
+    <col width="11.140625" customWidth="1" style="94" min="1" max="1"/>
+    <col width="19.42578125" customWidth="1" style="94" min="2" max="2"/>
+    <col width="7.85546875" customWidth="1" style="94" min="3" max="3"/>
+    <col width="5.85546875" customWidth="1" style="94" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" style="94" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" style="94" min="6" max="6"/>
+    <col width="12.5703125" customWidth="1" style="94" min="7" max="7"/>
+    <col width="12.42578125" customWidth="1" style="94" min="8" max="8"/>
+    <col width="12" customWidth="1" style="94" min="9" max="9"/>
+    <col width="9.7109375" customWidth="1" style="94" min="10" max="10"/>
     <col width="12.140625" customWidth="1" style="2" min="11" max="11"/>
     <col width="11.42578125" customWidth="1" style="3" min="12" max="15"/>
     <col width="25.42578125" customWidth="1" style="3" min="16" max="16"/>
@@ -5179,154 +5210,154 @@
     <col width="11.42578125" customWidth="1" style="3" min="20" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" s="87"/>
-    <row r="2" ht="12" customHeight="1" s="87"/>
-    <row r="3" ht="32.25" customHeight="1" s="87"/>
-    <row r="4" ht="12" customHeight="1" s="87">
-      <c r="A4" s="81" t="inlineStr">
+    <row r="1" ht="12" customHeight="1" s="96"/>
+    <row r="2" ht="12" customHeight="1" s="96"/>
+    <row r="3" ht="32.25" customHeight="1" s="96"/>
+    <row r="4" ht="12" customHeight="1" s="96">
+      <c r="A4" s="89" t="inlineStr">
         <is>
           <t>“2024. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="82" t="inlineStr">
+      <c r="A5" s="90" t="inlineStr">
         <is>
           <t>Asignación Académica</t>
         </is>
       </c>
-      <c r="B5" s="76" t="n"/>
-      <c r="C5" s="76" t="n"/>
-      <c r="D5" s="76" t="n"/>
-      <c r="E5" s="76" t="n"/>
-      <c r="F5" s="76" t="n"/>
-      <c r="G5" s="76" t="n"/>
-      <c r="H5" s="76" t="n"/>
-      <c r="I5" s="76" t="n"/>
-      <c r="J5" s="64" t="n"/>
-    </row>
-    <row r="6" ht="12" customHeight="1" s="87">
-      <c r="A6" s="77" t="inlineStr">
+      <c r="B5" s="81" t="n"/>
+      <c r="C5" s="81" t="n"/>
+      <c r="D5" s="81" t="n"/>
+      <c r="E5" s="81" t="n"/>
+      <c r="F5" s="81" t="n"/>
+      <c r="G5" s="81" t="n"/>
+      <c r="H5" s="81" t="n"/>
+      <c r="I5" s="81" t="n"/>
+      <c r="J5" s="82" t="n"/>
+    </row>
+    <row r="6" ht="12" customHeight="1" s="96">
+      <c r="A6" s="83" t="inlineStr">
         <is>
           <t>NOMBRE:</t>
         </is>
       </c>
-      <c r="B6" s="55" t="n"/>
-      <c r="C6" s="55" t="n"/>
-      <c r="D6" s="56" t="n"/>
-      <c r="E6" s="77" t="inlineStr">
+      <c r="B6" s="58" t="n"/>
+      <c r="C6" s="58" t="n"/>
+      <c r="D6" s="59" t="n"/>
+      <c r="E6" s="83" t="inlineStr">
         <is>
           <t>PROFESION:</t>
         </is>
       </c>
-      <c r="F6" s="55" t="n"/>
-      <c r="G6" s="55" t="n"/>
-      <c r="H6" s="55" t="n"/>
-      <c r="I6" s="55" t="n"/>
-      <c r="J6" s="56" t="n"/>
-    </row>
-    <row r="7" ht="12" customHeight="1" s="87">
-      <c r="A7" s="83" t="inlineStr">
+      <c r="F6" s="58" t="n"/>
+      <c r="G6" s="58" t="n"/>
+      <c r="H6" s="58" t="n"/>
+      <c r="I6" s="58" t="n"/>
+      <c r="J6" s="59" t="n"/>
+    </row>
+    <row r="7" ht="12" customHeight="1" s="96">
+      <c r="A7" s="91" t="inlineStr">
         <is>
           <t xml:space="preserve">AVILA GARCÍA LORENZO </t>
         </is>
       </c>
-      <c r="B7" s="61" t="n"/>
-      <c r="C7" s="61" t="n"/>
-      <c r="D7" s="62" t="n"/>
-      <c r="E7" s="80" t="inlineStr">
+      <c r="B7" s="64" t="n"/>
+      <c r="C7" s="64" t="n"/>
+      <c r="D7" s="65" t="n"/>
+      <c r="E7" s="86" t="inlineStr">
         <is>
           <t>ING. INDUSTRIAL / M. EN RELACIONES INTERINSTITUCIONALES</t>
         </is>
       </c>
-      <c r="F7" s="61" t="n"/>
-      <c r="G7" s="61" t="n"/>
-      <c r="H7" s="61" t="n"/>
-      <c r="I7" s="61" t="n"/>
-      <c r="J7" s="62" t="n"/>
-    </row>
-    <row r="8" ht="12" customHeight="1" s="87">
-      <c r="A8" s="77" t="inlineStr">
+      <c r="F7" s="64" t="n"/>
+      <c r="G7" s="64" t="n"/>
+      <c r="H7" s="64" t="n"/>
+      <c r="I7" s="64" t="n"/>
+      <c r="J7" s="65" t="n"/>
+    </row>
+    <row r="8" ht="12" customHeight="1" s="96">
+      <c r="A8" s="83" t="inlineStr">
         <is>
           <t>ADSCRIPCIÓN:</t>
         </is>
       </c>
-      <c r="B8" s="55" t="n"/>
-      <c r="C8" s="55" t="n"/>
-      <c r="D8" s="56" t="n"/>
-      <c r="E8" s="77" t="inlineStr">
+      <c r="B8" s="58" t="n"/>
+      <c r="C8" s="58" t="n"/>
+      <c r="D8" s="59" t="n"/>
+      <c r="E8" s="83" t="inlineStr">
         <is>
           <t>INGRESO AL TECNOLÓGICO</t>
         </is>
       </c>
-      <c r="F8" s="55" t="n"/>
-      <c r="G8" s="56" t="n"/>
-      <c r="H8" s="77" t="inlineStr">
+      <c r="F8" s="58" t="n"/>
+      <c r="G8" s="59" t="n"/>
+      <c r="H8" s="83" t="inlineStr">
         <is>
           <t>TIEMPO INDETERMINADO</t>
         </is>
       </c>
-      <c r="I8" s="55" t="n"/>
-      <c r="J8" s="56" t="n"/>
-    </row>
-    <row r="9" ht="12" customHeight="1" s="87">
-      <c r="A9" s="80" t="inlineStr">
+      <c r="I8" s="58" t="n"/>
+      <c r="J8" s="59" t="n"/>
+    </row>
+    <row r="9" ht="12" customHeight="1" s="96">
+      <c r="A9" s="86" t="inlineStr">
         <is>
           <t>PTC ASOCIADO "B" DE ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B9" s="61" t="n"/>
-      <c r="C9" s="61" t="n"/>
-      <c r="D9" s="62" t="n"/>
-      <c r="E9" s="80" t="inlineStr">
+      <c r="B9" s="64" t="n"/>
+      <c r="C9" s="64" t="n"/>
+      <c r="D9" s="65" t="n"/>
+      <c r="E9" s="86" t="inlineStr">
         <is>
           <t>01 DE ENERO DE 1999</t>
         </is>
       </c>
-      <c r="F9" s="61" t="n"/>
-      <c r="G9" s="62" t="n"/>
-      <c r="H9" s="80" t="inlineStr">
+      <c r="F9" s="64" t="n"/>
+      <c r="G9" s="65" t="n"/>
+      <c r="H9" s="86" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
       </c>
-      <c r="I9" s="61" t="n"/>
-      <c r="J9" s="62" t="n"/>
-    </row>
-    <row r="10" ht="12" customHeight="1" s="87">
-      <c r="A10" s="77" t="inlineStr">
+      <c r="I9" s="64" t="n"/>
+      <c r="J9" s="65" t="n"/>
+    </row>
+    <row r="10" ht="12" customHeight="1" s="96">
+      <c r="A10" s="83" t="inlineStr">
         <is>
           <t>PERIODO:</t>
         </is>
       </c>
-      <c r="B10" s="55" t="n"/>
-      <c r="C10" s="55" t="n"/>
-      <c r="D10" s="56" t="n"/>
-      <c r="E10" s="78" t="inlineStr">
+      <c r="B10" s="58" t="n"/>
+      <c r="C10" s="58" t="n"/>
+      <c r="D10" s="59" t="n"/>
+      <c r="E10" s="84" t="inlineStr">
         <is>
           <t>HORAS TIPO</t>
         </is>
       </c>
-      <c r="F10" s="76" t="n"/>
-      <c r="G10" s="76" t="n"/>
-      <c r="H10" s="64" t="n"/>
-      <c r="I10" s="78" t="inlineStr">
+      <c r="F10" s="81" t="n"/>
+      <c r="G10" s="81" t="n"/>
+      <c r="H10" s="82" t="n"/>
+      <c r="I10" s="84" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="J10" s="64" t="n"/>
-    </row>
-    <row r="11" ht="12" customHeight="1" s="87">
-      <c r="A11" s="79" t="inlineStr">
+      <c r="J10" s="82" t="n"/>
+    </row>
+    <row r="11" ht="12" customHeight="1" s="96">
+      <c r="A11" s="85" t="inlineStr">
         <is>
           <t>2024-1 (MARZO-AGOSTO 2024)</t>
         </is>
       </c>
-      <c r="B11" s="61" t="n"/>
-      <c r="C11" s="61" t="n"/>
-      <c r="D11" s="61" t="n"/>
-      <c r="E11" s="78" t="inlineStr">
+      <c r="B11" s="64" t="n"/>
+      <c r="C11" s="64" t="n"/>
+      <c r="D11" s="64" t="n"/>
+      <c r="E11" s="84" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -5352,7 +5383,7 @@
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
-    <row r="12" ht="5.1" customHeight="1" s="87">
+    <row r="12" ht="5.1" customHeight="1" s="96">
       <c r="A12" s="8" t="n"/>
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="8" t="n"/>
@@ -5364,23 +5395,23 @@
       <c r="I12" s="8" t="n"/>
       <c r="J12" s="8" t="n"/>
     </row>
-    <row r="13" ht="12" customHeight="1" s="87">
-      <c r="A13" s="78" t="inlineStr">
+    <row r="13" ht="12" customHeight="1" s="96">
+      <c r="A13" s="84" t="inlineStr">
         <is>
           <t>Asignación de Horas Frente a Grupo</t>
         </is>
       </c>
-      <c r="B13" s="76" t="n"/>
-      <c r="C13" s="76" t="n"/>
-      <c r="D13" s="76" t="n"/>
-      <c r="E13" s="76" t="n"/>
-      <c r="F13" s="76" t="n"/>
-      <c r="G13" s="76" t="n"/>
-      <c r="H13" s="76" t="n"/>
-      <c r="I13" s="76" t="n"/>
-      <c r="J13" s="64" t="n"/>
-    </row>
-    <row r="14" ht="12" customHeight="1" s="87">
+      <c r="B13" s="81" t="n"/>
+      <c r="C13" s="81" t="n"/>
+      <c r="D13" s="81" t="n"/>
+      <c r="E13" s="81" t="n"/>
+      <c r="F13" s="81" t="n"/>
+      <c r="G13" s="81" t="n"/>
+      <c r="H13" s="81" t="n"/>
+      <c r="I13" s="81" t="n"/>
+      <c r="J13" s="82" t="n"/>
+    </row>
+    <row r="14" ht="12" customHeight="1" s="96">
       <c r="A14" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -5484,9 +5515,9 @@
         </is>
       </c>
       <c r="K15" s="15" t="n"/>
-      <c r="N15" s="88" t="n"/>
-    </row>
-    <row r="16" ht="21.75" customHeight="1" s="87">
+      <c r="N15" s="97" t="n"/>
+    </row>
+    <row r="16" ht="21.75" customHeight="1" s="96">
       <c r="A16" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -5538,9 +5569,9 @@
         </is>
       </c>
       <c r="K16" s="17" t="n"/>
-      <c r="N16" s="88" t="n"/>
-    </row>
-    <row r="17" ht="21.75" customHeight="1" s="87">
+      <c r="N16" s="97" t="n"/>
+    </row>
+    <row r="17" ht="21.75" customHeight="1" s="96">
       <c r="A17" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -5646,7 +5677,7 @@
       </c>
       <c r="K18" s="17" t="n"/>
     </row>
-    <row r="19" ht="20.25" customHeight="1" s="87">
+    <row r="19" ht="20.25" customHeight="1" s="96">
       <c r="A19" s="10" t="n"/>
       <c r="B19" s="11" t="inlineStr"/>
       <c r="C19" s="12" t="inlineStr">
@@ -5687,7 +5718,7 @@
       </c>
       <c r="K19" s="17" t="n"/>
     </row>
-    <row r="20" ht="19.5" customHeight="1" s="87">
+    <row r="20" ht="19.5" customHeight="1" s="96">
       <c r="A20" s="10" t="n"/>
       <c r="B20" s="11" t="inlineStr"/>
       <c r="C20" s="12" t="inlineStr">
@@ -5728,7 +5759,7 @@
       </c>
       <c r="K20" s="17" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="87">
+    <row r="21" ht="18" customHeight="1" s="96">
       <c r="A21" s="10" t="n"/>
       <c r="B21" s="11" t="inlineStr"/>
       <c r="C21" s="12" t="inlineStr">
@@ -5769,7 +5800,7 @@
       </c>
       <c r="K21" s="17" t="n"/>
     </row>
-    <row r="22" ht="18" customHeight="1" s="87">
+    <row r="22" ht="18" customHeight="1" s="96">
       <c r="A22" s="10" t="n"/>
       <c r="B22" s="11" t="inlineStr"/>
       <c r="C22" s="12" t="inlineStr">
@@ -5831,14 +5862,14 @@
       <c r="J23" s="23" t="n"/>
       <c r="K23" s="17" t="n"/>
     </row>
-    <row r="24" ht="12" customHeight="1" s="87">
-      <c r="A24" s="67" t="inlineStr">
+    <row r="24" ht="12" customHeight="1" s="96">
+      <c r="A24" s="72" t="inlineStr">
         <is>
           <t>Asignación de Horas de Descarga para otras Actividades</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="12" customHeight="1" s="87">
+    <row r="25" ht="12" customHeight="1" s="96">
       <c r="A25" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -5890,7 +5921,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="24.75" customHeight="1" s="87">
+    <row r="26" ht="24.75" customHeight="1" s="96">
       <c r="A26" s="24" t="n"/>
       <c r="B26" s="25" t="inlineStr">
         <is>
@@ -5939,7 +5970,7 @@
       </c>
       <c r="K26" s="27" t="n"/>
     </row>
-    <row r="27" ht="28.5" customHeight="1" s="87">
+    <row r="27" ht="28.5" customHeight="1" s="96">
       <c r="A27" s="24" t="n"/>
       <c r="B27" s="25" t="inlineStr">
         <is>
@@ -5988,7 +6019,7 @@
       </c>
       <c r="K27" s="27" t="n"/>
     </row>
-    <row r="28" ht="26.25" customHeight="1" s="87">
+    <row r="28" ht="26.25" customHeight="1" s="96">
       <c r="A28" s="24" t="n"/>
       <c r="B28" s="25" t="inlineStr">
         <is>
@@ -6037,7 +6068,7 @@
       </c>
       <c r="K28" s="27" t="n"/>
     </row>
-    <row r="29" ht="30" customHeight="1" s="87">
+    <row r="29" ht="30" customHeight="1" s="96">
       <c r="A29" s="24" t="n"/>
       <c r="B29" s="25" t="inlineStr">
         <is>
@@ -6086,7 +6117,7 @@
       </c>
       <c r="K29" s="27" t="n"/>
     </row>
-    <row r="30" ht="33" customHeight="1" s="87">
+    <row r="30" ht="33" customHeight="1" s="96">
       <c r="A30" s="24" t="n"/>
       <c r="B30" s="25" t="inlineStr">
         <is>
@@ -6135,7 +6166,7 @@
       </c>
       <c r="K30" s="27" t="n"/>
     </row>
-    <row r="31" ht="19.5" customHeight="1" s="87">
+    <row r="31" ht="19.5" customHeight="1" s="96">
       <c r="A31" s="24" t="n"/>
       <c r="B31" s="25" t="inlineStr">
         <is>
@@ -6184,7 +6215,7 @@
       </c>
       <c r="K31" s="27" t="n"/>
     </row>
-    <row r="32" ht="34.5" customHeight="1" s="87">
+    <row r="32" ht="34.5" customHeight="1" s="96">
       <c r="A32" s="24" t="n"/>
       <c r="B32" s="25" t="inlineStr">
         <is>
@@ -6233,7 +6264,7 @@
       </c>
       <c r="K32" s="27" t="n"/>
     </row>
-    <row r="33" ht="21" customHeight="1" s="87">
+    <row r="33" ht="21" customHeight="1" s="96">
       <c r="A33" s="24" t="n"/>
       <c r="B33" s="25" t="inlineStr">
         <is>
@@ -6303,14 +6334,14 @@
       <c r="J34" s="28" t="n"/>
       <c r="K34" s="27" t="n"/>
     </row>
-    <row r="35" ht="12" customHeight="1" s="87">
-      <c r="A35" s="67" t="inlineStr">
+    <row r="35" ht="12" customHeight="1" s="96">
+      <c r="A35" s="72" t="inlineStr">
         <is>
           <t>Asignación de Horas de Presidente y Secretario de Academia</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="12" customHeight="1" s="87">
+    <row r="36" ht="12" customHeight="1" s="96">
       <c r="A36" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -6362,7 +6393,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="87">
+    <row r="37" ht="18.75" customHeight="1" s="96">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="25" t="inlineStr">
         <is>
@@ -6403,7 +6434,7 @@
       </c>
       <c r="K37" s="31" t="n"/>
     </row>
-    <row r="38" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="38" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A38" s="32" t="n"/>
       <c r="B38" s="33" t="n"/>
       <c r="C38" s="34" t="inlineStr">
@@ -6419,14 +6450,14 @@
       <c r="I38" s="26" t="n"/>
       <c r="J38" s="35" t="n"/>
     </row>
-    <row r="39" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="39" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A39" s="36" t="n"/>
-      <c r="B39" s="68" t="inlineStr">
+      <c r="B39" s="73" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="C39" s="69" t="n"/>
+      <c r="C39" s="74" t="n"/>
       <c r="D39" s="37" t="n">
         <v>40</v>
       </c>
@@ -6437,31 +6468,31 @@
       <c r="I39" s="38" t="n"/>
       <c r="J39" s="39" t="n"/>
     </row>
-    <row r="40" ht="12" customHeight="1" s="87" thickBot="1">
+    <row r="40" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A40" s="36" t="n"/>
       <c r="B40" s="40" t="n"/>
       <c r="C40" s="41" t="n"/>
       <c r="D40" s="38" t="n"/>
-      <c r="E40" s="70" t="inlineStr">
+      <c r="E40" s="75" t="inlineStr">
         <is>
           <t>FECHA DE APLICACIÓN</t>
         </is>
       </c>
-      <c r="G40" s="71" t="inlineStr">
-        <is>
-          <t>25/01/2025</t>
-        </is>
-      </c>
-      <c r="H40" s="69" t="n"/>
-      <c r="I40" s="69" t="n"/>
-      <c r="J40" s="72" t="n"/>
-    </row>
-    <row r="41" ht="12" customHeight="1" s="87" thickBot="1">
+      <c r="G40" s="76" t="inlineStr">
+        <is>
+          <t>28/01/2025</t>
+        </is>
+      </c>
+      <c r="H40" s="74" t="n"/>
+      <c r="I40" s="74" t="n"/>
+      <c r="J40" s="77" t="n"/>
+    </row>
+    <row r="41" ht="12" customHeight="1" s="96" thickBot="1">
       <c r="A41" s="36" t="n"/>
       <c r="B41" s="40" t="n"/>
       <c r="C41" s="41" t="n"/>
       <c r="D41" s="38" t="n"/>
-      <c r="E41" s="70" t="inlineStr">
+      <c r="E41" s="75" t="inlineStr">
         <is>
           <t>CONSECUTIVO</t>
         </is>
@@ -6475,7 +6506,7 @@
       <c r="I41" s="38" t="n"/>
       <c r="J41" s="39" t="n"/>
     </row>
-    <row r="42" ht="9.75" customFormat="1" customHeight="1" s="58">
+    <row r="42" ht="9.75" customFormat="1" customHeight="1" s="61">
       <c r="C42" s="44" t="n"/>
       <c r="D42" s="44" t="n"/>
       <c r="E42" s="44" t="n"/>
@@ -6486,72 +6517,80 @@
       <c r="J42" s="44" t="n"/>
       <c r="K42" s="45" t="n"/>
     </row>
-    <row r="43" customFormat="1" s="58">
-      <c r="A43" s="73" t="n"/>
-      <c r="B43" s="56" t="n"/>
-      <c r="C43" s="74" t="inlineStr">
+    <row r="43" customFormat="1" s="61">
+      <c r="A43" s="78" t="inlineStr">
+        <is>
+          <t>JEFA DE DIVISIÓN DE ING. INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B43" s="59" t="n"/>
+      <c r="C43" s="79" t="inlineStr">
         <is>
           <t>REVISO</t>
         </is>
       </c>
-      <c r="D43" s="55" t="n"/>
-      <c r="E43" s="55" t="n"/>
-      <c r="F43" s="56" t="n"/>
-      <c r="G43" s="75" t="inlineStr">
+      <c r="D43" s="58" t="n"/>
+      <c r="E43" s="58" t="n"/>
+      <c r="F43" s="59" t="n"/>
+      <c r="G43" s="80" t="inlineStr">
         <is>
           <t>FIRMA DE CONFORMIDAD</t>
         </is>
       </c>
-      <c r="H43" s="76" t="n"/>
-      <c r="I43" s="76" t="n"/>
-      <c r="J43" s="64" t="n"/>
+      <c r="H43" s="81" t="n"/>
+      <c r="I43" s="81" t="n"/>
+      <c r="J43" s="82" t="n"/>
       <c r="K43" s="45" t="n"/>
     </row>
-    <row r="44" ht="16.5" customFormat="1" customHeight="1" s="58">
+    <row r="44" ht="16.5" customFormat="1" customHeight="1" s="61">
       <c r="A44" s="46" t="n"/>
       <c r="B44" s="47" t="n"/>
       <c r="C44" s="48" t="n"/>
       <c r="D44" s="48" t="n"/>
       <c r="E44" s="48" t="n"/>
       <c r="F44" s="49" t="n"/>
-      <c r="G44" s="54" t="inlineStr">
+      <c r="G44" s="57" t="inlineStr">
         <is>
           <t xml:space="preserve">AVILA GARCÍA LORENZO </t>
         </is>
       </c>
-      <c r="H44" s="55" t="n"/>
-      <c r="I44" s="55" t="n"/>
-      <c r="J44" s="56" t="n"/>
+      <c r="H44" s="58" t="n"/>
+      <c r="I44" s="58" t="n"/>
+      <c r="J44" s="59" t="n"/>
       <c r="K44" s="45" t="n"/>
     </row>
-    <row r="45" ht="12" customFormat="1" customHeight="1" s="58">
+    <row r="45" ht="12" customFormat="1" customHeight="1" s="61">
       <c r="A45" s="0" t="n"/>
       <c r="B45" s="0" t="n"/>
-      <c r="C45" s="63" t="inlineStr">
+      <c r="C45" s="66" t="inlineStr">
         <is>
           <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ
 ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
         </is>
       </c>
-      <c r="F45" s="59" t="n"/>
-      <c r="G45" s="57" t="n"/>
-      <c r="J45" s="59" t="n"/>
+      <c r="F45" s="62" t="n"/>
+      <c r="G45" s="60" t="n"/>
+      <c r="J45" s="62" t="n"/>
       <c r="K45" s="45" t="n"/>
     </row>
-    <row r="46" ht="37.5" customFormat="1" customHeight="1" s="58">
-      <c r="A46" s="86" t="n"/>
-      <c r="B46" s="62" t="n"/>
-      <c r="C46" s="60" t="n"/>
-      <c r="D46" s="61" t="n"/>
-      <c r="E46" s="61" t="n"/>
-      <c r="F46" s="62" t="n"/>
-      <c r="G46" s="60" t="n"/>
-      <c r="H46" s="61" t="n"/>
-      <c r="I46" s="61" t="n"/>
-      <c r="J46" s="62" t="n"/>
+    <row r="46" ht="37.5" customFormat="1" customHeight="1" s="61">
+      <c r="A46" s="67" t="inlineStr">
+        <is>
+          <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
+        </is>
+      </c>
+      <c r="B46" s="65" t="n"/>
+      <c r="C46" s="63" t="n"/>
+      <c r="D46" s="64" t="n"/>
+      <c r="E46" s="64" t="n"/>
+      <c r="F46" s="65" t="n"/>
+      <c r="G46" s="63" t="n"/>
+      <c r="H46" s="64" t="n"/>
+      <c r="I46" s="64" t="n"/>
+      <c r="J46" s="65" t="n"/>
       <c r="K46" s="45" t="n"/>
     </row>
-    <row r="47" ht="1.35" customHeight="1" s="87">
+    <row r="47" ht="1.35" customHeight="1" s="96">
       <c r="A47" s="50" t="n"/>
       <c r="B47" s="50" t="n"/>
       <c r="C47" s="50" t="n"/>
@@ -6565,23 +6604,23 @@
       <c r="P47" s="51" t="n"/>
       <c r="Q47" s="51" t="n"/>
     </row>
-    <row r="48" ht="12.75" customHeight="1" s="87">
-      <c r="A48" s="65" t="n"/>
-      <c r="C48" s="66" t="n"/>
-      <c r="G48" s="66" t="n"/>
+    <row r="48" ht="12.75" customHeight="1" s="96">
+      <c r="A48" s="68" t="n"/>
+      <c r="C48" s="93" t="n"/>
+      <c r="G48" s="93" t="n"/>
       <c r="K48" s="3" t="n"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1" s="87">
+    <row r="49" ht="12.75" customHeight="1" s="96">
       <c r="K49" s="3" t="n"/>
     </row>
-    <row r="50" ht="12.75" customHeight="1" s="87">
+    <row r="50" ht="12.75" customHeight="1" s="96">
       <c r="K50" s="3" t="n"/>
     </row>
-    <row r="51" ht="17.25" customHeight="1" s="87">
-      <c r="A51" s="52" t="n"/>
+    <row r="51" ht="17.25" customHeight="1" s="96">
+      <c r="A51" s="92" t="n"/>
       <c r="K51" s="3" t="n"/>
     </row>
-    <row r="52" ht="30" customHeight="1" s="87"/>
+    <row r="52" ht="30" customHeight="1" s="96"/>
     <row r="57">
       <c r="K57" s="3" t="n"/>
     </row>
@@ -6594,9 +6633,9 @@
     <mergeCell ref="A51:J52"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C45:F46"/>
     <mergeCell ref="A48:B50"/>
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="C45:F46"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="B39:C39"/>
@@ -6616,8 +6655,8 @@
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C43:F43"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C43:F43"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="H9:J9"/>
   </mergeCells>

</xml_diff>

<commit_message>
Implementacion de tabla para administrativos
</commit_message>
<xml_diff>
--- a/temp_reporte.xlsx
+++ b/temp_reporte.xlsx
@@ -226,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -464,13 +464,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="106">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -606,14 +617,38 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -621,13 +656,38 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -639,60 +699,36 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1163,22 +1199,22 @@
   </sheetPr>
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:J59"/>
+    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A36" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col width="11.140625" customWidth="1" style="57" min="1" max="1"/>
-    <col width="19.42578125" customWidth="1" style="57" min="2" max="2"/>
-    <col width="7.85546875" customWidth="1" style="57" min="3" max="3"/>
-    <col width="5.85546875" customWidth="1" style="57" min="4" max="4"/>
-    <col width="13.140625" customWidth="1" style="57" min="5" max="5"/>
-    <col width="13.7109375" customWidth="1" style="57" min="6" max="6"/>
-    <col width="12.5703125" customWidth="1" style="57" min="7" max="7"/>
-    <col width="12.42578125" customWidth="1" style="57" min="8" max="8"/>
-    <col width="12" customWidth="1" style="57" min="9" max="9"/>
-    <col width="9.7109375" customWidth="1" style="57" min="10" max="10"/>
+    <col width="11.140625" customWidth="1" style="100" min="1" max="1"/>
+    <col width="19.42578125" customWidth="1" style="100" min="2" max="2"/>
+    <col width="7.85546875" customWidth="1" style="100" min="3" max="3"/>
+    <col width="5.85546875" customWidth="1" style="100" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" style="100" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" style="100" min="6" max="6"/>
+    <col width="12.5703125" customWidth="1" style="100" min="7" max="7"/>
+    <col width="12.42578125" customWidth="1" style="100" min="8" max="8"/>
+    <col width="12" customWidth="1" style="100" min="9" max="9"/>
+    <col width="9.7109375" customWidth="1" style="100" min="10" max="10"/>
     <col width="12.140625" customWidth="1" style="2" min="11" max="11"/>
     <col width="11.42578125" customWidth="1" style="3" min="12" max="15"/>
     <col width="25.42578125" customWidth="1" style="3" min="16" max="16"/>
@@ -1187,56 +1223,56 @@
     <col width="11.42578125" customWidth="1" style="3" min="20" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" s="94">
-      <c r="A1" s="55" t="n"/>
-    </row>
-    <row r="2" ht="12" customHeight="1" s="94"/>
-    <row r="3" ht="32.25" customHeight="1" s="94"/>
-    <row r="4" ht="12" customHeight="1" s="94">
-      <c r="A4" s="56" t="inlineStr">
-        <is>
-          <t>“2024. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
+    <row r="1" ht="12" customHeight="1" s="101">
+      <c r="A1" s="84" t="n"/>
+    </row>
+    <row r="2" ht="12" customHeight="1" s="101"/>
+    <row r="3" ht="32.25" customHeight="1" s="101"/>
+    <row r="4" ht="12" customHeight="1" s="101">
+      <c r="A4" s="85" t="inlineStr">
+        <is>
+          <t>“2025. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="58" t="inlineStr">
+      <c r="A5" s="86" t="inlineStr">
         <is>
           <t>Asignación Académica</t>
         </is>
       </c>
-      <c r="B5" s="59" t="n"/>
-      <c r="C5" s="59" t="n"/>
-      <c r="D5" s="59" t="n"/>
-      <c r="E5" s="59" t="n"/>
-      <c r="F5" s="59" t="n"/>
-      <c r="G5" s="59" t="n"/>
-      <c r="H5" s="59" t="n"/>
-      <c r="I5" s="59" t="n"/>
-      <c r="J5" s="60" t="n"/>
-    </row>
-    <row r="6" ht="12" customHeight="1" s="94">
-      <c r="A6" s="61" t="inlineStr">
+      <c r="B5" s="73" t="n"/>
+      <c r="C5" s="73" t="n"/>
+      <c r="D5" s="73" t="n"/>
+      <c r="E5" s="73" t="n"/>
+      <c r="F5" s="73" t="n"/>
+      <c r="G5" s="73" t="n"/>
+      <c r="H5" s="73" t="n"/>
+      <c r="I5" s="73" t="n"/>
+      <c r="J5" s="74" t="n"/>
+    </row>
+    <row r="6" ht="12" customHeight="1" s="101">
+      <c r="A6" s="75" t="inlineStr">
         <is>
           <t>NOMBRE:</t>
         </is>
       </c>
-      <c r="B6" s="62" t="n"/>
-      <c r="C6" s="62" t="n"/>
-      <c r="D6" s="63" t="n"/>
-      <c r="E6" s="61" t="inlineStr">
+      <c r="B6" s="59" t="n"/>
+      <c r="C6" s="59" t="n"/>
+      <c r="D6" s="60" t="n"/>
+      <c r="E6" s="75" t="inlineStr">
         <is>
           <t>PROFESION:</t>
         </is>
       </c>
-      <c r="F6" s="62" t="n"/>
-      <c r="G6" s="62" t="n"/>
-      <c r="H6" s="62" t="n"/>
-      <c r="I6" s="62" t="n"/>
-      <c r="J6" s="63" t="n"/>
-    </row>
-    <row r="7" ht="12" customHeight="1" s="94">
-      <c r="A7" s="64" t="inlineStr">
+      <c r="F6" s="59" t="n"/>
+      <c r="G6" s="59" t="n"/>
+      <c r="H6" s="59" t="n"/>
+      <c r="I6" s="59" t="n"/>
+      <c r="J6" s="60" t="n"/>
+    </row>
+    <row r="7" ht="12" customHeight="1" s="101">
+      <c r="A7" s="87" t="inlineStr">
         <is>
           <t>AGUILAR GUGGEMBUHL JARUMI</t>
         </is>
@@ -1244,7 +1280,7 @@
       <c r="B7" s="65" t="n"/>
       <c r="C7" s="65" t="n"/>
       <c r="D7" s="66" t="n"/>
-      <c r="E7" s="67" t="inlineStr">
+      <c r="E7" s="88" t="inlineStr">
         <is>
           <t>LIC. VETERINARIA Y ZOOTECNIA/M. EN C. AGROPECUARIAS/ DR. BIOTECNOLOGÍA</t>
         </is>
@@ -1255,32 +1291,32 @@
       <c r="I7" s="65" t="n"/>
       <c r="J7" s="66" t="n"/>
     </row>
-    <row r="8" ht="12" customHeight="1" s="94">
-      <c r="A8" s="61" t="inlineStr">
+    <row r="8" ht="12" customHeight="1" s="101">
+      <c r="A8" s="75" t="inlineStr">
         <is>
           <t>ADSCRIPCIÓN:</t>
         </is>
       </c>
-      <c r="B8" s="62" t="n"/>
-      <c r="C8" s="62" t="n"/>
-      <c r="D8" s="63" t="n"/>
-      <c r="E8" s="61" t="inlineStr">
+      <c r="B8" s="59" t="n"/>
+      <c r="C8" s="59" t="n"/>
+      <c r="D8" s="60" t="n"/>
+      <c r="E8" s="75" t="inlineStr">
         <is>
           <t>INGRESO AL TECNOLÓGICO</t>
         </is>
       </c>
-      <c r="F8" s="62" t="n"/>
-      <c r="G8" s="63" t="n"/>
-      <c r="H8" s="61" t="inlineStr">
+      <c r="F8" s="59" t="n"/>
+      <c r="G8" s="60" t="n"/>
+      <c r="H8" s="75" t="inlineStr">
         <is>
           <t>TIEMPO INDETERMINADO</t>
         </is>
       </c>
-      <c r="I8" s="62" t="n"/>
-      <c r="J8" s="63" t="n"/>
-    </row>
-    <row r="9" ht="12" customHeight="1" s="94">
-      <c r="A9" s="67" t="inlineStr">
+      <c r="I8" s="59" t="n"/>
+      <c r="J8" s="60" t="n"/>
+    </row>
+    <row r="9" ht="12" customHeight="1" s="101">
+      <c r="A9" s="88" t="inlineStr">
         <is>
           <t>PROFESOR DE ASIGNATURA DE ING. INDUSTRIAL</t>
         </is>
@@ -1288,14 +1324,14 @@
       <c r="B9" s="65" t="n"/>
       <c r="C9" s="65" t="n"/>
       <c r="D9" s="66" t="n"/>
-      <c r="E9" s="67" t="inlineStr">
+      <c r="E9" s="88" t="inlineStr">
         <is>
           <t>01 DE SEPTIEMBRE 2014</t>
         </is>
       </c>
       <c r="F9" s="65" t="n"/>
       <c r="G9" s="66" t="n"/>
-      <c r="H9" s="67" t="inlineStr">
+      <c r="H9" s="88" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1303,32 +1339,32 @@
       <c r="I9" s="65" t="n"/>
       <c r="J9" s="66" t="n"/>
     </row>
-    <row r="10" ht="12" customHeight="1" s="94">
-      <c r="A10" s="61" t="inlineStr">
+    <row r="10" ht="12" customHeight="1" s="101">
+      <c r="A10" s="75" t="inlineStr">
         <is>
           <t>PERIODO:</t>
         </is>
       </c>
-      <c r="B10" s="62" t="n"/>
-      <c r="C10" s="62" t="n"/>
-      <c r="D10" s="63" t="n"/>
-      <c r="E10" s="73" t="inlineStr">
+      <c r="B10" s="59" t="n"/>
+      <c r="C10" s="59" t="n"/>
+      <c r="D10" s="60" t="n"/>
+      <c r="E10" s="76" t="inlineStr">
         <is>
           <t>HORAS TIPO</t>
         </is>
       </c>
-      <c r="F10" s="59" t="n"/>
-      <c r="G10" s="59" t="n"/>
-      <c r="H10" s="60" t="n"/>
-      <c r="I10" s="73" t="inlineStr">
+      <c r="F10" s="73" t="n"/>
+      <c r="G10" s="73" t="n"/>
+      <c r="H10" s="74" t="n"/>
+      <c r="I10" s="76" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="J10" s="60" t="n"/>
-    </row>
-    <row r="11" ht="12" customHeight="1" s="94">
-      <c r="A11" s="74" t="inlineStr">
+      <c r="J10" s="74" t="n"/>
+    </row>
+    <row r="11" ht="12" customHeight="1" s="101">
+      <c r="A11" s="77" t="inlineStr">
         <is>
           <t>2024-1 (MARZO-AGOSTO 2024)</t>
         </is>
@@ -1336,7 +1372,7 @@
       <c r="B11" s="65" t="n"/>
       <c r="C11" s="65" t="n"/>
       <c r="D11" s="65" t="n"/>
-      <c r="E11" s="73" t="inlineStr">
+      <c r="E11" s="76" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -1362,7 +1398,7 @@
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
-    <row r="12" ht="5.1" customHeight="1" s="94">
+    <row r="12" ht="5.1" customHeight="1" s="101">
       <c r="A12" s="8" t="n"/>
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="8" t="n"/>
@@ -1374,23 +1410,23 @@
       <c r="I12" s="8" t="n"/>
       <c r="J12" s="8" t="n"/>
     </row>
-    <row r="13" ht="12" customHeight="1" s="94">
-      <c r="A13" s="73" t="inlineStr">
+    <row r="13" ht="12" customHeight="1" s="101">
+      <c r="A13" s="76" t="inlineStr">
         <is>
           <t>Asignación de Horas Frente a Grupo</t>
         </is>
       </c>
-      <c r="B13" s="59" t="n"/>
-      <c r="C13" s="59" t="n"/>
-      <c r="D13" s="59" t="n"/>
-      <c r="E13" s="59" t="n"/>
-      <c r="F13" s="59" t="n"/>
-      <c r="G13" s="59" t="n"/>
-      <c r="H13" s="59" t="n"/>
-      <c r="I13" s="59" t="n"/>
-      <c r="J13" s="60" t="n"/>
-    </row>
-    <row r="14" ht="12" customHeight="1" s="94">
+      <c r="B13" s="73" t="n"/>
+      <c r="C13" s="73" t="n"/>
+      <c r="D13" s="73" t="n"/>
+      <c r="E13" s="73" t="n"/>
+      <c r="F13" s="73" t="n"/>
+      <c r="G13" s="73" t="n"/>
+      <c r="H13" s="73" t="n"/>
+      <c r="I13" s="73" t="n"/>
+      <c r="J13" s="74" t="n"/>
+    </row>
+    <row r="14" ht="12" customHeight="1" s="101">
       <c r="A14" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -1494,9 +1530,9 @@
         </is>
       </c>
       <c r="K15" s="15" t="n"/>
-      <c r="N15" s="95" t="n"/>
-    </row>
-    <row r="16" ht="21.75" customHeight="1" s="94">
+      <c r="N15" s="102" t="n"/>
+    </row>
+    <row r="16" ht="21.75" customHeight="1" s="101">
       <c r="A16" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -1548,9 +1584,9 @@
         </is>
       </c>
       <c r="K16" s="17" t="n"/>
-      <c r="N16" s="95" t="n"/>
-    </row>
-    <row r="17" ht="21.75" customHeight="1" s="94">
+      <c r="N16" s="102" t="n"/>
+    </row>
+    <row r="17" ht="21.75" customHeight="1" s="101">
       <c r="A17" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
@@ -1644,7 +1680,7 @@
       </c>
       <c r="K18" s="17" t="n"/>
     </row>
-    <row r="19" ht="20.25" customHeight="1" s="94">
+    <row r="19" ht="20.25" customHeight="1" s="101">
       <c r="A19" s="10" t="n"/>
       <c r="B19" s="11" t="inlineStr"/>
       <c r="C19" s="12" t="inlineStr">
@@ -1685,7 +1721,7 @@
       </c>
       <c r="K19" s="17" t="n"/>
     </row>
-    <row r="20" ht="19.5" customHeight="1" s="94">
+    <row r="20" ht="19.5" customHeight="1" s="101">
       <c r="A20" s="10" t="n"/>
       <c r="B20" s="11" t="inlineStr"/>
       <c r="C20" s="12" t="inlineStr">
@@ -1726,7 +1762,7 @@
       </c>
       <c r="K20" s="17" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="94">
+    <row r="21" ht="18" customHeight="1" s="101">
       <c r="A21" s="10" t="n"/>
       <c r="B21" s="11" t="inlineStr"/>
       <c r="C21" s="12" t="inlineStr">
@@ -1767,7 +1803,7 @@
       </c>
       <c r="K21" s="17" t="n"/>
     </row>
-    <row r="22" ht="18" customHeight="1" s="94">
+    <row r="22" ht="18" customHeight="1" s="101">
       <c r="A22" s="10" t="n"/>
       <c r="B22" s="11" t="inlineStr"/>
       <c r="C22" s="12" t="inlineStr">
@@ -1829,14 +1865,14 @@
       <c r="J23" s="23" t="n"/>
       <c r="K23" s="17" t="n"/>
     </row>
-    <row r="24" ht="12" customHeight="1" s="94">
-      <c r="A24" s="75" t="inlineStr">
+    <row r="24" ht="12" customHeight="1" s="101">
+      <c r="A24" s="78" t="inlineStr">
         <is>
           <t>Asignación de Horas de Descarga para otras Actividades</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="12" customHeight="1" s="94">
+    <row r="25" ht="12" customHeight="1" s="101">
       <c r="A25" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -1888,7 +1924,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="24.75" customHeight="1" s="94">
+    <row r="26" ht="24.75" customHeight="1" s="101">
       <c r="A26" s="24" t="n"/>
       <c r="B26" s="25" t="inlineStr">
         <is>
@@ -1937,7 +1973,7 @@
       </c>
       <c r="K26" s="27" t="n"/>
     </row>
-    <row r="27" ht="28.5" customHeight="1" s="94">
+    <row r="27" ht="28.5" customHeight="1" s="101">
       <c r="A27" s="24" t="n"/>
       <c r="B27" s="25" t="inlineStr">
         <is>
@@ -1986,7 +2022,7 @@
       </c>
       <c r="K27" s="27" t="n"/>
     </row>
-    <row r="28" ht="26.25" customHeight="1" s="94">
+    <row r="28" ht="26.25" customHeight="1" s="101">
       <c r="A28" s="24" t="n"/>
       <c r="B28" s="25" t="inlineStr">
         <is>
@@ -2035,7 +2071,7 @@
       </c>
       <c r="K28" s="27" t="n"/>
     </row>
-    <row r="29" ht="30" customHeight="1" s="94">
+    <row r="29" ht="30" customHeight="1" s="101">
       <c r="A29" s="24" t="n"/>
       <c r="B29" s="25" t="inlineStr">
         <is>
@@ -2084,7 +2120,7 @@
       </c>
       <c r="K29" s="27" t="n"/>
     </row>
-    <row r="30" ht="33" customHeight="1" s="94">
+    <row r="30" ht="33" customHeight="1" s="101">
       <c r="A30" s="24" t="n"/>
       <c r="B30" s="25" t="inlineStr">
         <is>
@@ -2133,7 +2169,7 @@
       </c>
       <c r="K30" s="27" t="n"/>
     </row>
-    <row r="31" ht="19.5" customHeight="1" s="94">
+    <row r="31" ht="19.5" customHeight="1" s="101">
       <c r="A31" s="24" t="n"/>
       <c r="B31" s="25" t="inlineStr"/>
       <c r="C31" s="26" t="inlineStr"/>
@@ -2170,7 +2206,7 @@
       </c>
       <c r="K31" s="27" t="n"/>
     </row>
-    <row r="32" ht="34.5" customHeight="1" s="94">
+    <row r="32" ht="34.5" customHeight="1" s="101">
       <c r="A32" s="24" t="n"/>
       <c r="B32" s="25" t="inlineStr"/>
       <c r="C32" s="26" t="inlineStr"/>
@@ -2207,7 +2243,7 @@
       </c>
       <c r="K32" s="27" t="n"/>
     </row>
-    <row r="33" ht="21" customHeight="1" s="94">
+    <row r="33" ht="21" customHeight="1" s="101">
       <c r="A33" s="24" t="n"/>
       <c r="B33" s="25" t="inlineStr"/>
       <c r="C33" s="26" t="inlineStr"/>
@@ -2265,14 +2301,14 @@
       <c r="J34" s="28" t="n"/>
       <c r="K34" s="27" t="n"/>
     </row>
-    <row r="35" ht="12" customHeight="1" s="94">
-      <c r="A35" s="75" t="inlineStr">
+    <row r="35" ht="12" customHeight="1" s="101">
+      <c r="A35" s="78" t="inlineStr">
         <is>
           <t>Asignación de Horas de Presidente y Secretario de Academia</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="12" customHeight="1" s="94">
+    <row r="36" ht="12" customHeight="1" s="101">
       <c r="A36" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -2324,7 +2360,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="94">
+    <row r="37" ht="18.75" customHeight="1" s="101">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="25" t="inlineStr">
         <is>
@@ -2365,7 +2401,7 @@
       </c>
       <c r="K37" s="31" t="n"/>
     </row>
-    <row r="38" ht="12" customHeight="1" s="94" thickBot="1">
+    <row r="38" ht="12" customHeight="1" s="101" thickBot="1">
       <c r="A38" s="32" t="n"/>
       <c r="B38" s="33" t="n"/>
       <c r="C38" s="34" t="inlineStr">
@@ -2381,14 +2417,14 @@
       <c r="I38" s="26" t="n"/>
       <c r="J38" s="35" t="n"/>
     </row>
-    <row r="39" ht="12" customHeight="1" s="94" thickBot="1">
+    <row r="39" ht="12" customHeight="1" s="101" thickBot="1">
       <c r="A39" s="36" t="n"/>
-      <c r="B39" s="76" t="inlineStr">
+      <c r="B39" s="79" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="C39" s="77" t="n"/>
+      <c r="C39" s="80" t="n"/>
       <c r="D39" s="37" t="n">
         <v>40</v>
       </c>
@@ -2399,31 +2435,31 @@
       <c r="I39" s="38" t="n"/>
       <c r="J39" s="39" t="n"/>
     </row>
-    <row r="40" ht="12" customHeight="1" s="94" thickBot="1">
+    <row r="40" ht="12" customHeight="1" s="101" thickBot="1">
       <c r="A40" s="36" t="n"/>
       <c r="B40" s="40" t="n"/>
       <c r="C40" s="41" t="n"/>
       <c r="D40" s="38" t="n"/>
-      <c r="E40" s="78" t="inlineStr">
+      <c r="E40" s="81" t="inlineStr">
         <is>
           <t>FECHA DE APLICACIÓN</t>
         </is>
       </c>
-      <c r="G40" s="79" t="inlineStr">
-        <is>
-          <t>29/01/2025</t>
-        </is>
-      </c>
-      <c r="H40" s="77" t="n"/>
-      <c r="I40" s="77" t="n"/>
-      <c r="J40" s="80" t="n"/>
-    </row>
-    <row r="41" ht="12" customHeight="1" s="94" thickBot="1">
+      <c r="G40" s="82" t="inlineStr">
+        <is>
+          <t>30/01/2025</t>
+        </is>
+      </c>
+      <c r="H40" s="80" t="n"/>
+      <c r="I40" s="80" t="n"/>
+      <c r="J40" s="83" t="n"/>
+    </row>
+    <row r="41" ht="12" customHeight="1" s="101" thickBot="1">
       <c r="A41" s="36" t="n"/>
       <c r="B41" s="40" t="n"/>
       <c r="C41" s="41" t="n"/>
       <c r="D41" s="38" t="n"/>
-      <c r="E41" s="78" t="inlineStr">
+      <c r="E41" s="81" t="inlineStr">
         <is>
           <t>CONSECUTIVO</t>
         </is>
@@ -2437,7 +2473,7 @@
       <c r="I41" s="38" t="n"/>
       <c r="J41" s="39" t="n"/>
     </row>
-    <row r="42" ht="9.75" customFormat="1" customHeight="1" s="86">
+    <row r="42" ht="9.75" customFormat="1" customHeight="1" s="62">
       <c r="C42" s="44" t="n"/>
       <c r="D42" s="44" t="n"/>
       <c r="E42" s="44" t="n"/>
@@ -2448,80 +2484,83 @@
       <c r="J42" s="44" t="n"/>
       <c r="K42" s="45" t="n"/>
     </row>
-    <row r="43" customFormat="1" s="86">
-      <c r="A43" s="70" t="inlineStr">
+    <row r="43" customFormat="1" s="62">
+      <c r="A43" s="91" t="inlineStr">
         <is>
           <t>JEFA DE DIVISIÓN DE ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B43" s="63" t="n"/>
-      <c r="C43" s="71" t="inlineStr">
+      <c r="B43" s="60" t="n"/>
+      <c r="C43" s="92" t="inlineStr">
         <is>
           <t>REVISO</t>
         </is>
       </c>
-      <c r="D43" s="62" t="n"/>
-      <c r="E43" s="62" t="n"/>
-      <c r="F43" s="63" t="n"/>
+      <c r="D43" s="59" t="n"/>
+      <c r="E43" s="59" t="n"/>
+      <c r="F43" s="60" t="n"/>
       <c r="G43" s="72" t="inlineStr">
         <is>
           <t>FIRMA DE CONFORMIDAD</t>
         </is>
       </c>
-      <c r="H43" s="59" t="n"/>
-      <c r="I43" s="59" t="n"/>
-      <c r="J43" s="60" t="n"/>
+      <c r="H43" s="73" t="n"/>
+      <c r="I43" s="73" t="n"/>
+      <c r="J43" s="74" t="n"/>
       <c r="K43" s="45" t="n"/>
     </row>
-    <row r="44" ht="16.5" customFormat="1" customHeight="1" s="86">
+    <row r="44" ht="16.5" customFormat="1" customHeight="1" s="62">
       <c r="A44" s="46" t="n"/>
       <c r="B44" s="47" t="n"/>
       <c r="C44" s="48" t="n"/>
       <c r="D44" s="48" t="n"/>
       <c r="E44" s="48" t="n"/>
       <c r="F44" s="49" t="n"/>
-      <c r="G44" s="84" t="inlineStr">
+      <c r="G44" s="58" t="inlineStr">
         <is>
           <t>AGUILAR GUGGEMBUHL JARUMI</t>
         </is>
       </c>
-      <c r="H44" s="62" t="n"/>
-      <c r="I44" s="62" t="n"/>
-      <c r="J44" s="63" t="n"/>
+      <c r="H44" s="59" t="n"/>
+      <c r="I44" s="59" t="n"/>
+      <c r="J44" s="60" t="n"/>
       <c r="K44" s="45" t="n"/>
     </row>
-    <row r="45" ht="12" customFormat="1" customHeight="1" s="86">
+    <row r="45" ht="38.25" customFormat="1" customHeight="1" s="62">
       <c r="A45" s="54" t="n"/>
       <c r="B45" s="0" t="n"/>
-      <c r="C45" s="89" t="inlineStr">
-        <is>
-          <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ
-ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
-        </is>
-      </c>
-      <c r="F45" s="87" t="n"/>
-      <c r="G45" s="85" t="n"/>
-      <c r="J45" s="87" t="n"/>
+      <c r="C45" s="103" t="inlineStr">
+        <is>
+          <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ</t>
+        </is>
+      </c>
+      <c r="F45" s="63" t="n"/>
+      <c r="G45" s="61" t="n"/>
+      <c r="J45" s="63" t="n"/>
       <c r="K45" s="45" t="n"/>
     </row>
-    <row r="46" ht="37.5" customFormat="1" customHeight="1" s="86">
-      <c r="A46" s="90" t="inlineStr">
+    <row r="46" ht="10.5" customFormat="1" customHeight="1" s="62">
+      <c r="A46" s="67" t="inlineStr">
         <is>
           <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
         </is>
       </c>
       <c r="B46" s="66" t="n"/>
-      <c r="C46" s="88" t="n"/>
+      <c r="C46" s="104" t="inlineStr">
+        <is>
+          <t>ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
+        </is>
+      </c>
       <c r="D46" s="65" t="n"/>
       <c r="E46" s="65" t="n"/>
       <c r="F46" s="66" t="n"/>
-      <c r="G46" s="88" t="n"/>
+      <c r="G46" s="64" t="n"/>
       <c r="H46" s="65" t="n"/>
       <c r="I46" s="65" t="n"/>
       <c r="J46" s="66" t="n"/>
       <c r="K46" s="45" t="n"/>
     </row>
-    <row r="47" ht="1.35" customHeight="1" s="94">
+    <row r="47" ht="1.35" customHeight="1" s="101">
       <c r="A47" s="50" t="n"/>
       <c r="B47" s="50" t="n"/>
       <c r="C47" s="50" t="n"/>
@@ -2535,27 +2574,27 @@
       <c r="P47" s="51" t="n"/>
       <c r="Q47" s="51" t="n"/>
     </row>
-    <row r="48" ht="9" customHeight="1" s="94">
-      <c r="A48" s="91" t="n"/>
-      <c r="C48" s="96" t="inlineStr">
+    <row r="48" ht="9" customHeight="1" s="101">
+      <c r="A48" s="68" t="n"/>
+      <c r="C48" s="105" t="inlineStr">
         <is>
           <t>Vo. Bo</t>
         </is>
       </c>
-      <c r="G48" s="92" t="n"/>
+      <c r="G48" s="99" t="n"/>
       <c r="K48" s="3" t="n"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1" s="94">
+    <row r="49" ht="12.75" customHeight="1" s="101">
       <c r="K49" s="3" t="n"/>
     </row>
-    <row r="50" ht="13.5" customHeight="1" s="94">
+    <row r="50" ht="13.5" customHeight="1" s="101">
       <c r="C50" s="65" t="n"/>
       <c r="D50" s="65" t="n"/>
       <c r="E50" s="65" t="n"/>
       <c r="F50" s="65" t="n"/>
       <c r="K50" s="3" t="n"/>
     </row>
-    <row r="51" ht="1.5" customHeight="1" s="94">
+    <row r="51" ht="1.5" customHeight="1" s="101">
       <c r="A51" s="52" t="n"/>
       <c r="B51" s="53" t="n"/>
       <c r="C51" s="53" t="n"/>
@@ -2568,10 +2607,10 @@
       <c r="J51" s="53" t="n"/>
       <c r="K51" s="3" t="n"/>
     </row>
-    <row r="52" ht="10.5" customHeight="1" s="94">
+    <row r="52" ht="10.5" customHeight="1" s="101">
       <c r="A52" s="53" t="n"/>
       <c r="B52" s="53" t="n"/>
-      <c r="C52" s="81" t="inlineStr">
+      <c r="C52" s="55" t="inlineStr">
         <is>
           <t>DRA C.CLAUDIA PÉREZ MARTÍNEZ</t>
         </is>
@@ -2582,14 +2621,14 @@
       <c r="J52" s="53" t="n"/>
     </row>
     <row r="53">
-      <c r="C53" s="81" t="inlineStr">
+      <c r="C53" s="55" t="inlineStr">
         <is>
           <t>DIRECTORA GENERAL</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="55" t="n"/>
+      <c r="A54" s="84" t="n"/>
     </row>
     <row r="55"/>
     <row r="56"/>
@@ -2599,7 +2638,7 @@
     <row r="58"/>
     <row r="59"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="37">
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A8:D8"/>
@@ -2609,32 +2648,33 @@
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="A48:B50"/>
     <mergeCell ref="A10:D10"/>
-    <mergeCell ref="C45:F46"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="G40:J40"/>
     <mergeCell ref="C53:F53"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="A9:D9"/>
     <mergeCell ref="G44:J46"/>
     <mergeCell ref="G43:J43"/>
     <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A54:J59"/>
+    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A54:J59"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="E7:J7"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A1:J3"/>
-    <mergeCell ref="A6:D6"/>
     <mergeCell ref="G48:J50"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C43:F43"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C43:F43"/>
     <mergeCell ref="E8:G8"/>
+    <mergeCell ref="C46:F46"/>
     <mergeCell ref="H9:J9"/>
   </mergeCells>
   <conditionalFormatting sqref="E15:J22">

</xml_diff>

<commit_message>
Organización por carreras: Movido a carpeta industrial
</commit_message>
<xml_diff>
--- a/temp_reporte.xlsx
+++ b/temp_reporte.xlsx
@@ -87,7 +87,7 @@
     <numFmt numFmtId="164" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <name val="Arial"/>
       <sz val="10"/>
@@ -180,14 +180,8 @@
       <family val="2"/>
       <sz val="7"/>
     </font>
-    <font>
-      <name val="Helvetica"/>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="7"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -224,12 +218,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00757171"/>
-        <bgColor rgb="00757171"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -486,7 +474,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="118">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -764,9 +752,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
@@ -1285,7 +1270,7 @@
     <row r="4" ht="12" customHeight="1" s="108">
       <c r="A4" s="54" t="inlineStr">
         <is>
-          <t>“2025. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
+          <t>“2024. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
         </is>
       </c>
     </row>
@@ -1328,7 +1313,7 @@
     <row r="7" ht="12" customHeight="1" s="108">
       <c r="A7" s="62" t="inlineStr">
         <is>
-          <t>AGUILAR ORTEGA RICARDO</t>
+          <t>IVAN</t>
         </is>
       </c>
       <c r="B7" s="69" t="n"/>
@@ -1336,7 +1321,7 @@
       <c r="D7" s="70" t="n"/>
       <c r="E7" s="65" t="inlineStr">
         <is>
-          <t>ING. CIVIL / M. EN RELACIONES INTERINSTITUCIONALES</t>
+          <t>ING. INDUSTRIAL</t>
         </is>
       </c>
       <c r="F7" s="69" t="n"/>
@@ -1387,7 +1372,7 @@
       <c r="G9" s="70" t="n"/>
       <c r="H9" s="68" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="I9" s="69" t="n"/>
@@ -1420,7 +1405,7 @@
     <row r="11" ht="12" customHeight="1" s="108">
       <c r="A11" s="75" t="inlineStr">
         <is>
-          <t>2024-1 (MARZO-AGOSTO 2024)</t>
+          <t>MARZO-AGOSTO 2024</t>
         </is>
       </c>
       <c r="B11" s="69" t="n"/>
@@ -1432,7 +1417,7 @@
         </is>
       </c>
       <c r="F11" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11" s="6" t="inlineStr">
         <is>
@@ -1440,7 +1425,7 @@
         </is>
       </c>
       <c r="H11" s="5" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I11" s="7" t="inlineStr">
         <is>
@@ -1448,7 +1433,7 @@
         </is>
       </c>
       <c r="J11" s="5" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
@@ -1540,42 +1525,42 @@
       </c>
       <c r="B15" s="11" t="inlineStr">
         <is>
-          <t>DIBUJO INDUSTRIAL (INN-1008)</t>
+          <t>QUÍMICA (INC-1025)</t>
         </is>
       </c>
       <c r="C15" s="12" t="inlineStr">
         <is>
-          <t>1101</t>
+          <t>1181</t>
         </is>
       </c>
       <c r="D15" s="12" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E15" s="109" t="inlineStr">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E15" s="14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">07:00 09:00 H.T. </t>
+        </is>
+      </c>
+      <c r="F15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H15" s="14" t="inlineStr">
         <is>
           <t>07:00 09:00</t>
         </is>
       </c>
-      <c r="F15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G15" s="109" t="inlineStr">
-        <is>
-          <t>07:00 09:00</t>
-        </is>
-      </c>
-      <c r="H15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I15" s="109" t="inlineStr">
-        <is>
-          <t>07:00 09:00</t>
+      <c r="I15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="J15" s="14" t="inlineStr">
@@ -1584,32 +1569,20 @@
         </is>
       </c>
       <c r="K15" s="15" t="n"/>
-      <c r="N15" s="110" t="n"/>
+      <c r="N15" s="109" t="n"/>
     </row>
     <row r="16" ht="21.75" customHeight="1" s="108">
-      <c r="A16" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B16" s="11" t="inlineStr">
-        <is>
-          <t>PROPIEDADES DE LOS MATERIALES (INC-1024)</t>
-        </is>
-      </c>
+      <c r="A16" s="10" t="n"/>
+      <c r="B16" s="11" t="inlineStr"/>
       <c r="C16" s="12" t="inlineStr">
         <is>
-          <t>1201</t>
-        </is>
-      </c>
-      <c r="D16" s="12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E16" s="109" t="inlineStr">
-        <is>
-          <t>09:00 11:00</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D16" s="12" t="inlineStr"/>
+      <c r="E16" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="F16" s="14" t="inlineStr">
@@ -1617,9 +1590,9 @@
           <t> </t>
         </is>
       </c>
-      <c r="G16" s="109" t="inlineStr">
-        <is>
-          <t>09:00 11:00</t>
+      <c r="G16" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="H16" s="14" t="inlineStr">
@@ -1638,32 +1611,20 @@
         </is>
       </c>
       <c r="K16" s="17" t="n"/>
-      <c r="N16" s="110" t="n"/>
+      <c r="N16" s="109" t="n"/>
     </row>
     <row r="17" ht="21.75" customHeight="1" s="108">
-      <c r="A17" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B17" s="11" t="inlineStr">
-        <is>
-          <t>PROPIEDADES DE LOS MATERIALES (INC-1024)</t>
-        </is>
-      </c>
+      <c r="A17" s="10" t="n"/>
+      <c r="B17" s="11" t="inlineStr"/>
       <c r="C17" s="12" t="inlineStr">
         <is>
-          <t>1251</t>
-        </is>
-      </c>
-      <c r="D17" s="12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E17" s="109" t="inlineStr">
-        <is>
-          <t>14:00 16:00</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D17" s="12" t="inlineStr"/>
+      <c r="E17" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="F17" s="14" t="inlineStr">
@@ -1671,9 +1632,9 @@
           <t> </t>
         </is>
       </c>
-      <c r="G17" s="109" t="inlineStr">
-        <is>
-          <t>14:00 16:00</t>
+      <c r="G17" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="H17" s="14" t="inlineStr">
@@ -1694,26 +1655,14 @@
       <c r="K17" s="17" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B18" s="11" t="inlineStr">
-        <is>
-          <t>PROPIEDADES DE LOS MATERIALES (INC-1024)</t>
-        </is>
-      </c>
+      <c r="A18" s="10" t="n"/>
+      <c r="B18" s="11" t="inlineStr"/>
       <c r="C18" s="12" t="inlineStr">
         <is>
-          <t>1281</t>
-        </is>
-      </c>
-      <c r="D18" s="12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D18" s="12" t="inlineStr"/>
       <c r="E18" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -1724,9 +1673,9 @@
           <t> </t>
         </is>
       </c>
-      <c r="G18" s="109" t="inlineStr">
-        <is>
-          <t>16:00 18:00</t>
+      <c r="G18" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="H18" s="14" t="inlineStr">
@@ -1734,9 +1683,9 @@
           <t> </t>
         </is>
       </c>
-      <c r="I18" s="109" t="inlineStr">
-        <is>
-          <t>09:00 11:00</t>
+      <c r="I18" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="J18" s="14" t="inlineStr">
@@ -1747,29 +1696,17 @@
       <c r="K18" s="17" t="n"/>
     </row>
     <row r="19" ht="20.25" customHeight="1" s="108">
-      <c r="A19" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B19" s="11" t="inlineStr">
-        <is>
-          <t>FÍSICA (INC-1013)</t>
-        </is>
-      </c>
+      <c r="A19" s="10" t="n"/>
+      <c r="B19" s="11" t="inlineStr"/>
       <c r="C19" s="12" t="inlineStr">
         <is>
-          <t>1481</t>
-        </is>
-      </c>
-      <c r="D19" s="12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E19" s="109" t="inlineStr">
-        <is>
-          <t>16:00 18:00</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D19" s="12" t="inlineStr"/>
+      <c r="E19" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="F19" s="14" t="inlineStr">
@@ -1777,9 +1714,9 @@
           <t> </t>
         </is>
       </c>
-      <c r="G19" s="109" t="inlineStr">
-        <is>
-          <t>11:00 13:00</t>
+      <c r="G19" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="H19" s="14" t="inlineStr">
@@ -1932,7 +1869,7 @@
       </c>
       <c r="D23" s="9" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E23" s="21" t="n"/>
@@ -2004,21 +1941,9 @@
     </row>
     <row r="26" ht="24.75" customHeight="1" s="108">
       <c r="A26" s="24" t="inlineStr"/>
-      <c r="B26" s="25" t="inlineStr">
-        <is>
-          <t>ASESORIA DE DIBUJO ASISTIDO POR COMPUTADORA</t>
-        </is>
-      </c>
-      <c r="C26" s="26" t="inlineStr">
-        <is>
-          <t>1101</t>
-        </is>
-      </c>
-      <c r="D26" s="26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B26" s="25" t="inlineStr"/>
+      <c r="C26" s="26" t="inlineStr"/>
+      <c r="D26" s="26" t="inlineStr"/>
       <c r="E26" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -2039,9 +1964,9 @@
           <t> </t>
         </is>
       </c>
-      <c r="I26" s="109" t="inlineStr">
-        <is>
-          <t>13:00 14:00</t>
+      <c r="I26" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="J26" s="14" t="inlineStr">
@@ -2053,21 +1978,9 @@
     </row>
     <row r="27" ht="28.5" customHeight="1" s="108">
       <c r="A27" s="24" t="inlineStr"/>
-      <c r="B27" s="25" t="inlineStr">
-        <is>
-          <t>ASESORIA DE CIENCIAS DE LA INGENIERÍA</t>
-        </is>
-      </c>
-      <c r="C27" s="26" t="inlineStr">
-        <is>
-          <t>1201/1251</t>
-        </is>
-      </c>
-      <c r="D27" s="26" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="B27" s="25" t="inlineStr"/>
+      <c r="C27" s="26" t="inlineStr"/>
+      <c r="D27" s="26" t="inlineStr"/>
       <c r="E27" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -2078,9 +1991,9 @@
           <t> </t>
         </is>
       </c>
-      <c r="G27" s="109" t="inlineStr">
-        <is>
-          <t>13:00 14:00</t>
+      <c r="G27" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="H27" s="14" t="inlineStr">
@@ -2088,9 +2001,9 @@
           <t> </t>
         </is>
       </c>
-      <c r="I27" s="109" t="inlineStr">
-        <is>
-          <t>12:00 13:00</t>
+      <c r="I27" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="J27" s="14" t="inlineStr">
@@ -2102,24 +2015,12 @@
     </row>
     <row r="28" ht="26.25" customHeight="1" s="108">
       <c r="A28" s="24" t="inlineStr"/>
-      <c r="B28" s="25" t="inlineStr">
-        <is>
-          <t>ACTIVIDAD COMPLEMENTARIA (PRESENCIAL)</t>
-        </is>
-      </c>
-      <c r="C28" s="26" t="inlineStr">
-        <is>
-          <t>NG</t>
-        </is>
-      </c>
-      <c r="D28" s="26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E28" s="109" t="inlineStr">
-        <is>
-          <t>13:00 14:00</t>
+      <c r="B28" s="25" t="inlineStr"/>
+      <c r="C28" s="26" t="inlineStr"/>
+      <c r="D28" s="26" t="inlineStr"/>
+      <c r="E28" s="14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
       <c r="F28" s="14" t="inlineStr">
@@ -2151,24 +2052,12 @@
     </row>
     <row r="29" ht="30" customHeight="1" s="108">
       <c r="A29" s="24" t="inlineStr"/>
-      <c r="B29" s="25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">COORDINACIÓN DE ACTIVIDAD COMPLEMENTARÍA </t>
-        </is>
-      </c>
-      <c r="C29" s="26" t="inlineStr">
-        <is>
-          <t>NG</t>
-        </is>
-      </c>
-      <c r="D29" s="26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B29" s="25" t="inlineStr"/>
+      <c r="C29" s="26" t="inlineStr"/>
+      <c r="D29" s="26" t="inlineStr"/>
       <c r="E29" s="14" t="inlineStr">
         <is>
-          <t>11:00 12:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="F29" s="14" t="inlineStr">
@@ -2200,21 +2089,9 @@
     </row>
     <row r="30" ht="33" customHeight="1" s="108">
       <c r="A30" s="24" t="inlineStr"/>
-      <c r="B30" s="25" t="inlineStr">
-        <is>
-          <t>FORTALECIMIENTO A LA CALIDAD EDUCATIVA (ESPECIALIDAD/CACEI)</t>
-        </is>
-      </c>
-      <c r="C30" s="26" t="inlineStr">
-        <is>
-          <t>NG</t>
-        </is>
-      </c>
-      <c r="D30" s="26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B30" s="25" t="inlineStr"/>
+      <c r="C30" s="26" t="inlineStr"/>
+      <c r="D30" s="26" t="inlineStr"/>
       <c r="E30" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -2237,7 +2114,7 @@
       </c>
       <c r="I30" s="14" t="inlineStr">
         <is>
-          <t>11:00 12:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="J30" s="14" t="inlineStr">
@@ -2368,7 +2245,7 @@
       </c>
       <c r="D34" s="9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E34" s="30" t="n"/>
@@ -2504,7 +2381,7 @@
       </c>
       <c r="C39" s="78" t="n"/>
       <c r="D39" s="37" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="E39" s="38" t="n"/>
       <c r="F39" s="38" t="n"/>
@@ -2525,7 +2402,7 @@
       </c>
       <c r="G40" s="80" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>06/02/2025</t>
         </is>
       </c>
       <c r="H40" s="78" t="n"/>
@@ -2588,15 +2465,15 @@
       <c r="K43" s="45" t="n"/>
     </row>
     <row r="44" ht="21.75" customFormat="1" customHeight="1" s="43">
-      <c r="A44" s="111" t="n"/>
-      <c r="B44" s="112" t="n"/>
+      <c r="A44" s="110" t="n"/>
+      <c r="B44" s="111" t="n"/>
       <c r="C44" s="52" t="n"/>
       <c r="D44" s="46" t="n"/>
       <c r="E44" s="46" t="n"/>
       <c r="F44" s="47" t="n"/>
       <c r="G44" s="85" t="inlineStr">
         <is>
-          <t>AGUILAR ORTEGA RICARDO</t>
+          <t>IVAN</t>
         </is>
       </c>
       <c r="H44" s="60" t="n"/>
@@ -2605,16 +2482,16 @@
       <c r="K44" s="45" t="n"/>
     </row>
     <row r="45" ht="27.75" customFormat="1" customHeight="1" s="43">
-      <c r="A45" s="113" t="n"/>
-      <c r="B45" s="112" t="n"/>
-      <c r="C45" s="114" t="inlineStr">
+      <c r="A45" s="112" t="n"/>
+      <c r="B45" s="111" t="n"/>
+      <c r="C45" s="113" t="inlineStr">
         <is>
           <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ</t>
         </is>
       </c>
-      <c r="F45" s="112" t="n"/>
-      <c r="G45" s="115" t="n"/>
-      <c r="J45" s="112" t="n"/>
+      <c r="F45" s="111" t="n"/>
+      <c r="G45" s="114" t="n"/>
+      <c r="J45" s="111" t="n"/>
       <c r="K45" s="45" t="n"/>
     </row>
     <row r="46" ht="12" customFormat="1" customHeight="1" s="43">
@@ -2624,7 +2501,7 @@
         </is>
       </c>
       <c r="B46" s="70" t="n"/>
-      <c r="C46" s="116" t="inlineStr">
+      <c r="C46" s="115" t="inlineStr">
         <is>
           <t>ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
         </is>
@@ -2632,7 +2509,7 @@
       <c r="D46" s="69" t="n"/>
       <c r="E46" s="69" t="n"/>
       <c r="F46" s="70" t="n"/>
-      <c r="G46" s="117" t="n"/>
+      <c r="G46" s="116" t="n"/>
       <c r="H46" s="69" t="n"/>
       <c r="I46" s="69" t="n"/>
       <c r="J46" s="70" t="n"/>
@@ -2654,7 +2531,7 @@
     </row>
     <row r="48" ht="9" customHeight="1" s="108">
       <c r="A48" s="93" t="n"/>
-      <c r="C48" s="118" t="inlineStr">
+      <c r="C48" s="117" t="inlineStr">
         <is>
           <t>Vo. Bo</t>
         </is>

</xml_diff>

<commit_message>
Implementacion de reporteador para todas las carreras y reporteador automatico
</commit_message>
<xml_diff>
--- a/temp_reporte.xlsx
+++ b/temp_reporte.xlsx
@@ -498,7 +498,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -632,6 +632,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -704,6 +707,12 @@
     <xf numFmtId="164" fontId="15" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,9 +744,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,11 +775,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -938,10 +941,10 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>53</row>
+      <row>55</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8248650" cy="1028700"/>
+    <ext cx="8248650" cy="628650"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -1266,22 +1269,22 @@
   </sheetPr>
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A42" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:B45"/>
+    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A44" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col width="11.140625" customWidth="1" style="68" min="1" max="1"/>
-    <col width="19.42578125" customWidth="1" style="68" min="2" max="2"/>
-    <col width="7.85546875" customWidth="1" style="68" min="3" max="3"/>
-    <col width="5.85546875" customWidth="1" style="68" min="4" max="4"/>
-    <col width="13.140625" customWidth="1" style="68" min="5" max="5"/>
-    <col width="13.7109375" customWidth="1" style="68" min="6" max="6"/>
-    <col width="12.5703125" customWidth="1" style="68" min="7" max="7"/>
-    <col width="12.42578125" customWidth="1" style="68" min="8" max="8"/>
-    <col width="12" customWidth="1" style="68" min="9" max="9"/>
-    <col width="9.7109375" customWidth="1" style="68" min="10" max="10"/>
+    <col width="11.140625" customWidth="1" style="69" min="1" max="1"/>
+    <col width="19.42578125" customWidth="1" style="69" min="2" max="2"/>
+    <col width="7.85546875" customWidth="1" style="69" min="3" max="3"/>
+    <col width="5.85546875" customWidth="1" style="69" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" style="69" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" style="69" min="6" max="6"/>
+    <col width="12.5703125" customWidth="1" style="69" min="7" max="7"/>
+    <col width="12.42578125" customWidth="1" style="69" min="8" max="8"/>
+    <col width="12" customWidth="1" style="69" min="9" max="9"/>
+    <col width="9.7109375" customWidth="1" style="69" min="10" max="10"/>
     <col width="12.140625" customWidth="1" style="2" min="11" max="11"/>
     <col width="11.42578125" customWidth="1" style="3" min="12" max="15"/>
     <col width="25.42578125" customWidth="1" style="3" min="16" max="16"/>
@@ -1290,156 +1293,156 @@
     <col width="11.42578125" customWidth="1" style="3" min="20" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" s="108">
-      <c r="A1" s="94" t="n"/>
-    </row>
-    <row r="2" ht="12" customHeight="1" s="108"/>
-    <row r="3" ht="32.25" customHeight="1" s="108"/>
-    <row r="4" ht="12" customHeight="1" s="108">
-      <c r="A4" s="95" t="inlineStr">
-        <is>
-          <t>“2024. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
+    <row r="1" ht="12" customHeight="1" s="109">
+      <c r="A1" s="53" t="n"/>
+    </row>
+    <row r="2" ht="12" customHeight="1" s="109"/>
+    <row r="3" ht="32.25" customHeight="1" s="109"/>
+    <row r="4" ht="12" customHeight="1" s="109">
+      <c r="A4" s="97" t="inlineStr">
+        <is>
+          <t>“2025. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="96" t="inlineStr">
+      <c r="A5" s="98" t="inlineStr">
         <is>
           <t>Asignación Académica</t>
         </is>
       </c>
-      <c r="B5" s="80" t="n"/>
-      <c r="C5" s="80" t="n"/>
-      <c r="D5" s="80" t="n"/>
-      <c r="E5" s="80" t="n"/>
-      <c r="F5" s="80" t="n"/>
-      <c r="G5" s="80" t="n"/>
-      <c r="H5" s="80" t="n"/>
-      <c r="I5" s="80" t="n"/>
-      <c r="J5" s="81" t="n"/>
-    </row>
-    <row r="6" ht="12" customHeight="1" s="108">
-      <c r="A6" s="82" t="inlineStr">
+      <c r="B5" s="83" t="n"/>
+      <c r="C5" s="83" t="n"/>
+      <c r="D5" s="83" t="n"/>
+      <c r="E5" s="83" t="n"/>
+      <c r="F5" s="83" t="n"/>
+      <c r="G5" s="83" t="n"/>
+      <c r="H5" s="83" t="n"/>
+      <c r="I5" s="83" t="n"/>
+      <c r="J5" s="84" t="n"/>
+    </row>
+    <row r="6" ht="12" customHeight="1" s="109">
+      <c r="A6" s="85" t="inlineStr">
         <is>
           <t>NOMBRE:</t>
         </is>
       </c>
-      <c r="B6" s="83" t="n"/>
-      <c r="C6" s="83" t="n"/>
-      <c r="D6" s="84" t="n"/>
-      <c r="E6" s="82" t="inlineStr">
+      <c r="B6" s="86" t="n"/>
+      <c r="C6" s="86" t="n"/>
+      <c r="D6" s="87" t="n"/>
+      <c r="E6" s="85" t="inlineStr">
         <is>
           <t>PROFESION:</t>
         </is>
       </c>
-      <c r="F6" s="83" t="n"/>
-      <c r="G6" s="83" t="n"/>
-      <c r="H6" s="83" t="n"/>
-      <c r="I6" s="83" t="n"/>
-      <c r="J6" s="84" t="n"/>
-    </row>
-    <row r="7" ht="12" customHeight="1" s="108">
-      <c r="A7" s="97" t="inlineStr">
+      <c r="F6" s="86" t="n"/>
+      <c r="G6" s="86" t="n"/>
+      <c r="H6" s="86" t="n"/>
+      <c r="I6" s="86" t="n"/>
+      <c r="J6" s="87" t="n"/>
+    </row>
+    <row r="7" ht="12" customHeight="1" s="109">
+      <c r="A7" s="99" t="inlineStr">
         <is>
           <t>IVAN</t>
         </is>
       </c>
-      <c r="B7" s="87" t="n"/>
-      <c r="C7" s="87" t="n"/>
-      <c r="D7" s="102" t="n"/>
-      <c r="E7" s="98" t="inlineStr">
+      <c r="B7" s="90" t="n"/>
+      <c r="C7" s="90" t="n"/>
+      <c r="D7" s="104" t="n"/>
+      <c r="E7" s="100" t="inlineStr">
         <is>
           <t>ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="F7" s="87" t="n"/>
-      <c r="G7" s="87" t="n"/>
-      <c r="H7" s="87" t="n"/>
-      <c r="I7" s="87" t="n"/>
-      <c r="J7" s="102" t="n"/>
-    </row>
-    <row r="8" ht="12" customHeight="1" s="108">
-      <c r="A8" s="82" t="inlineStr">
+      <c r="F7" s="90" t="n"/>
+      <c r="G7" s="90" t="n"/>
+      <c r="H7" s="90" t="n"/>
+      <c r="I7" s="90" t="n"/>
+      <c r="J7" s="104" t="n"/>
+    </row>
+    <row r="8" ht="12" customHeight="1" s="109">
+      <c r="A8" s="85" t="inlineStr">
         <is>
           <t>ADSCRIPCIÓN:</t>
         </is>
       </c>
-      <c r="B8" s="83" t="n"/>
-      <c r="C8" s="83" t="n"/>
-      <c r="D8" s="84" t="n"/>
-      <c r="E8" s="82" t="inlineStr">
+      <c r="B8" s="86" t="n"/>
+      <c r="C8" s="86" t="n"/>
+      <c r="D8" s="87" t="n"/>
+      <c r="E8" s="85" t="inlineStr">
         <is>
           <t>INGRESO AL TECNOLÓGICO</t>
         </is>
       </c>
-      <c r="F8" s="83" t="n"/>
-      <c r="G8" s="84" t="n"/>
-      <c r="H8" s="82" t="inlineStr">
+      <c r="F8" s="86" t="n"/>
+      <c r="G8" s="87" t="n"/>
+      <c r="H8" s="85" t="inlineStr">
         <is>
           <t>TIEMPO INDETERMINADO</t>
         </is>
       </c>
-      <c r="I8" s="83" t="n"/>
-      <c r="J8" s="84" t="n"/>
-    </row>
-    <row r="9" ht="12" customHeight="1" s="108">
-      <c r="A9" s="98" t="inlineStr">
+      <c r="I8" s="86" t="n"/>
+      <c r="J8" s="87" t="n"/>
+    </row>
+    <row r="9" ht="12" customHeight="1" s="109">
+      <c r="A9" s="100" t="inlineStr">
         <is>
           <t>PROFESOR DE ASIGNATURA DE ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B9" s="87" t="n"/>
-      <c r="C9" s="87" t="n"/>
-      <c r="D9" s="102" t="n"/>
-      <c r="E9" s="101" t="inlineStr">
+      <c r="B9" s="90" t="n"/>
+      <c r="C9" s="90" t="n"/>
+      <c r="D9" s="104" t="n"/>
+      <c r="E9" s="103" t="inlineStr">
         <is>
           <t>01 DE MARZO DE 2011</t>
         </is>
       </c>
-      <c r="F9" s="87" t="n"/>
-      <c r="G9" s="102" t="n"/>
-      <c r="H9" s="101" t="inlineStr">
+      <c r="F9" s="90" t="n"/>
+      <c r="G9" s="104" t="n"/>
+      <c r="H9" s="103" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
       </c>
-      <c r="I9" s="87" t="n"/>
-      <c r="J9" s="102" t="n"/>
-    </row>
-    <row r="10" ht="12" customHeight="1" s="108">
-      <c r="A10" s="82" t="inlineStr">
+      <c r="I9" s="90" t="n"/>
+      <c r="J9" s="104" t="n"/>
+    </row>
+    <row r="10" ht="12" customHeight="1" s="109">
+      <c r="A10" s="85" t="inlineStr">
         <is>
           <t>PERIODO:</t>
         </is>
       </c>
-      <c r="B10" s="83" t="n"/>
-      <c r="C10" s="83" t="n"/>
-      <c r="D10" s="84" t="n"/>
-      <c r="E10" s="85" t="inlineStr">
+      <c r="B10" s="86" t="n"/>
+      <c r="C10" s="86" t="n"/>
+      <c r="D10" s="87" t="n"/>
+      <c r="E10" s="88" t="inlineStr">
         <is>
           <t>HORAS TIPO</t>
         </is>
       </c>
-      <c r="F10" s="80" t="n"/>
-      <c r="G10" s="80" t="n"/>
-      <c r="H10" s="81" t="n"/>
-      <c r="I10" s="85" t="inlineStr">
+      <c r="F10" s="83" t="n"/>
+      <c r="G10" s="83" t="n"/>
+      <c r="H10" s="84" t="n"/>
+      <c r="I10" s="88" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="J10" s="81" t="n"/>
-    </row>
-    <row r="11" ht="12" customHeight="1" s="108">
-      <c r="A11" s="86" t="inlineStr">
+      <c r="J10" s="84" t="n"/>
+    </row>
+    <row r="11" ht="12" customHeight="1" s="109">
+      <c r="A11" s="89" t="inlineStr">
         <is>
           <t>MARZO-AGOSTO 2024</t>
         </is>
       </c>
-      <c r="B11" s="87" t="n"/>
-      <c r="C11" s="87" t="n"/>
-      <c r="D11" s="87" t="n"/>
-      <c r="E11" s="85" t="inlineStr">
+      <c r="B11" s="90" t="n"/>
+      <c r="C11" s="90" t="n"/>
+      <c r="D11" s="90" t="n"/>
+      <c r="E11" s="88" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -1465,7 +1468,7 @@
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
-    <row r="12" ht="5.1" customHeight="1" s="108">
+    <row r="12" ht="5.1" customHeight="1" s="109">
       <c r="A12" s="8" t="n"/>
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="8" t="n"/>
@@ -1477,23 +1480,23 @@
       <c r="I12" s="8" t="n"/>
       <c r="J12" s="8" t="n"/>
     </row>
-    <row r="13" ht="12" customHeight="1" s="108">
-      <c r="A13" s="85" t="inlineStr">
+    <row r="13" ht="12" customHeight="1" s="109">
+      <c r="A13" s="88" t="inlineStr">
         <is>
           <t>Asignación de Horas Frente a Grupo</t>
         </is>
       </c>
-      <c r="B13" s="80" t="n"/>
-      <c r="C13" s="80" t="n"/>
-      <c r="D13" s="80" t="n"/>
-      <c r="E13" s="80" t="n"/>
-      <c r="F13" s="80" t="n"/>
-      <c r="G13" s="80" t="n"/>
-      <c r="H13" s="80" t="n"/>
-      <c r="I13" s="80" t="n"/>
-      <c r="J13" s="81" t="n"/>
-    </row>
-    <row r="14" ht="12" customHeight="1" s="108">
+      <c r="B13" s="83" t="n"/>
+      <c r="C13" s="83" t="n"/>
+      <c r="D13" s="83" t="n"/>
+      <c r="E13" s="83" t="n"/>
+      <c r="F13" s="83" t="n"/>
+      <c r="G13" s="83" t="n"/>
+      <c r="H13" s="83" t="n"/>
+      <c r="I13" s="83" t="n"/>
+      <c r="J13" s="84" t="n"/>
+    </row>
+    <row r="14" ht="12" customHeight="1" s="109">
       <c r="A14" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -1566,7 +1569,7 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E15" s="109" t="inlineStr">
+      <c r="E15" s="110" t="inlineStr">
         <is>
           <t xml:space="preserve">07:00 09:00 H.T. </t>
         </is>
@@ -1597,9 +1600,9 @@
         </is>
       </c>
       <c r="K15" s="15" t="n"/>
-      <c r="N15" s="110" t="n"/>
-    </row>
-    <row r="16" ht="21.75" customHeight="1" s="108">
+      <c r="N15" s="111" t="n"/>
+    </row>
+    <row r="16" ht="21.75" customHeight="1" s="109">
       <c r="A16" s="10" t="n"/>
       <c r="B16" s="11" t="inlineStr"/>
       <c r="C16" s="12" t="inlineStr">
@@ -1639,9 +1642,9 @@
         </is>
       </c>
       <c r="K16" s="17" t="n"/>
-      <c r="N16" s="110" t="n"/>
-    </row>
-    <row r="17" ht="21.75" customHeight="1" s="108">
+      <c r="N16" s="111" t="n"/>
+    </row>
+    <row r="17" ht="21.75" customHeight="1" s="109">
       <c r="A17" s="10" t="n"/>
       <c r="B17" s="11" t="inlineStr"/>
       <c r="C17" s="12" t="inlineStr">
@@ -1723,7 +1726,7 @@
       </c>
       <c r="K18" s="17" t="n"/>
     </row>
-    <row r="19" ht="20.25" customHeight="1" s="108">
+    <row r="19" ht="20.25" customHeight="1" s="109">
       <c r="A19" s="10" t="n"/>
       <c r="B19" s="11" t="inlineStr"/>
       <c r="C19" s="12" t="inlineStr">
@@ -1764,7 +1767,7 @@
       </c>
       <c r="K19" s="17" t="n"/>
     </row>
-    <row r="20" ht="19.5" customHeight="1" s="108">
+    <row r="20" ht="19.5" customHeight="1" s="109">
       <c r="A20" s="10" t="n"/>
       <c r="B20" s="11" t="inlineStr"/>
       <c r="C20" s="12" t="inlineStr">
@@ -1805,7 +1808,7 @@
       </c>
       <c r="K20" s="17" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="108">
+    <row r="21" ht="18" customHeight="1" s="109">
       <c r="A21" s="10" t="n"/>
       <c r="B21" s="11" t="inlineStr"/>
       <c r="C21" s="12" t="inlineStr">
@@ -1846,7 +1849,7 @@
       </c>
       <c r="K21" s="17" t="n"/>
     </row>
-    <row r="22" ht="18" customHeight="1" s="108">
+    <row r="22" ht="18" customHeight="1" s="109">
       <c r="A22" s="10" t="n"/>
       <c r="B22" s="11" t="inlineStr"/>
       <c r="C22" s="12" t="inlineStr">
@@ -1908,14 +1911,14 @@
       <c r="J23" s="23" t="n"/>
       <c r="K23" s="17" t="n"/>
     </row>
-    <row r="24" ht="12" customHeight="1" s="108">
-      <c r="A24" s="88" t="inlineStr">
+    <row r="24" ht="12" customHeight="1" s="109">
+      <c r="A24" s="91" t="inlineStr">
         <is>
           <t>Asignación de Horas de Descarga para otras Actividades</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="12" customHeight="1" s="108">
+    <row r="25" ht="12" customHeight="1" s="109">
       <c r="A25" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -1967,7 +1970,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="24.75" customHeight="1" s="108">
+    <row r="26" ht="24.75" customHeight="1" s="109">
       <c r="A26" s="24" t="inlineStr">
         <is>
           <t>SISTEMAS COMPUTACIONALES</t>
@@ -2020,7 +2023,7 @@
       </c>
       <c r="K26" s="27" t="n"/>
     </row>
-    <row r="27" ht="28.5" customHeight="1" s="108">
+    <row r="27" ht="28.5" customHeight="1" s="109">
       <c r="A27" s="24" t="inlineStr">
         <is>
           <t>SISTEMAS COMPUTACIONALES</t>
@@ -2073,7 +2076,7 @@
       </c>
       <c r="K27" s="27" t="n"/>
     </row>
-    <row r="28" ht="26.25" customHeight="1" s="108">
+    <row r="28" ht="26.25" customHeight="1" s="109">
       <c r="A28" s="24" t="inlineStr"/>
       <c r="B28" s="25" t="inlineStr"/>
       <c r="C28" s="26" t="inlineStr"/>
@@ -2110,7 +2113,7 @@
       </c>
       <c r="K28" s="27" t="n"/>
     </row>
-    <row r="29" ht="30" customHeight="1" s="108">
+    <row r="29" ht="30" customHeight="1" s="109">
       <c r="A29" s="24" t="inlineStr"/>
       <c r="B29" s="25" t="inlineStr"/>
       <c r="C29" s="26" t="inlineStr"/>
@@ -2147,7 +2150,7 @@
       </c>
       <c r="K29" s="27" t="n"/>
     </row>
-    <row r="30" ht="33" customHeight="1" s="108">
+    <row r="30" ht="33" customHeight="1" s="109">
       <c r="A30" s="24" t="inlineStr"/>
       <c r="B30" s="25" t="inlineStr"/>
       <c r="C30" s="26" t="inlineStr"/>
@@ -2184,7 +2187,7 @@
       </c>
       <c r="K30" s="27" t="n"/>
     </row>
-    <row r="31" ht="19.5" customHeight="1" s="108">
+    <row r="31" ht="19.5" customHeight="1" s="109">
       <c r="A31" s="24" t="inlineStr"/>
       <c r="B31" s="25" t="inlineStr"/>
       <c r="C31" s="26" t="inlineStr"/>
@@ -2221,7 +2224,7 @@
       </c>
       <c r="K31" s="27" t="n"/>
     </row>
-    <row r="32" ht="34.5" customHeight="1" s="108">
+    <row r="32" ht="34.5" customHeight="1" s="109">
       <c r="A32" s="24" t="inlineStr"/>
       <c r="B32" s="25" t="inlineStr"/>
       <c r="C32" s="26" t="inlineStr"/>
@@ -2258,7 +2261,7 @@
       </c>
       <c r="K32" s="27" t="n"/>
     </row>
-    <row r="33" ht="21" customHeight="1" s="108">
+    <row r="33" ht="21" customHeight="1" s="109">
       <c r="A33" s="24" t="inlineStr"/>
       <c r="B33" s="25" t="inlineStr"/>
       <c r="C33" s="26" t="inlineStr"/>
@@ -2316,14 +2319,14 @@
       <c r="J34" s="28" t="n"/>
       <c r="K34" s="27" t="n"/>
     </row>
-    <row r="35" ht="12" customHeight="1" s="108">
-      <c r="A35" s="88" t="inlineStr">
+    <row r="35" ht="12" customHeight="1" s="109">
+      <c r="A35" s="91" t="inlineStr">
         <is>
           <t>Asignación de Horas de Presidente y Secretario de Academia</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="12" customHeight="1" s="108">
+    <row r="36" ht="12" customHeight="1" s="109">
       <c r="A36" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -2375,7 +2378,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="108">
+    <row r="37" ht="18.75" customHeight="1" s="109">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="25" t="inlineStr">
         <is>
@@ -2416,7 +2419,7 @@
       </c>
       <c r="K37" s="31" t="n"/>
     </row>
-    <row r="38" ht="12" customHeight="1" s="108" thickBot="1">
+    <row r="38" ht="12" customHeight="1" s="109" thickBot="1">
       <c r="A38" s="32" t="n"/>
       <c r="B38" s="33" t="n"/>
       <c r="C38" s="34" t="inlineStr">
@@ -2432,14 +2435,14 @@
       <c r="I38" s="26" t="n"/>
       <c r="J38" s="35" t="n"/>
     </row>
-    <row r="39" ht="12" customHeight="1" s="108" thickBot="1">
+    <row r="39" ht="12" customHeight="1" s="109" thickBot="1">
       <c r="A39" s="36" t="n"/>
-      <c r="B39" s="89" t="inlineStr">
+      <c r="B39" s="92" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="C39" s="90" t="n"/>
+      <c r="C39" s="93" t="n"/>
       <c r="D39" s="37" t="n">
         <v>8</v>
       </c>
@@ -2450,31 +2453,31 @@
       <c r="I39" s="38" t="n"/>
       <c r="J39" s="39" t="n"/>
     </row>
-    <row r="40" ht="12" customHeight="1" s="108" thickBot="1">
+    <row r="40" ht="12" customHeight="1" s="109" thickBot="1">
       <c r="A40" s="36" t="n"/>
       <c r="B40" s="40" t="n"/>
       <c r="C40" s="41" t="n"/>
       <c r="D40" s="38" t="n"/>
-      <c r="E40" s="91" t="inlineStr">
+      <c r="E40" s="94" t="inlineStr">
         <is>
           <t>FECHA DE APLICACIÓN</t>
         </is>
       </c>
-      <c r="G40" s="92" t="inlineStr">
-        <is>
-          <t>07/02/2025</t>
-        </is>
-      </c>
-      <c r="H40" s="90" t="n"/>
-      <c r="I40" s="90" t="n"/>
-      <c r="J40" s="93" t="n"/>
-    </row>
-    <row r="41" ht="12" customHeight="1" s="108" thickBot="1">
+      <c r="G40" s="95" t="inlineStr">
+        <is>
+          <t>20/02/2025</t>
+        </is>
+      </c>
+      <c r="H40" s="93" t="n"/>
+      <c r="I40" s="93" t="n"/>
+      <c r="J40" s="96" t="n"/>
+    </row>
+    <row r="41" ht="12" customHeight="1" s="109" thickBot="1">
       <c r="A41" s="36" t="n"/>
       <c r="B41" s="40" t="n"/>
       <c r="C41" s="41" t="n"/>
       <c r="D41" s="38" t="n"/>
-      <c r="E41" s="91" t="inlineStr">
+      <c r="E41" s="94" t="inlineStr">
         <is>
           <t>CONSECUTIVO</t>
         </is>
@@ -2500,90 +2503,90 @@
       <c r="K42" s="45" t="n"/>
     </row>
     <row r="43" ht="17.25" customFormat="1" customHeight="1" s="43">
-      <c r="A43" s="103" t="inlineStr">
+      <c r="A43" s="105" t="inlineStr">
         <is>
           <t>JEFA DE DIVISIÓN DE ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B43" s="84" t="n"/>
-      <c r="C43" s="105" t="inlineStr">
+      <c r="B43" s="87" t="n"/>
+      <c r="C43" s="107" t="inlineStr">
         <is>
           <t>REVISO</t>
         </is>
       </c>
-      <c r="D43" s="83" t="n"/>
-      <c r="E43" s="83" t="n"/>
-      <c r="F43" s="84" t="n"/>
-      <c r="G43" s="79" t="inlineStr">
+      <c r="D43" s="86" t="n"/>
+      <c r="E43" s="86" t="n"/>
+      <c r="F43" s="87" t="n"/>
+      <c r="G43" s="82" t="inlineStr">
         <is>
           <t>FIRMA DE CONFORMIDAD</t>
         </is>
       </c>
-      <c r="H43" s="80" t="n"/>
-      <c r="I43" s="80" t="n"/>
-      <c r="J43" s="81" t="n"/>
+      <c r="H43" s="83" t="n"/>
+      <c r="I43" s="83" t="n"/>
+      <c r="J43" s="84" t="n"/>
       <c r="K43" s="45" t="n"/>
     </row>
     <row r="44" ht="21.75" customFormat="1" customHeight="1" s="43">
-      <c r="A44" s="111" t="inlineStr">
+      <c r="A44" s="112" t="inlineStr">
         <is>
           <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
         </is>
       </c>
-      <c r="B44" s="112" t="n"/>
+      <c r="B44" s="113" t="n"/>
       <c r="C44" s="52" t="n"/>
       <c r="D44" s="46" t="n"/>
       <c r="E44" s="46" t="n"/>
       <c r="F44" s="47" t="n"/>
-      <c r="G44" s="56" t="inlineStr">
+      <c r="G44" s="57" t="inlineStr">
         <is>
           <t>IVAN</t>
         </is>
       </c>
-      <c r="H44" s="83" t="n"/>
-      <c r="I44" s="83" t="n"/>
-      <c r="J44" s="84" t="n"/>
+      <c r="H44" s="86" t="n"/>
+      <c r="I44" s="86" t="n"/>
+      <c r="J44" s="87" t="n"/>
       <c r="K44" s="45" t="n"/>
     </row>
     <row r="45" ht="27.75" customFormat="1" customHeight="1" s="43">
-      <c r="A45" s="113" t="inlineStr">
-        <is>
-          <t>JEFE DE DIVISIÓN DE ING. SISTEMAS COMPUTACIONALES</t>
-        </is>
-      </c>
-      <c r="B45" s="114" t="n"/>
-      <c r="C45" s="115" t="inlineStr">
+      <c r="A45" s="114" t="inlineStr">
+        <is>
+          <t>JEFA DE DIVISIÓN DE ING. EN SISTEMAS COMPUTACIONALES</t>
+        </is>
+      </c>
+      <c r="B45" s="115" t="n"/>
+      <c r="C45" s="116" t="inlineStr">
         <is>
           <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ</t>
         </is>
       </c>
-      <c r="F45" s="114" t="n"/>
-      <c r="G45" s="116" t="n"/>
-      <c r="J45" s="114" t="n"/>
+      <c r="F45" s="115" t="n"/>
+      <c r="G45" s="117" t="n"/>
+      <c r="J45" s="115" t="n"/>
       <c r="K45" s="45" t="n"/>
     </row>
     <row r="46" ht="12" customFormat="1" customHeight="1" s="43">
-      <c r="A46" s="65" t="inlineStr">
-        <is>
-          <t>IVAN CASTELAN ESTRADA</t>
-        </is>
-      </c>
-      <c r="B46" s="102" t="n"/>
-      <c r="C46" s="117" t="inlineStr">
+      <c r="A46" s="66" t="inlineStr">
+        <is>
+          <t>DRA. EN C.C. FABIOLA ORQUÍDEA SANCHEZ HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="B46" s="104" t="n"/>
+      <c r="C46" s="118" t="inlineStr">
         <is>
           <t>ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
         </is>
       </c>
-      <c r="D46" s="87" t="n"/>
-      <c r="E46" s="87" t="n"/>
-      <c r="F46" s="102" t="n"/>
-      <c r="G46" s="118" t="n"/>
-      <c r="H46" s="87" t="n"/>
-      <c r="I46" s="87" t="n"/>
-      <c r="J46" s="102" t="n"/>
+      <c r="D46" s="90" t="n"/>
+      <c r="E46" s="90" t="n"/>
+      <c r="F46" s="104" t="n"/>
+      <c r="G46" s="119" t="n"/>
+      <c r="H46" s="90" t="n"/>
+      <c r="I46" s="90" t="n"/>
+      <c r="J46" s="104" t="n"/>
       <c r="K46" s="45" t="n"/>
     </row>
-    <row r="47" ht="1.35" customHeight="1" s="108">
+    <row r="47" ht="1.35" customHeight="1" s="109">
       <c r="A47" s="48" t="n"/>
       <c r="B47" s="48" t="n"/>
       <c r="C47" s="48" t="n"/>
@@ -2597,27 +2600,27 @@
       <c r="P47" s="49" t="n"/>
       <c r="Q47" s="49" t="n"/>
     </row>
-    <row r="48" ht="9" customHeight="1" s="108">
-      <c r="A48" s="67" t="n"/>
-      <c r="C48" s="119" t="inlineStr">
+    <row r="48" ht="9" customHeight="1" s="109">
+      <c r="A48" s="68" t="n"/>
+      <c r="C48" s="120" t="inlineStr">
         <is>
           <t>Vo. Bo</t>
         </is>
       </c>
-      <c r="G48" s="69" t="n"/>
+      <c r="G48" s="70" t="n"/>
       <c r="K48" s="3" t="n"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1" s="108">
+    <row r="49" ht="12.75" customHeight="1" s="109">
       <c r="K49" s="3" t="n"/>
     </row>
-    <row r="50" ht="13.5" customHeight="1" s="108">
-      <c r="C50" s="87" t="n"/>
-      <c r="D50" s="87" t="n"/>
-      <c r="E50" s="87" t="n"/>
-      <c r="F50" s="87" t="n"/>
+    <row r="50" ht="13.5" customHeight="1" s="109">
+      <c r="C50" s="90" t="n"/>
+      <c r="D50" s="90" t="n"/>
+      <c r="E50" s="90" t="n"/>
+      <c r="F50" s="90" t="n"/>
       <c r="K50" s="3" t="n"/>
     </row>
-    <row r="51" ht="1.5" customHeight="1" s="108">
+    <row r="51" ht="1.5" customHeight="1" s="109">
       <c r="A51" s="50" t="n"/>
       <c r="B51" s="51" t="n"/>
       <c r="C51" s="51" t="n"/>
@@ -2630,10 +2633,10 @@
       <c r="J51" s="51" t="n"/>
       <c r="K51" s="3" t="n"/>
     </row>
-    <row r="52" ht="10.5" customHeight="1" s="108">
+    <row r="52" ht="10.5" customHeight="1" s="109">
       <c r="A52" s="51" t="n"/>
       <c r="B52" s="51" t="n"/>
-      <c r="C52" s="53" t="inlineStr">
+      <c r="C52" s="54" t="inlineStr">
         <is>
           <t>DR. ERNESTO M. RIVAS RIVAS</t>
         </is>
@@ -2644,34 +2647,41 @@
       <c r="J52" s="51" t="n"/>
     </row>
     <row r="53">
-      <c r="C53" s="53" t="inlineStr">
+      <c r="C53" s="54" t="inlineStr">
         <is>
           <t>DIRECTOR GENERAL</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="94" t="n"/>
+      <c r="A54" s="108" t="inlineStr">
+        <is>
+          <t>Los temarios de las asignaturas para este semestre debe ser descargados de la siguiente URL con la especialidad de Lean Manufacturing en la Industria 4.0: http://tescha.edomex.gob.mx/plan-de-estudio</t>
+        </is>
+      </c>
     </row>
     <row r="55"/>
-    <row r="56"/>
+    <row r="56">
+      <c r="A56" s="53" t="n"/>
+    </row>
     <row r="57">
       <c r="K57" s="3" t="n"/>
     </row>
     <row r="58"/>
     <row r="59"/>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="40">
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="C48:F50"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A35:J35"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E9:G9"/>
     <mergeCell ref="A48:B50"/>
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A54:J55"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="B39:C39"/>
@@ -2681,14 +2691,14 @@
     <mergeCell ref="G44:J46"/>
     <mergeCell ref="G43:J43"/>
     <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A54:J59"/>
+    <mergeCell ref="A56:J59"/>
+    <mergeCell ref="A24:J24"/>
     <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A24:J24"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="C45:F45"/>
+    <mergeCell ref="A1:J3"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:J3"/>
     <mergeCell ref="G48:J50"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="A7:D7"/>

</xml_diff>

<commit_message>
Implementacion de diseños azul/amarillo version 1.0
</commit_message>
<xml_diff>
--- a/temp_reporte.xlsx
+++ b/temp_reporte.xlsx
@@ -87,7 +87,7 @@
     <numFmt numFmtId="164" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <name val="Arial"/>
       <sz val="10"/>
@@ -185,14 +185,8 @@
       <family val="2"/>
       <sz val="7"/>
     </font>
-    <font>
-      <name val="Helvetica"/>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="7"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -229,14 +223,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00757171"/>
-        <bgColor rgb="00757171"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="24">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -485,20 +473,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="119">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -779,18 +760,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1344,7 +1321,7 @@
     <row r="7" ht="12" customHeight="1" s="109">
       <c r="A7" s="99" t="inlineStr">
         <is>
-          <t>IVAN</t>
+          <t xml:space="preserve">GELOVER MANZO HUGO </t>
         </is>
       </c>
       <c r="B7" s="90" t="n"/>
@@ -1352,7 +1329,7 @@
       <c r="D7" s="104" t="n"/>
       <c r="E7" s="100" t="inlineStr">
         <is>
-          <t>ING. INDUSTRIAL</t>
+          <t>ING. ELECTROMECÁNICO</t>
         </is>
       </c>
       <c r="F7" s="90" t="n"/>
@@ -1396,14 +1373,14 @@
       <c r="D9" s="104" t="n"/>
       <c r="E9" s="103" t="inlineStr">
         <is>
-          <t>01 DE MARZO DE 2011</t>
+          <t>01 DE SEPTIEMBRE DE 2019</t>
         </is>
       </c>
       <c r="F9" s="90" t="n"/>
       <c r="G9" s="104" t="n"/>
       <c r="H9" s="103" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="I9" s="90" t="n"/>
@@ -1436,7 +1413,7 @@
     <row r="11" ht="12" customHeight="1" s="109">
       <c r="A11" s="89" t="inlineStr">
         <is>
-          <t>MARZO-AGOSTO 2024</t>
+          <t>2024-1 (MARZO-AGOSTO 2024)</t>
         </is>
       </c>
       <c r="B11" s="90" t="n"/>
@@ -1448,7 +1425,7 @@
         </is>
       </c>
       <c r="F11" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G11" s="6" t="inlineStr">
         <is>
@@ -1456,7 +1433,7 @@
         </is>
       </c>
       <c r="H11" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11" s="7" t="inlineStr">
         <is>
@@ -1464,7 +1441,7 @@
         </is>
       </c>
       <c r="J11" s="5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
@@ -1549,71 +1526,79 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="inlineStr">
+      <c r="A15" s="10" t="n"/>
+      <c r="B15" s="11" t="inlineStr">
+        <is>
+          <t>CÁLCULO INTEGRAL (ACF-0902)</t>
+        </is>
+      </c>
+      <c r="C15" s="12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D15" s="12" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E15" s="14" t="inlineStr">
+        <is>
+          <t>07:00 09:00</t>
+        </is>
+      </c>
+      <c r="F15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G15" s="14" t="inlineStr">
+        <is>
+          <t>07:00 09:00</t>
+        </is>
+      </c>
+      <c r="H15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I15" s="14" t="inlineStr">
+        <is>
+          <t>07:00 08:00</t>
+        </is>
+      </c>
+      <c r="J15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K15" s="15" t="n"/>
+      <c r="N15" s="110" t="n"/>
+    </row>
+    <row r="16" ht="21.75" customHeight="1" s="109">
+      <c r="A16" s="10" t="inlineStr">
         <is>
           <t>INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B15" s="11" t="inlineStr">
-        <is>
-          <t>QUÍMICA (INC-1025)</t>
-        </is>
-      </c>
-      <c r="C15" s="12" t="inlineStr">
-        <is>
-          <t>1181</t>
-        </is>
-      </c>
-      <c r="D15" s="12" t="inlineStr">
+      <c r="B16" s="11" t="inlineStr">
+        <is>
+          <t>PROCESOS DE FABRICACIÓN (INC-1023)</t>
+        </is>
+      </c>
+      <c r="C16" s="12" t="inlineStr">
+        <is>
+          <t>1401</t>
+        </is>
+      </c>
+      <c r="D16" s="12" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E15" s="110" t="inlineStr">
-        <is>
-          <t xml:space="preserve">07:00 09:00 H.T. </t>
-        </is>
-      </c>
-      <c r="F15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H15" s="14" t="inlineStr">
-        <is>
-          <t>07:00 09:00</t>
-        </is>
-      </c>
-      <c r="I15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K15" s="15" t="n"/>
-      <c r="N15" s="111" t="n"/>
-    </row>
-    <row r="16" ht="21.75" customHeight="1" s="109">
-      <c r="A16" s="10" t="n"/>
-      <c r="B16" s="11" t="inlineStr"/>
-      <c r="C16" s="12" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D16" s="12" t="inlineStr"/>
       <c r="E16" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>09:00 11:00</t>
         </is>
       </c>
       <c r="F16" s="14" t="inlineStr">
@@ -1623,7 +1608,7 @@
       </c>
       <c r="G16" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>09:00 11:00</t>
         </is>
       </c>
       <c r="H16" s="14" t="inlineStr">
@@ -1642,20 +1627,32 @@
         </is>
       </c>
       <c r="K16" s="17" t="n"/>
-      <c r="N16" s="111" t="n"/>
+      <c r="N16" s="110" t="n"/>
     </row>
     <row r="17" ht="21.75" customHeight="1" s="109">
-      <c r="A17" s="10" t="n"/>
-      <c r="B17" s="11" t="inlineStr"/>
+      <c r="A17" s="10" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B17" s="11" t="inlineStr">
+        <is>
+          <t>PROCESOS DE FABRICACIÓN (INC-1023)</t>
+        </is>
+      </c>
       <c r="C17" s="12" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D17" s="12" t="inlineStr"/>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="D17" s="12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="E17" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>15:00 17:00</t>
         </is>
       </c>
       <c r="F17" s="14" t="inlineStr">
@@ -1665,7 +1662,7 @@
       </c>
       <c r="G17" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>15:00 17:00</t>
         </is>
       </c>
       <c r="H17" s="14" t="inlineStr">
@@ -1686,17 +1683,29 @@
       <c r="K17" s="17" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="n"/>
-      <c r="B18" s="11" t="inlineStr"/>
+      <c r="A18" s="10" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B18" s="11" t="inlineStr">
+        <is>
+          <t>PROCESOS DE FABRICACIÓN (INC-1023)</t>
+        </is>
+      </c>
       <c r="C18" s="12" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D18" s="12" t="inlineStr"/>
+          <t>1481</t>
+        </is>
+      </c>
+      <c r="D18" s="12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E18" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>11:00 13:00</t>
         </is>
       </c>
       <c r="F18" s="14" t="inlineStr">
@@ -1727,17 +1736,29 @@
       <c r="K18" s="17" t="n"/>
     </row>
     <row r="19" ht="20.25" customHeight="1" s="109">
-      <c r="A19" s="10" t="n"/>
-      <c r="B19" s="11" t="inlineStr"/>
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B19" s="11" t="inlineStr">
+        <is>
+          <t>PROCESOS DE FABRICACIÓN (INC-1023)</t>
+        </is>
+      </c>
       <c r="C19" s="12" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D19" s="12" t="inlineStr"/>
+          <t>1481</t>
+        </is>
+      </c>
+      <c r="D19" s="12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E19" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve">13:00 15:00 H.T. </t>
         </is>
       </c>
       <c r="F19" s="14" t="inlineStr">
@@ -1768,14 +1789,26 @@
       <c r="K19" s="17" t="n"/>
     </row>
     <row r="20" ht="19.5" customHeight="1" s="109">
-      <c r="A20" s="10" t="n"/>
-      <c r="B20" s="11" t="inlineStr"/>
+      <c r="A20" s="10" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B20" s="11" t="inlineStr">
+        <is>
+          <t>ADMINISTRACIÓN DEL MANTENIMIENTO (INC-1004)</t>
+        </is>
+      </c>
       <c r="C20" s="12" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D20" s="12" t="inlineStr"/>
+          <t>1601</t>
+        </is>
+      </c>
+      <c r="D20" s="12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="E20" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -1788,7 +1821,7 @@
       </c>
       <c r="G20" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>11:00 13:00</t>
         </is>
       </c>
       <c r="H20" s="14" t="inlineStr">
@@ -1798,7 +1831,7 @@
       </c>
       <c r="I20" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>11:00 13:00</t>
         </is>
       </c>
       <c r="J20" s="14" t="inlineStr">
@@ -1809,14 +1842,26 @@
       <c r="K20" s="17" t="n"/>
     </row>
     <row r="21" ht="18" customHeight="1" s="109">
-      <c r="A21" s="10" t="n"/>
-      <c r="B21" s="11" t="inlineStr"/>
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B21" s="11" t="inlineStr">
+        <is>
+          <t>ADMINISTRACIÓN DEL MANTENIMIENTO (INC-1004)</t>
+        </is>
+      </c>
       <c r="C21" s="12" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D21" s="12" t="inlineStr"/>
+          <t>1681</t>
+        </is>
+      </c>
+      <c r="D21" s="12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="E21" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -1829,7 +1874,7 @@
       </c>
       <c r="G21" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve">13:00 15:00 H.T. </t>
         </is>
       </c>
       <c r="H21" s="14" t="inlineStr">
@@ -1839,7 +1884,7 @@
       </c>
       <c r="I21" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>10:00 11:00</t>
         </is>
       </c>
       <c r="J21" s="14" t="inlineStr">
@@ -1850,14 +1895,26 @@
       <c r="K21" s="17" t="n"/>
     </row>
     <row r="22" ht="18" customHeight="1" s="109">
-      <c r="A22" s="10" t="n"/>
-      <c r="B22" s="11" t="inlineStr"/>
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B22" s="11" t="inlineStr">
+        <is>
+          <t>ADMINISTRACIÓN DEL MANTENIMIENTO (INC-1004)</t>
+        </is>
+      </c>
       <c r="C22" s="12" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D22" s="12" t="inlineStr"/>
+          <t>1681</t>
+        </is>
+      </c>
+      <c r="D22" s="12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="E22" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -1880,7 +1937,7 @@
       </c>
       <c r="I22" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>13:00 14:00</t>
         </is>
       </c>
       <c r="J22" s="14" t="inlineStr">
@@ -1900,7 +1957,7 @@
       </c>
       <c r="D23" s="9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>25</t>
         </is>
       </c>
       <c r="E23" s="21" t="n"/>
@@ -1971,29 +2028,13 @@
       </c>
     </row>
     <row r="26" ht="24.75" customHeight="1" s="109">
-      <c r="A26" s="24" t="inlineStr">
-        <is>
-          <t>SISTEMAS COMPUTACIONALES</t>
-        </is>
-      </c>
-      <c r="B26" s="25" t="inlineStr">
-        <is>
-          <t>TUTORIA</t>
-        </is>
-      </c>
-      <c r="C26" s="26" t="inlineStr">
-        <is>
-          <t>4102</t>
-        </is>
-      </c>
-      <c r="D26" s="26" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="A26" s="24" t="inlineStr"/>
+      <c r="B26" s="25" t="inlineStr"/>
+      <c r="C26" s="26" t="inlineStr"/>
+      <c r="D26" s="26" t="inlineStr"/>
       <c r="E26" s="14" t="inlineStr">
         <is>
-          <t>09:00 11:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="F26" s="14" t="inlineStr">
@@ -2024,29 +2065,13 @@
       <c r="K26" s="27" t="n"/>
     </row>
     <row r="27" ht="28.5" customHeight="1" s="109">
-      <c r="A27" s="24" t="inlineStr">
-        <is>
-          <t>SISTEMAS COMPUTACIONALES</t>
-        </is>
-      </c>
-      <c r="B27" s="25" t="inlineStr">
-        <is>
-          <t>COORDINACIÓN DE SEGUIMIENTO DE COHORTE GENERACIONAL</t>
-        </is>
-      </c>
-      <c r="C27" s="26" t="inlineStr">
-        <is>
-          <t>5201</t>
-        </is>
-      </c>
-      <c r="D27" s="26" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="A27" s="24" t="inlineStr"/>
+      <c r="B27" s="25" t="inlineStr"/>
+      <c r="C27" s="26" t="inlineStr"/>
+      <c r="D27" s="26" t="inlineStr"/>
       <c r="E27" s="14" t="inlineStr">
         <is>
-          <t>14:00 16:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="F27" s="14" t="inlineStr">
@@ -2308,7 +2333,7 @@
       </c>
       <c r="D34" s="9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E34" s="30" t="n"/>
@@ -2444,7 +2469,7 @@
       </c>
       <c r="C39" s="93" t="n"/>
       <c r="D39" s="37" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E39" s="38" t="n"/>
       <c r="F39" s="38" t="n"/>
@@ -2465,7 +2490,7 @@
       </c>
       <c r="G40" s="95" t="inlineStr">
         <is>
-          <t>20/02/2025</t>
+          <t>01/03/2025</t>
         </is>
       </c>
       <c r="H40" s="93" t="n"/>
@@ -2528,19 +2553,15 @@
       <c r="K43" s="45" t="n"/>
     </row>
     <row r="44" ht="21.75" customFormat="1" customHeight="1" s="43">
-      <c r="A44" s="112" t="inlineStr">
-        <is>
-          <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
-        </is>
-      </c>
-      <c r="B44" s="113" t="n"/>
+      <c r="A44" s="111" t="n"/>
+      <c r="B44" s="112" t="n"/>
       <c r="C44" s="52" t="n"/>
       <c r="D44" s="46" t="n"/>
       <c r="E44" s="46" t="n"/>
       <c r="F44" s="47" t="n"/>
       <c r="G44" s="57" t="inlineStr">
         <is>
-          <t>IVAN</t>
+          <t xml:space="preserve">GELOVER MANZO HUGO </t>
         </is>
       </c>
       <c r="H44" s="86" t="n"/>
@@ -2549,30 +2570,26 @@
       <c r="K44" s="45" t="n"/>
     </row>
     <row r="45" ht="27.75" customFormat="1" customHeight="1" s="43">
-      <c r="A45" s="114" t="inlineStr">
-        <is>
-          <t>JEFA DE DIVISIÓN DE ING. EN SISTEMAS COMPUTACIONALES</t>
-        </is>
-      </c>
-      <c r="B45" s="115" t="n"/>
-      <c r="C45" s="116" t="inlineStr">
+      <c r="A45" s="113" t="n"/>
+      <c r="B45" s="112" t="n"/>
+      <c r="C45" s="114" t="inlineStr">
         <is>
           <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ</t>
         </is>
       </c>
-      <c r="F45" s="115" t="n"/>
-      <c r="G45" s="117" t="n"/>
-      <c r="J45" s="115" t="n"/>
+      <c r="F45" s="112" t="n"/>
+      <c r="G45" s="115" t="n"/>
+      <c r="J45" s="112" t="n"/>
       <c r="K45" s="45" t="n"/>
     </row>
     <row r="46" ht="12" customFormat="1" customHeight="1" s="43">
       <c r="A46" s="66" t="inlineStr">
         <is>
-          <t>DRA. EN C.C. FABIOLA ORQUÍDEA SANCHEZ HERNANDEZ</t>
+          <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
         </is>
       </c>
       <c r="B46" s="104" t="n"/>
-      <c r="C46" s="118" t="inlineStr">
+      <c r="C46" s="116" t="inlineStr">
         <is>
           <t>ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
         </is>
@@ -2580,7 +2597,7 @@
       <c r="D46" s="90" t="n"/>
       <c r="E46" s="90" t="n"/>
       <c r="F46" s="104" t="n"/>
-      <c r="G46" s="119" t="n"/>
+      <c r="G46" s="117" t="n"/>
       <c r="H46" s="90" t="n"/>
       <c r="I46" s="90" t="n"/>
       <c r="J46" s="104" t="n"/>
@@ -2602,7 +2619,7 @@
     </row>
     <row r="48" ht="9" customHeight="1" s="109">
       <c r="A48" s="68" t="n"/>
-      <c r="C48" s="120" t="inlineStr">
+      <c r="C48" s="118" t="inlineStr">
         <is>
           <t>Vo. Bo</t>
         </is>

</xml_diff>

<commit_message>
Cambio de exportacion PDF y entregable de AcademyReport version 1.0
</commit_message>
<xml_diff>
--- a/temp_reporte.xlsx
+++ b/temp_reporte.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja(1)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hoja(32)" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="ADSCRIPCION">#REF!</definedName>
@@ -73,9 +73,9 @@
     <definedName name="TIPO_A">#REF!</definedName>
     <definedName name="TIPO_B">#REF!</definedName>
     <definedName name="VIERNES">#REF!</definedName>
-    <definedName name="ASIGNACION" localSheetId="0">'Hoja(1)'!$K:$K</definedName>
-    <definedName name="FORMATO" localSheetId="0">'Hoja(1)'!$A:$K</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Hoja(1)'!$A$1:$J$59</definedName>
+    <definedName name="ASIGNACION" localSheetId="0">'Hoja(32)'!$K:$K</definedName>
+    <definedName name="FORMATO" localSheetId="0">'Hoja(32)'!$A:$K</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Hoja(32)'!$A$1:$J$59</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -87,7 +87,7 @@
     <numFmt numFmtId="164" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <name val="Arial"/>
       <sz val="10"/>
@@ -180,11 +180,6 @@
       <family val="2"/>
       <sz val="7"/>
     </font>
-    <font>
-      <name val="Gill Sans MT"/>
-      <family val="2"/>
-      <sz val="7"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -224,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -473,13 +468,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="123">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -616,46 +618,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -664,6 +626,70 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -673,27 +699,31 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -702,8 +732,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -711,20 +739,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -734,46 +761,31 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -785,7 +797,875 @@
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal 2 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="128">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1246,22 +2126,22 @@
   </sheetPr>
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A44" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:J55"/>
+    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A39" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col width="11.140625" customWidth="1" style="69" min="1" max="1"/>
-    <col width="19.42578125" customWidth="1" style="69" min="2" max="2"/>
-    <col width="7.85546875" customWidth="1" style="69" min="3" max="3"/>
-    <col width="5.85546875" customWidth="1" style="69" min="4" max="4"/>
-    <col width="13.140625" customWidth="1" style="69" min="5" max="5"/>
-    <col width="13.7109375" customWidth="1" style="69" min="6" max="6"/>
-    <col width="12.5703125" customWidth="1" style="69" min="7" max="7"/>
-    <col width="12.42578125" customWidth="1" style="69" min="8" max="8"/>
-    <col width="12" customWidth="1" style="69" min="9" max="9"/>
-    <col width="9.7109375" customWidth="1" style="69" min="10" max="10"/>
+    <col width="11.140625" customWidth="1" style="55" min="1" max="1"/>
+    <col width="19.42578125" customWidth="1" style="55" min="2" max="2"/>
+    <col width="7.85546875" customWidth="1" style="55" min="3" max="3"/>
+    <col width="5.85546875" customWidth="1" style="55" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" style="55" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" style="55" min="6" max="6"/>
+    <col width="12.5703125" customWidth="1" style="55" min="7" max="7"/>
+    <col width="12.42578125" customWidth="1" style="55" min="8" max="8"/>
+    <col width="12" customWidth="1" style="55" min="9" max="9"/>
+    <col width="9.7109375" customWidth="1" style="55" min="10" max="10"/>
     <col width="12.140625" customWidth="1" style="2" min="11" max="11"/>
     <col width="11.42578125" customWidth="1" style="3" min="12" max="15"/>
     <col width="25.42578125" customWidth="1" style="3" min="16" max="16"/>
@@ -1270,156 +2150,156 @@
     <col width="11.42578125" customWidth="1" style="3" min="20" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" s="109">
+    <row r="1" ht="12" customHeight="1" s="112">
       <c r="A1" s="53" t="n"/>
     </row>
-    <row r="2" ht="12" customHeight="1" s="109"/>
-    <row r="3" ht="32.25" customHeight="1" s="109"/>
-    <row r="4" ht="12" customHeight="1" s="109">
-      <c r="A4" s="97" t="inlineStr">
+    <row r="2" ht="12" customHeight="1" s="112"/>
+    <row r="3" ht="32.25" customHeight="1" s="112"/>
+    <row r="4" ht="12" customHeight="1" s="112">
+      <c r="A4" s="106" t="inlineStr">
         <is>
           <t>“2025. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="98" t="inlineStr">
+      <c r="A5" s="107" t="inlineStr">
         <is>
           <t>Asignación Académica</t>
         </is>
       </c>
-      <c r="B5" s="83" t="n"/>
-      <c r="C5" s="83" t="n"/>
-      <c r="D5" s="83" t="n"/>
-      <c r="E5" s="83" t="n"/>
-      <c r="F5" s="83" t="n"/>
-      <c r="G5" s="83" t="n"/>
-      <c r="H5" s="83" t="n"/>
-      <c r="I5" s="83" t="n"/>
-      <c r="J5" s="84" t="n"/>
-    </row>
-    <row r="6" ht="12" customHeight="1" s="109">
-      <c r="A6" s="85" t="inlineStr">
+      <c r="B5" s="95" t="n"/>
+      <c r="C5" s="95" t="n"/>
+      <c r="D5" s="95" t="n"/>
+      <c r="E5" s="95" t="n"/>
+      <c r="F5" s="95" t="n"/>
+      <c r="G5" s="95" t="n"/>
+      <c r="H5" s="95" t="n"/>
+      <c r="I5" s="95" t="n"/>
+      <c r="J5" s="96" t="n"/>
+    </row>
+    <row r="6" ht="12" customHeight="1" s="112">
+      <c r="A6" s="97" t="inlineStr">
         <is>
           <t>NOMBRE:</t>
         </is>
       </c>
-      <c r="B6" s="86" t="n"/>
-      <c r="C6" s="86" t="n"/>
-      <c r="D6" s="87" t="n"/>
-      <c r="E6" s="85" t="inlineStr">
+      <c r="B6" s="92" t="n"/>
+      <c r="C6" s="92" t="n"/>
+      <c r="D6" s="93" t="n"/>
+      <c r="E6" s="97" t="inlineStr">
         <is>
           <t>PROFESION:</t>
         </is>
       </c>
-      <c r="F6" s="86" t="n"/>
-      <c r="G6" s="86" t="n"/>
-      <c r="H6" s="86" t="n"/>
-      <c r="I6" s="86" t="n"/>
-      <c r="J6" s="87" t="n"/>
-    </row>
-    <row r="7" ht="12" customHeight="1" s="109">
-      <c r="A7" s="99" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GELOVER MANZO HUGO </t>
-        </is>
-      </c>
-      <c r="B7" s="90" t="n"/>
-      <c r="C7" s="90" t="n"/>
-      <c r="D7" s="104" t="n"/>
-      <c r="E7" s="100" t="inlineStr">
-        <is>
-          <t>ING. ELECTROMECÁNICO</t>
-        </is>
-      </c>
-      <c r="F7" s="90" t="n"/>
-      <c r="G7" s="90" t="n"/>
-      <c r="H7" s="90" t="n"/>
-      <c r="I7" s="90" t="n"/>
-      <c r="J7" s="104" t="n"/>
-    </row>
-    <row r="8" ht="12" customHeight="1" s="109">
-      <c r="A8" s="85" t="inlineStr">
+      <c r="F6" s="92" t="n"/>
+      <c r="G6" s="92" t="n"/>
+      <c r="H6" s="92" t="n"/>
+      <c r="I6" s="92" t="n"/>
+      <c r="J6" s="93" t="n"/>
+    </row>
+    <row r="7" ht="12" customHeight="1" s="112">
+      <c r="A7" s="108" t="inlineStr">
+        <is>
+          <t>AGUILAR GUGGEMBUHL JARUMI</t>
+        </is>
+      </c>
+      <c r="B7" s="100" t="n"/>
+      <c r="C7" s="100" t="n"/>
+      <c r="D7" s="105" t="n"/>
+      <c r="E7" s="101" t="inlineStr">
+        <is>
+          <t>LIC. VETERINARIA Y ZOOTECNIA/M. EN C. AGROPECUARIAS/ DR. BIOTECNOLOGÍA</t>
+        </is>
+      </c>
+      <c r="F7" s="100" t="n"/>
+      <c r="G7" s="100" t="n"/>
+      <c r="H7" s="100" t="n"/>
+      <c r="I7" s="100" t="n"/>
+      <c r="J7" s="105" t="n"/>
+    </row>
+    <row r="8" ht="12" customHeight="1" s="112">
+      <c r="A8" s="97" t="inlineStr">
         <is>
           <t>ADSCRIPCIÓN:</t>
         </is>
       </c>
-      <c r="B8" s="86" t="n"/>
-      <c r="C8" s="86" t="n"/>
-      <c r="D8" s="87" t="n"/>
-      <c r="E8" s="85" t="inlineStr">
+      <c r="B8" s="92" t="n"/>
+      <c r="C8" s="92" t="n"/>
+      <c r="D8" s="93" t="n"/>
+      <c r="E8" s="97" t="inlineStr">
         <is>
           <t>INGRESO AL TECNOLÓGICO</t>
         </is>
       </c>
-      <c r="F8" s="86" t="n"/>
-      <c r="G8" s="87" t="n"/>
-      <c r="H8" s="85" t="inlineStr">
+      <c r="F8" s="92" t="n"/>
+      <c r="G8" s="93" t="n"/>
+      <c r="H8" s="97" t="inlineStr">
         <is>
           <t>TIEMPO INDETERMINADO</t>
         </is>
       </c>
-      <c r="I8" s="86" t="n"/>
-      <c r="J8" s="87" t="n"/>
-    </row>
-    <row r="9" ht="12" customHeight="1" s="109">
-      <c r="A9" s="100" t="inlineStr">
+      <c r="I8" s="92" t="n"/>
+      <c r="J8" s="93" t="n"/>
+    </row>
+    <row r="9" ht="12" customHeight="1" s="112">
+      <c r="A9" s="101" t="inlineStr">
         <is>
           <t>PROFESOR DE ASIGNATURA DE ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B9" s="90" t="n"/>
-      <c r="C9" s="90" t="n"/>
-      <c r="D9" s="104" t="n"/>
-      <c r="E9" s="103" t="inlineStr">
-        <is>
-          <t>01 DE SEPTIEMBRE DE 2019</t>
-        </is>
-      </c>
-      <c r="F9" s="90" t="n"/>
-      <c r="G9" s="104" t="n"/>
-      <c r="H9" s="103" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="I9" s="90" t="n"/>
-      <c r="J9" s="104" t="n"/>
-    </row>
-    <row r="10" ht="12" customHeight="1" s="109">
-      <c r="A10" s="85" t="inlineStr">
+      <c r="B9" s="100" t="n"/>
+      <c r="C9" s="100" t="n"/>
+      <c r="D9" s="105" t="n"/>
+      <c r="E9" s="104" t="inlineStr">
+        <is>
+          <t>01 DE SEPTIEMBRE 2014</t>
+        </is>
+      </c>
+      <c r="F9" s="100" t="n"/>
+      <c r="G9" s="105" t="n"/>
+      <c r="H9" s="104" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="I9" s="100" t="n"/>
+      <c r="J9" s="105" t="n"/>
+    </row>
+    <row r="10" ht="12" customHeight="1" s="112">
+      <c r="A10" s="97" t="inlineStr">
         <is>
           <t>PERIODO:</t>
         </is>
       </c>
-      <c r="B10" s="86" t="n"/>
-      <c r="C10" s="86" t="n"/>
-      <c r="D10" s="87" t="n"/>
-      <c r="E10" s="88" t="inlineStr">
+      <c r="B10" s="92" t="n"/>
+      <c r="C10" s="92" t="n"/>
+      <c r="D10" s="93" t="n"/>
+      <c r="E10" s="98" t="inlineStr">
         <is>
           <t>HORAS TIPO</t>
         </is>
       </c>
-      <c r="F10" s="83" t="n"/>
-      <c r="G10" s="83" t="n"/>
-      <c r="H10" s="84" t="n"/>
-      <c r="I10" s="88" t="inlineStr">
+      <c r="F10" s="95" t="n"/>
+      <c r="G10" s="95" t="n"/>
+      <c r="H10" s="96" t="n"/>
+      <c r="I10" s="98" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="J10" s="84" t="n"/>
-    </row>
-    <row r="11" ht="12" customHeight="1" s="109">
-      <c r="A11" s="89" t="inlineStr">
+      <c r="J10" s="96" t="n"/>
+    </row>
+    <row r="11" ht="12" customHeight="1" s="112">
+      <c r="A11" s="99" t="inlineStr">
         <is>
           <t>2024-1 (MARZO-AGOSTO 2024)</t>
         </is>
       </c>
-      <c r="B11" s="90" t="n"/>
-      <c r="C11" s="90" t="n"/>
-      <c r="D11" s="90" t="n"/>
-      <c r="E11" s="88" t="inlineStr">
+      <c r="B11" s="100" t="n"/>
+      <c r="C11" s="100" t="n"/>
+      <c r="D11" s="100" t="n"/>
+      <c r="E11" s="98" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -1445,7 +2325,7 @@
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
-    <row r="12" ht="5.1" customHeight="1" s="109">
+    <row r="12" ht="5.1" customHeight="1" s="112">
       <c r="A12" s="8" t="n"/>
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="8" t="n"/>
@@ -1457,23 +2337,23 @@
       <c r="I12" s="8" t="n"/>
       <c r="J12" s="8" t="n"/>
     </row>
-    <row r="13" ht="12" customHeight="1" s="109">
-      <c r="A13" s="88" t="inlineStr">
+    <row r="13" ht="12" customHeight="1" s="112">
+      <c r="A13" s="98" t="inlineStr">
         <is>
           <t>Asignación de Horas Frente a Grupo</t>
         </is>
       </c>
-      <c r="B13" s="83" t="n"/>
-      <c r="C13" s="83" t="n"/>
-      <c r="D13" s="83" t="n"/>
-      <c r="E13" s="83" t="n"/>
-      <c r="F13" s="83" t="n"/>
-      <c r="G13" s="83" t="n"/>
-      <c r="H13" s="83" t="n"/>
-      <c r="I13" s="83" t="n"/>
-      <c r="J13" s="84" t="n"/>
-    </row>
-    <row r="14" ht="12" customHeight="1" s="109">
+      <c r="B13" s="95" t="n"/>
+      <c r="C13" s="95" t="n"/>
+      <c r="D13" s="95" t="n"/>
+      <c r="E13" s="95" t="n"/>
+      <c r="F13" s="95" t="n"/>
+      <c r="G13" s="95" t="n"/>
+      <c r="H13" s="95" t="n"/>
+      <c r="I13" s="95" t="n"/>
+      <c r="J13" s="96" t="n"/>
+    </row>
+    <row r="14" ht="12" customHeight="1" s="112">
       <c r="A14" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -1526,133 +2406,137 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="n"/>
+      <c r="A15" s="10" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
       <c r="B15" s="11" t="inlineStr">
         <is>
-          <t>CÁLCULO INTEGRAL (ACF-0902)</t>
+          <t>QUÍMICA (INC-1025)</t>
         </is>
       </c>
       <c r="C15" s="12" t="inlineStr">
         <is>
-          <t> </t>
+          <t>1101</t>
         </is>
       </c>
       <c r="D15" s="12" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E15" s="14" t="inlineStr">
+        <is>
+          <t>11:00 13:00</t>
+        </is>
+      </c>
+      <c r="F15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G15" s="14" t="inlineStr">
+        <is>
+          <t>11:00 13:00</t>
+        </is>
+      </c>
+      <c r="H15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J15" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K15" s="15" t="n"/>
+      <c r="N15" s="113" t="n"/>
+    </row>
+    <row r="16" ht="21.75" customHeight="1" s="112">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B16" s="11" t="inlineStr">
+        <is>
+          <t>DESARROLLO SUSTENTABLE (ACD-0908)</t>
+        </is>
+      </c>
+      <c r="C16" s="12" t="inlineStr">
+        <is>
+          <t>1501</t>
+        </is>
+      </c>
+      <c r="D16" s="12" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E15" s="14" t="inlineStr">
-        <is>
-          <t>07:00 09:00</t>
-        </is>
-      </c>
-      <c r="F15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G15" s="14" t="inlineStr">
-        <is>
-          <t>07:00 09:00</t>
-        </is>
-      </c>
-      <c r="H15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I15" s="14" t="inlineStr">
-        <is>
-          <t>07:00 08:00</t>
-        </is>
-      </c>
-      <c r="J15" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K15" s="15" t="n"/>
-      <c r="N15" s="110" t="n"/>
-    </row>
-    <row r="16" ht="21.75" customHeight="1" s="109">
-      <c r="A16" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B16" s="11" t="inlineStr">
-        <is>
-          <t>PROCESOS DE FABRICACIÓN (INC-1023)</t>
-        </is>
-      </c>
-      <c r="C16" s="12" t="inlineStr">
-        <is>
-          <t>1401</t>
-        </is>
-      </c>
-      <c r="D16" s="12" t="inlineStr">
+      <c r="E16" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F16" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G16" s="14" t="inlineStr">
+        <is>
+          <t>09:00 11:00</t>
+        </is>
+      </c>
+      <c r="H16" s="14" t="inlineStr">
+        <is>
+          <t>10:00 12:00</t>
+        </is>
+      </c>
+      <c r="I16" s="14" t="inlineStr">
+        <is>
+          <t>11:00 12:00</t>
+        </is>
+      </c>
+      <c r="J16" s="14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K16" s="17" t="n"/>
+      <c r="N16" s="113" t="n"/>
+    </row>
+    <row r="17" ht="21.75" customHeight="1" s="112">
+      <c r="A17" s="10" t="inlineStr">
+        <is>
+          <t>SISTEMAS COMPUTACIONALES</t>
+        </is>
+      </c>
+      <c r="B17" s="11" t="inlineStr">
+        <is>
+          <t>MINECRAFT</t>
+        </is>
+      </c>
+      <c r="C17" s="12" t="inlineStr">
+        <is>
+          <t>4102</t>
+        </is>
+      </c>
+      <c r="D17" s="12" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E16" s="14" t="inlineStr">
-        <is>
-          <t>09:00 11:00</t>
-        </is>
-      </c>
-      <c r="F16" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G16" s="14" t="inlineStr">
-        <is>
-          <t>09:00 11:00</t>
-        </is>
-      </c>
-      <c r="H16" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I16" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J16" s="14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K16" s="17" t="n"/>
-      <c r="N16" s="110" t="n"/>
-    </row>
-    <row r="17" ht="21.75" customHeight="1" s="109">
-      <c r="A17" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B17" s="11" t="inlineStr">
-        <is>
-          <t>PROCESOS DE FABRICACIÓN (INC-1023)</t>
-        </is>
-      </c>
-      <c r="C17" s="12" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="D17" s="12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="E17" s="14" t="inlineStr">
         <is>
-          <t>15:00 17:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="F17" s="14" t="inlineStr">
@@ -1662,7 +2546,7 @@
       </c>
       <c r="G17" s="14" t="inlineStr">
         <is>
-          <t>15:00 17:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="H17" s="14" t="inlineStr">
@@ -1682,30 +2566,18 @@
       </c>
       <c r="K17" s="17" t="n"/>
     </row>
-    <row r="18">
-      <c r="A18" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B18" s="11" t="inlineStr">
-        <is>
-          <t>PROCESOS DE FABRICACIÓN (INC-1023)</t>
-        </is>
-      </c>
+    <row r="18" ht="17.25" customHeight="1" s="112">
+      <c r="A18" s="10" t="n"/>
+      <c r="B18" s="11" t="inlineStr"/>
       <c r="C18" s="12" t="inlineStr">
         <is>
-          <t>1481</t>
-        </is>
-      </c>
-      <c r="D18" s="12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D18" s="12" t="inlineStr"/>
       <c r="E18" s="14" t="inlineStr">
         <is>
-          <t>11:00 13:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="F18" s="14" t="inlineStr">
@@ -1735,30 +2607,18 @@
       </c>
       <c r="K18" s="17" t="n"/>
     </row>
-    <row r="19" ht="20.25" customHeight="1" s="109">
-      <c r="A19" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B19" s="11" t="inlineStr">
-        <is>
-          <t>PROCESOS DE FABRICACIÓN (INC-1023)</t>
-        </is>
-      </c>
+    <row r="19" ht="20.25" customHeight="1" s="112">
+      <c r="A19" s="10" t="n"/>
+      <c r="B19" s="11" t="inlineStr"/>
       <c r="C19" s="12" t="inlineStr">
         <is>
-          <t>1481</t>
-        </is>
-      </c>
-      <c r="D19" s="12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D19" s="12" t="inlineStr"/>
       <c r="E19" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">13:00 15:00 H.T. </t>
+          <t> </t>
         </is>
       </c>
       <c r="F19" s="14" t="inlineStr">
@@ -1788,27 +2648,15 @@
       </c>
       <c r="K19" s="17" t="n"/>
     </row>
-    <row r="20" ht="19.5" customHeight="1" s="109">
-      <c r="A20" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B20" s="11" t="inlineStr">
-        <is>
-          <t>ADMINISTRACIÓN DEL MANTENIMIENTO (INC-1004)</t>
-        </is>
-      </c>
+    <row r="20" ht="19.5" customHeight="1" s="112">
+      <c r="A20" s="10" t="n"/>
+      <c r="B20" s="11" t="inlineStr"/>
       <c r="C20" s="12" t="inlineStr">
         <is>
-          <t>1601</t>
-        </is>
-      </c>
-      <c r="D20" s="12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D20" s="12" t="inlineStr"/>
       <c r="E20" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -1821,7 +2669,7 @@
       </c>
       <c r="G20" s="14" t="inlineStr">
         <is>
-          <t>11:00 13:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="H20" s="14" t="inlineStr">
@@ -1831,7 +2679,7 @@
       </c>
       <c r="I20" s="14" t="inlineStr">
         <is>
-          <t>11:00 13:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="J20" s="14" t="inlineStr">
@@ -1841,27 +2689,15 @@
       </c>
       <c r="K20" s="17" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="109">
-      <c r="A21" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B21" s="11" t="inlineStr">
-        <is>
-          <t>ADMINISTRACIÓN DEL MANTENIMIENTO (INC-1004)</t>
-        </is>
-      </c>
+    <row r="21" ht="18" customHeight="1" s="112">
+      <c r="A21" s="10" t="n"/>
+      <c r="B21" s="11" t="inlineStr"/>
       <c r="C21" s="12" t="inlineStr">
         <is>
-          <t>1681</t>
-        </is>
-      </c>
-      <c r="D21" s="12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D21" s="12" t="inlineStr"/>
       <c r="E21" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -1874,7 +2710,7 @@
       </c>
       <c r="G21" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">13:00 15:00 H.T. </t>
+          <t> </t>
         </is>
       </c>
       <c r="H21" s="14" t="inlineStr">
@@ -1884,7 +2720,7 @@
       </c>
       <c r="I21" s="14" t="inlineStr">
         <is>
-          <t>10:00 11:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="J21" s="14" t="inlineStr">
@@ -1894,27 +2730,15 @@
       </c>
       <c r="K21" s="17" t="n"/>
     </row>
-    <row r="22" ht="18" customHeight="1" s="109">
-      <c r="A22" s="10" t="inlineStr">
-        <is>
-          <t>INDUSTRIAL</t>
-        </is>
-      </c>
-      <c r="B22" s="11" t="inlineStr">
-        <is>
-          <t>ADMINISTRACIÓN DEL MANTENIMIENTO (INC-1004)</t>
-        </is>
-      </c>
+    <row r="22" ht="18" customHeight="1" s="112">
+      <c r="A22" s="10" t="n"/>
+      <c r="B22" s="11" t="inlineStr"/>
       <c r="C22" s="12" t="inlineStr">
         <is>
-          <t>1681</t>
-        </is>
-      </c>
-      <c r="D22" s="12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D22" s="12" t="inlineStr"/>
       <c r="E22" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -1937,7 +2761,7 @@
       </c>
       <c r="I22" s="14" t="inlineStr">
         <is>
-          <t>13:00 14:00</t>
+          <t> </t>
         </is>
       </c>
       <c r="J22" s="14" t="inlineStr">
@@ -1957,7 +2781,7 @@
       </c>
       <c r="D23" s="9" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E23" s="21" t="n"/>
@@ -1968,14 +2792,14 @@
       <c r="J23" s="23" t="n"/>
       <c r="K23" s="17" t="n"/>
     </row>
-    <row r="24" ht="12" customHeight="1" s="109">
-      <c r="A24" s="91" t="inlineStr">
+    <row r="24" ht="12" customHeight="1" s="112">
+      <c r="A24" s="83" t="inlineStr">
         <is>
           <t>Asignación de Horas de Descarga para otras Actividades</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="12" customHeight="1" s="109">
+    <row r="25" ht="12" customHeight="1" s="112">
       <c r="A25" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -2027,11 +2851,27 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="24.75" customHeight="1" s="109">
-      <c r="A26" s="24" t="inlineStr"/>
-      <c r="B26" s="25" t="inlineStr"/>
-      <c r="C26" s="26" t="inlineStr"/>
-      <c r="D26" s="26" t="inlineStr"/>
+    <row r="26" ht="21.75" customHeight="1" s="112">
+      <c r="A26" s="24" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B26" s="25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ASESORÍA DE QUÍMICA </t>
+        </is>
+      </c>
+      <c r="C26" s="26" t="inlineStr">
+        <is>
+          <t>1101</t>
+        </is>
+      </c>
+      <c r="D26" s="26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E26" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -2054,7 +2894,7 @@
       </c>
       <c r="I26" s="14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>10:00 11:00</t>
         </is>
       </c>
       <c r="J26" s="14" t="inlineStr">
@@ -2064,11 +2904,27 @@
       </c>
       <c r="K26" s="27" t="n"/>
     </row>
-    <row r="27" ht="28.5" customHeight="1" s="109">
-      <c r="A27" s="24" t="inlineStr"/>
-      <c r="B27" s="25" t="inlineStr"/>
-      <c r="C27" s="26" t="inlineStr"/>
-      <c r="D27" s="26" t="inlineStr"/>
+    <row r="27" ht="24.75" customHeight="1" s="112">
+      <c r="A27" s="24" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B27" s="25" t="inlineStr">
+        <is>
+          <t>APORTACIÓN A LA LINEA DE INVESTIGACIÓN Y C.A</t>
+        </is>
+      </c>
+      <c r="C27" s="26" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="D27" s="26" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
       <c r="E27" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -2101,11 +2957,27 @@
       </c>
       <c r="K27" s="27" t="n"/>
     </row>
-    <row r="28" ht="26.25" customHeight="1" s="109">
-      <c r="A28" s="24" t="inlineStr"/>
-      <c r="B28" s="25" t="inlineStr"/>
-      <c r="C28" s="26" t="inlineStr"/>
-      <c r="D28" s="26" t="inlineStr"/>
+    <row r="28" ht="23.25" customHeight="1" s="112">
+      <c r="A28" s="24" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B28" s="25" t="inlineStr">
+        <is>
+          <t>ACTIVIDAD COMPLEMENTARIA (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="C28" s="26" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="D28" s="26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E28" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -2138,11 +3010,27 @@
       </c>
       <c r="K28" s="27" t="n"/>
     </row>
-    <row r="29" ht="30" customHeight="1" s="109">
-      <c r="A29" s="24" t="inlineStr"/>
-      <c r="B29" s="25" t="inlineStr"/>
-      <c r="C29" s="26" t="inlineStr"/>
-      <c r="D29" s="26" t="inlineStr"/>
+    <row r="29" ht="24" customHeight="1" s="112">
+      <c r="A29" s="24" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B29" s="25" t="inlineStr">
+        <is>
+          <t>DISEÑO DE PROGRAMA EDUCATIVO DE POSGRADO (MAESTRÍA)</t>
+        </is>
+      </c>
+      <c r="C29" s="26" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="D29" s="26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="E29" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -2175,11 +3063,27 @@
       </c>
       <c r="K29" s="27" t="n"/>
     </row>
-    <row r="30" ht="33" customHeight="1" s="109">
-      <c r="A30" s="24" t="inlineStr"/>
-      <c r="B30" s="25" t="inlineStr"/>
-      <c r="C30" s="26" t="inlineStr"/>
-      <c r="D30" s="26" t="inlineStr"/>
+    <row r="30" ht="24" customHeight="1" s="112">
+      <c r="A30" s="24" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B30" s="25" t="inlineStr">
+        <is>
+          <t>ASESOR DE RESIDENCIAS PROFESIONALES Y TITULACIÓN POR VIICYT 2024</t>
+        </is>
+      </c>
+      <c r="C30" s="26" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="D30" s="26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="E30" s="14" t="inlineStr">
         <is>
           <t> </t>
@@ -2212,7 +3116,7 @@
       </c>
       <c r="K30" s="27" t="n"/>
     </row>
-    <row r="31" ht="19.5" customHeight="1" s="109">
+    <row r="31" ht="23.25" customHeight="1" s="112">
       <c r="A31" s="24" t="inlineStr"/>
       <c r="B31" s="25" t="inlineStr"/>
       <c r="C31" s="26" t="inlineStr"/>
@@ -2249,7 +3153,7 @@
       </c>
       <c r="K31" s="27" t="n"/>
     </row>
-    <row r="32" ht="34.5" customHeight="1" s="109">
+    <row r="32" ht="24" customHeight="1" s="112">
       <c r="A32" s="24" t="inlineStr"/>
       <c r="B32" s="25" t="inlineStr"/>
       <c r="C32" s="26" t="inlineStr"/>
@@ -2286,7 +3190,7 @@
       </c>
       <c r="K32" s="27" t="n"/>
     </row>
-    <row r="33" ht="21" customHeight="1" s="109">
+    <row r="33" ht="21" customHeight="1" s="112">
       <c r="A33" s="24" t="inlineStr"/>
       <c r="B33" s="25" t="inlineStr"/>
       <c r="C33" s="26" t="inlineStr"/>
@@ -2333,7 +3237,7 @@
       </c>
       <c r="D34" s="9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E34" s="30" t="n"/>
@@ -2344,14 +3248,14 @@
       <c r="J34" s="28" t="n"/>
       <c r="K34" s="27" t="n"/>
     </row>
-    <row r="35" ht="12" customHeight="1" s="109">
-      <c r="A35" s="91" t="inlineStr">
+    <row r="35" ht="12" customHeight="1" s="112">
+      <c r="A35" s="83" t="inlineStr">
         <is>
           <t>Asignación de Horas de Presidente y Secretario de Academia</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="12" customHeight="1" s="109">
+    <row r="36" ht="12" customHeight="1" s="112">
       <c r="A36" s="18" t="inlineStr">
         <is>
           <t>Carrera</t>
@@ -2403,7 +3307,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="109">
+    <row r="37" ht="18.75" customHeight="1" s="112">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="25" t="inlineStr">
         <is>
@@ -2444,7 +3348,7 @@
       </c>
       <c r="K37" s="31" t="n"/>
     </row>
-    <row r="38" ht="12" customHeight="1" s="109" thickBot="1">
+    <row r="38" ht="12" customHeight="1" s="112" thickBot="1">
       <c r="A38" s="32" t="n"/>
       <c r="B38" s="33" t="n"/>
       <c r="C38" s="34" t="inlineStr">
@@ -2460,14 +3364,14 @@
       <c r="I38" s="26" t="n"/>
       <c r="J38" s="35" t="n"/>
     </row>
-    <row r="39" ht="12" customHeight="1" s="109" thickBot="1">
+    <row r="39" ht="12" customHeight="1" s="112" thickBot="1">
       <c r="A39" s="36" t="n"/>
-      <c r="B39" s="92" t="inlineStr">
+      <c r="B39" s="84" t="inlineStr">
         <is>
           <t>TOTAL DE HORAS</t>
         </is>
       </c>
-      <c r="C39" s="93" t="n"/>
+      <c r="C39" s="85" t="n"/>
       <c r="D39" s="37" t="n">
         <v>0</v>
       </c>
@@ -2478,31 +3382,31 @@
       <c r="I39" s="38" t="n"/>
       <c r="J39" s="39" t="n"/>
     </row>
-    <row r="40" ht="12" customHeight="1" s="109" thickBot="1">
+    <row r="40" ht="12" customHeight="1" s="112" thickBot="1">
       <c r="A40" s="36" t="n"/>
       <c r="B40" s="40" t="n"/>
       <c r="C40" s="41" t="n"/>
       <c r="D40" s="38" t="n"/>
-      <c r="E40" s="94" t="inlineStr">
+      <c r="E40" s="86" t="inlineStr">
         <is>
           <t>FECHA DE APLICACIÓN</t>
         </is>
       </c>
-      <c r="G40" s="95" t="inlineStr">
-        <is>
-          <t>01/03/2025</t>
-        </is>
-      </c>
-      <c r="H40" s="93" t="n"/>
-      <c r="I40" s="93" t="n"/>
-      <c r="J40" s="96" t="n"/>
-    </row>
-    <row r="41" ht="12" customHeight="1" s="109" thickBot="1">
+      <c r="G40" s="87" t="inlineStr">
+        <is>
+          <t>03/03/2025</t>
+        </is>
+      </c>
+      <c r="H40" s="85" t="n"/>
+      <c r="I40" s="85" t="n"/>
+      <c r="J40" s="88" t="n"/>
+    </row>
+    <row r="41" ht="12" customHeight="1" s="112" thickBot="1">
       <c r="A41" s="36" t="n"/>
       <c r="B41" s="40" t="n"/>
       <c r="C41" s="41" t="n"/>
       <c r="D41" s="38" t="n"/>
-      <c r="E41" s="94" t="inlineStr">
+      <c r="E41" s="86" t="inlineStr">
         <is>
           <t>CONSECUTIVO</t>
         </is>
@@ -2528,82 +3432,90 @@
       <c r="K42" s="45" t="n"/>
     </row>
     <row r="43" ht="17.25" customFormat="1" customHeight="1" s="43">
-      <c r="A43" s="105" t="inlineStr">
+      <c r="A43" s="89" t="inlineStr">
         <is>
           <t>JEFA DE DIVISIÓN DE ING. INDUSTRIAL</t>
         </is>
       </c>
-      <c r="B43" s="87" t="n"/>
-      <c r="C43" s="107" t="inlineStr">
+      <c r="B43" s="93" t="n"/>
+      <c r="C43" s="91" t="inlineStr">
         <is>
           <t>REVISO</t>
         </is>
       </c>
-      <c r="D43" s="86" t="n"/>
-      <c r="E43" s="86" t="n"/>
-      <c r="F43" s="87" t="n"/>
-      <c r="G43" s="82" t="inlineStr">
+      <c r="D43" s="92" t="n"/>
+      <c r="E43" s="92" t="n"/>
+      <c r="F43" s="93" t="n"/>
+      <c r="G43" s="94" t="inlineStr">
         <is>
           <t>FIRMA DE CONFORMIDAD</t>
         </is>
       </c>
-      <c r="H43" s="83" t="n"/>
-      <c r="I43" s="83" t="n"/>
-      <c r="J43" s="84" t="n"/>
+      <c r="H43" s="95" t="n"/>
+      <c r="I43" s="95" t="n"/>
+      <c r="J43" s="96" t="n"/>
       <c r="K43" s="45" t="n"/>
     </row>
     <row r="44" ht="21.75" customFormat="1" customHeight="1" s="43">
-      <c r="A44" s="111" t="n"/>
-      <c r="B44" s="112" t="n"/>
+      <c r="A44" s="114" t="inlineStr">
+        <is>
+          <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
+        </is>
+      </c>
+      <c r="B44" s="115" t="n"/>
       <c r="C44" s="52" t="n"/>
       <c r="D44" s="46" t="n"/>
       <c r="E44" s="46" t="n"/>
       <c r="F44" s="47" t="n"/>
-      <c r="G44" s="57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GELOVER MANZO HUGO </t>
-        </is>
-      </c>
-      <c r="H44" s="86" t="n"/>
-      <c r="I44" s="86" t="n"/>
-      <c r="J44" s="87" t="n"/>
+      <c r="G44" s="64" t="inlineStr">
+        <is>
+          <t>AGUILAR GUGGEMBUHL JARUMI</t>
+        </is>
+      </c>
+      <c r="H44" s="92" t="n"/>
+      <c r="I44" s="92" t="n"/>
+      <c r="J44" s="93" t="n"/>
       <c r="K44" s="45" t="n"/>
     </row>
-    <row r="45" ht="27.75" customFormat="1" customHeight="1" s="43">
-      <c r="A45" s="113" t="n"/>
-      <c r="B45" s="112" t="n"/>
-      <c r="C45" s="114" t="inlineStr">
+    <row r="45" ht="18.75" customFormat="1" customHeight="1" s="43">
+      <c r="A45" s="116" t="inlineStr">
+        <is>
+          <t>JEFA DE DIVISIÓN DE ING. EN SISTEMAS COMPUTACIONALES</t>
+        </is>
+      </c>
+      <c r="B45" s="117" t="n"/>
+      <c r="C45" s="118" t="inlineStr">
         <is>
           <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ</t>
         </is>
       </c>
-      <c r="F45" s="112" t="n"/>
-      <c r="G45" s="115" t="n"/>
-      <c r="J45" s="112" t="n"/>
+      <c r="F45" s="117" t="n"/>
+      <c r="G45" s="119" t="n"/>
+      <c r="J45" s="117" t="n"/>
       <c r="K45" s="45" t="n"/>
     </row>
-    <row r="46" ht="12" customFormat="1" customHeight="1" s="43">
-      <c r="A46" s="66" t="inlineStr">
-        <is>
-          <t>M. EN R.I. VIANCA LISSETH PEREZ CRUZ</t>
-        </is>
-      </c>
-      <c r="B46" s="104" t="n"/>
-      <c r="C46" s="116" t="inlineStr">
+    <row r="46" ht="18.75" customFormat="1" customHeight="1" s="43">
+      <c r="A46" s="78" t="inlineStr">
+        <is>
+          <t>DRA. EN C.C. FABIOLA ORQUÍDEA SANCHEZ HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="B46" s="105" t="n"/>
+      <c r="C46" s="120" t="inlineStr">
         <is>
           <t>ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
         </is>
       </c>
-      <c r="D46" s="90" t="n"/>
-      <c r="E46" s="90" t="n"/>
-      <c r="F46" s="104" t="n"/>
-      <c r="G46" s="117" t="n"/>
-      <c r="H46" s="90" t="n"/>
-      <c r="I46" s="90" t="n"/>
-      <c r="J46" s="104" t="n"/>
+      <c r="D46" s="100" t="n"/>
+      <c r="E46" s="100" t="n"/>
+      <c r="F46" s="105" t="n"/>
+      <c r="G46" s="121" t="n"/>
+      <c r="H46" s="100" t="n"/>
+      <c r="I46" s="100" t="n"/>
+      <c r="J46" s="105" t="n"/>
       <c r="K46" s="45" t="n"/>
     </row>
-    <row r="47" ht="1.35" customHeight="1" s="109">
+    <row r="47" ht="1.35" customHeight="1" s="112">
       <c r="A47" s="48" t="n"/>
       <c r="B47" s="48" t="n"/>
       <c r="C47" s="48" t="n"/>
@@ -2617,27 +3529,27 @@
       <c r="P47" s="49" t="n"/>
       <c r="Q47" s="49" t="n"/>
     </row>
-    <row r="48" ht="9" customHeight="1" s="109">
-      <c r="A48" s="68" t="n"/>
-      <c r="C48" s="118" t="inlineStr">
+    <row r="48" ht="9" customHeight="1" s="112">
+      <c r="A48" s="54" t="n"/>
+      <c r="C48" s="122" t="inlineStr">
         <is>
           <t>Vo. Bo</t>
         </is>
       </c>
-      <c r="G48" s="70" t="n"/>
+      <c r="G48" s="56" t="n"/>
       <c r="K48" s="3" t="n"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1" s="109">
+    <row r="49" ht="12.75" customHeight="1" s="112">
       <c r="K49" s="3" t="n"/>
     </row>
-    <row r="50" ht="13.5" customHeight="1" s="109">
-      <c r="C50" s="90" t="n"/>
-      <c r="D50" s="90" t="n"/>
-      <c r="E50" s="90" t="n"/>
-      <c r="F50" s="90" t="n"/>
+    <row r="50" ht="16.5" customHeight="1" s="112">
+      <c r="C50" s="100" t="n"/>
+      <c r="D50" s="100" t="n"/>
+      <c r="E50" s="100" t="n"/>
+      <c r="F50" s="100" t="n"/>
       <c r="K50" s="3" t="n"/>
     </row>
-    <row r="51" ht="1.5" customHeight="1" s="109">
+    <row r="51" ht="0.75" customHeight="1" s="112">
       <c r="A51" s="50" t="n"/>
       <c r="B51" s="51" t="n"/>
       <c r="C51" s="51" t="n"/>
@@ -2650,10 +3562,10 @@
       <c r="J51" s="51" t="n"/>
       <c r="K51" s="3" t="n"/>
     </row>
-    <row r="52" ht="10.5" customHeight="1" s="109">
+    <row r="52" ht="9" customHeight="1" s="112">
       <c r="A52" s="51" t="n"/>
       <c r="B52" s="51" t="n"/>
-      <c r="C52" s="54" t="inlineStr">
+      <c r="C52" s="58" t="inlineStr">
         <is>
           <t>DR. ERNESTO M. RIVAS RIVAS</t>
         </is>
@@ -2663,15 +3575,15 @@
       <c r="I52" s="51" t="n"/>
       <c r="J52" s="51" t="n"/>
     </row>
-    <row r="53">
-      <c r="C53" s="54" t="inlineStr">
+    <row r="53" ht="10.5" customHeight="1" s="112">
+      <c r="C53" s="58" t="inlineStr">
         <is>
           <t>DIRECTOR GENERAL</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="108" t="inlineStr">
+      <c r="A54" s="61" t="inlineStr">
         <is>
           <t>Los temarios de las asignaturas para este semestre debe ser descargados de la siguiente URL con la especialidad de Lean Manufacturing en la Industria 4.0: http://tescha.edomex.gob.mx/plan-de-estudio</t>
         </is>
@@ -2694,8 +3606,8 @@
     <mergeCell ref="C48:F50"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A4:J4"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="A4:J4"/>
     <mergeCell ref="A48:B50"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A54:J55"/>

</xml_diff>